<commit_message>
adult sheets now work
</commit_message>
<xml_diff>
--- a/data/template.xlsx
+++ b/data/template.xlsx
@@ -5,16 +5,17 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\me\Desktop\Development\nsbl-create-spreadsheets\src\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\me\Desktop\Development\nsbl-create-spreadsheets\src\nsblextracter\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B616914-5C4E-4067-8708-4D9C012C3E43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCEE5E9E-2BE8-45CC-B809-88745C590258}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3510" yWindow="3510" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{026AB82B-103F-4DF3-A0CA-05AA2F209D25}"/>
+    <workbookView xWindow="2730" yWindow="2730" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{026AB82B-103F-4DF3-A0CA-05AA2F209D25}"/>
   </bookViews>
   <sheets>
-    <sheet name="runsheet" sheetId="5" r:id="rId1"/>
-    <sheet name="scoresheet" sheetId="10" r:id="rId2"/>
+    <sheet name="runsheet-k" sheetId="5" r:id="rId1"/>
+    <sheet name="runsheet-a" sheetId="11" r:id="rId2"/>
+    <sheet name="scoresheet" sheetId="10" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="79">
   <si>
     <t>COURT 1</t>
   </si>
@@ -254,13 +255,31 @@
   </si>
   <si>
     <t>GRADES _year_group_</t>
+  </si>
+  <si>
+    <t>7pm</t>
+  </si>
+  <si>
+    <t>745pm</t>
+  </si>
+  <si>
+    <t>_7_c1_s_</t>
+  </si>
+  <si>
+    <t>_7_c2_s_</t>
+  </si>
+  <si>
+    <t>_745_c1_s_</t>
+  </si>
+  <si>
+    <t>_745_c2_s_</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="16" x14ac:knownFonts="1">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -349,13 +368,6 @@
     </font>
     <font>
       <sz val="18"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="18"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -909,7 +921,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="90">
+  <cellXfs count="88">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1010,105 +1022,17 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="28" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="14" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="15" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="31" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="29" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="30" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="29" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="28" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="27" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="26" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="35" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="34" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="33" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="32" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="6" fillId="7" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="36" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="37" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="31" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="29" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="36" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="14" fontId="11" fillId="0" borderId="27" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -1126,6 +1050,90 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="7" borderId="27" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="6" fillId="7" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="31" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="29" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="30" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="29" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="36" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="37" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="28" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="27" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="26" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="31" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="29" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="36" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="35" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="34" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="33" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="32" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="15" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="14" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1522,291 +1530,264 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06001A37-2C87-4F4D-8D59-4864FA219C19}">
-  <dimension ref="A1:F20"/>
+  <dimension ref="A1:G20"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="33.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="29.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="56.85546875" customWidth="1"/>
-    <col min="4" max="4" width="29.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="45.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="29.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="56.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="49"/>
-      <c r="D1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="50"/>
-    </row>
-    <row r="2" spans="1:6" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="E1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="G1" s="49"/>
+    </row>
+    <row r="2" spans="1:7" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="51" t="s">
+      <c r="B2" s="50" t="s">
         <v>46</v>
       </c>
-      <c r="C2" s="49"/>
-      <c r="D2" s="3" t="s">
+      <c r="C2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="51" t="s">
+      <c r="D2" s="50" t="s">
         <v>47</v>
       </c>
-      <c r="F2" s="50"/>
-    </row>
-    <row r="3" spans="1:6" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="E2" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" s="52" t="s">
+        <v>68</v>
+      </c>
+      <c r="G2" s="49"/>
+    </row>
+    <row r="3" spans="1:7" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="51" t="s">
+      <c r="B3" s="50" t="s">
         <v>48</v>
       </c>
-      <c r="C3" s="49"/>
-      <c r="D3" s="3" t="s">
+      <c r="C3" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="51" t="s">
+      <c r="D3" s="50" t="s">
         <v>49</v>
       </c>
-      <c r="F3" s="50"/>
-    </row>
-    <row r="4" spans="1:6" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="E3" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="F3" s="52" t="s">
+        <v>69</v>
+      </c>
+      <c r="G3" s="49"/>
+    </row>
+    <row r="4" spans="1:7" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="B4" s="51" t="s">
+      <c r="B4" s="50" t="s">
         <v>51</v>
       </c>
-      <c r="C4" s="49"/>
-      <c r="D4" s="4" t="s">
+      <c r="C4" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="E4" s="52" t="s">
+      <c r="D4" s="51" t="s">
         <v>52</v>
       </c>
-      <c r="F4" s="50"/>
-    </row>
-    <row r="5" spans="1:6" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="E4" s="49"/>
+      <c r="F4" s="49"/>
+      <c r="G4" s="49"/>
+    </row>
+    <row r="5" spans="1:7" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A5" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="52" t="s">
+      <c r="B5" s="51" t="s">
         <v>53</v>
       </c>
-      <c r="C5" s="49"/>
-      <c r="D5" s="4" t="s">
+      <c r="C5" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="E5" s="52" t="s">
+      <c r="D5" s="51" t="s">
         <v>54</v>
       </c>
-      <c r="F5" s="50"/>
-    </row>
-    <row r="6" spans="1:6" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="E5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G5" s="49"/>
+    </row>
+    <row r="6" spans="1:7" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A6" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="B6" s="52" t="s">
+      <c r="B6" s="51" t="s">
         <v>56</v>
       </c>
-      <c r="C6" s="49"/>
-      <c r="D6" s="4" t="s">
+      <c r="C6" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="E6" s="52" t="s">
+      <c r="D6" s="51" t="s">
         <v>57</v>
       </c>
-      <c r="F6" s="50"/>
-    </row>
-    <row r="7" spans="1:6" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="E6" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="F6" s="52" t="s">
+        <v>70</v>
+      </c>
+      <c r="G6" s="49"/>
+    </row>
+    <row r="7" spans="1:7" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A7" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="53" t="s">
+      <c r="B7" s="52" t="s">
         <v>58</v>
       </c>
-      <c r="C7" s="49"/>
-      <c r="D7" s="5" t="s">
+      <c r="C7" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="E7" s="53" t="s">
+      <c r="D7" s="52" t="s">
         <v>59</v>
       </c>
-      <c r="F7" s="50"/>
-    </row>
-    <row r="8" spans="1:6" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="E7" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="F7" s="52" t="s">
+        <v>71</v>
+      </c>
+      <c r="G7" s="49"/>
+    </row>
+    <row r="8" spans="1:7" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A8" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="B8" s="54" t="s">
+      <c r="B8" s="53" t="s">
         <v>60</v>
       </c>
-      <c r="C8" s="55"/>
-      <c r="D8" s="6" t="s">
+      <c r="C8" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="E8" s="54" t="s">
+      <c r="D8" s="53" t="s">
         <v>61</v>
       </c>
-      <c r="F8" s="50"/>
-    </row>
-    <row r="9" spans="1:6" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="E8" s="49"/>
+    </row>
+    <row r="9" spans="1:7" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A9" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="B9" s="54" t="s">
+      <c r="B9" s="53" t="s">
         <v>62</v>
       </c>
-      <c r="C9" s="49"/>
-      <c r="D9" s="6" t="s">
+      <c r="C9" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="E9" s="54" t="s">
+      <c r="D9" s="53" t="s">
         <v>63</v>
       </c>
-      <c r="F9" s="50"/>
-    </row>
-    <row r="10" spans="1:6" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="E9" s="49"/>
+    </row>
+    <row r="10" spans="1:7" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A10" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="B10" s="54" t="s">
+      <c r="B10" s="53" t="s">
         <v>64</v>
       </c>
-      <c r="C10" s="49"/>
-      <c r="D10" s="6" t="s">
+      <c r="C10" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="E10" s="54" t="s">
+      <c r="D10" s="53" t="s">
         <v>65</v>
       </c>
-      <c r="F10" s="50"/>
-    </row>
-    <row r="11" spans="1:6" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="E10" s="49"/>
+    </row>
+    <row r="11" spans="1:7" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A11" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="54" t="s">
+      <c r="B11" s="53" t="s">
         <v>66</v>
       </c>
-      <c r="C11" s="49"/>
-      <c r="D11" s="6" t="s">
+      <c r="C11" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="E11" s="54" t="s">
+      <c r="D11" s="53" t="s">
         <v>67</v>
       </c>
-      <c r="F11" s="50"/>
-    </row>
-    <row r="12" spans="1:6" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A12" s="50"/>
-      <c r="B12" s="50"/>
-      <c r="C12" s="50"/>
-      <c r="D12" s="50"/>
-      <c r="E12" s="50"/>
-      <c r="F12" s="50"/>
-    </row>
-    <row r="13" spans="1:6" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A13" s="50"/>
-      <c r="B13" s="50"/>
-      <c r="C13" s="50"/>
-      <c r="D13" s="50"/>
-      <c r="E13" s="50"/>
-      <c r="F13" s="50"/>
-    </row>
-    <row r="14" spans="1:6" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A14" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C14" s="50"/>
-      <c r="D14" s="50"/>
-      <c r="E14" s="50"/>
-      <c r="F14" s="50"/>
-    </row>
-    <row r="15" spans="1:6" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A15" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="B15" s="53" t="s">
-        <v>68</v>
-      </c>
-      <c r="C15" s="50"/>
-      <c r="D15" s="50"/>
-      <c r="E15" s="50"/>
-      <c r="F15" s="50"/>
-    </row>
-    <row r="16" spans="1:6" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A16" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="B16" s="53" t="s">
-        <v>69</v>
-      </c>
-      <c r="C16" s="49"/>
-      <c r="D16" s="50"/>
-      <c r="E16" s="50"/>
-      <c r="F16" s="50"/>
-    </row>
-    <row r="17" spans="1:6" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A17" s="50"/>
-      <c r="B17" s="50"/>
-      <c r="C17" s="50"/>
-      <c r="D17" s="50"/>
-      <c r="E17" s="50"/>
-      <c r="F17" s="50"/>
-    </row>
-    <row r="18" spans="1:6" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A18" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C18" s="50"/>
-      <c r="D18" s="50"/>
-      <c r="E18" s="50"/>
-      <c r="F18" s="50"/>
-    </row>
-    <row r="19" spans="1:6" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A19" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="B19" s="53" t="s">
-        <v>70</v>
-      </c>
-      <c r="C19" s="50"/>
-      <c r="D19" s="50"/>
-      <c r="E19" s="50"/>
-      <c r="F19" s="50"/>
-    </row>
-    <row r="20" spans="1:6" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A20" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="B20" s="53" t="s">
-        <v>71</v>
-      </c>
-      <c r="C20" s="50"/>
-      <c r="D20" s="50"/>
-      <c r="E20" s="50"/>
-      <c r="F20" s="50"/>
+      <c r="E11" s="49"/>
+    </row>
+    <row r="12" spans="1:7" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A12" s="49"/>
+      <c r="B12" s="49"/>
+      <c r="C12" s="49"/>
+      <c r="D12" s="49"/>
+      <c r="E12" s="49"/>
+    </row>
+    <row r="13" spans="1:7" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A13" s="49"/>
+      <c r="B13" s="49"/>
+      <c r="C13" s="49"/>
+      <c r="D13" s="49"/>
+      <c r="E13" s="49"/>
+    </row>
+    <row r="14" spans="1:7" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="D14" s="49"/>
+      <c r="E14" s="49"/>
+    </row>
+    <row r="15" spans="1:7" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="D15" s="49"/>
+      <c r="E15" s="49"/>
+    </row>
+    <row r="16" spans="1:7" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="D16" s="49"/>
+      <c r="E16" s="49"/>
+    </row>
+    <row r="17" spans="4:5" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="D17" s="49"/>
+      <c r="E17" s="49"/>
+    </row>
+    <row r="18" spans="4:5" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="D18" s="49"/>
+      <c r="E18" s="49"/>
+    </row>
+    <row r="19" spans="4:5" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="D19" s="49"/>
+      <c r="E19" s="49"/>
+    </row>
+    <row r="20" spans="4:5" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="D20" s="49"/>
+      <c r="E20" s="49"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1815,13 +1796,142 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1BC4CC0-FE9D-498F-AEB1-D5F0C0522F79}">
+  <dimension ref="A1:E20"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="D18" sqref="D18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="33.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="29.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="56.85546875" customWidth="1"/>
+    <col min="3" max="3" width="29.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="56.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="49"/>
+    </row>
+    <row r="2" spans="1:5" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A2" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="B2" s="50" t="s">
+        <v>75</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="D2" s="50" t="s">
+        <v>76</v>
+      </c>
+      <c r="E2" s="49"/>
+    </row>
+    <row r="3" spans="1:5" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A3" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="B3" s="50" t="s">
+        <v>77</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="D3" s="50" t="s">
+        <v>78</v>
+      </c>
+      <c r="E3" s="49"/>
+    </row>
+    <row r="4" spans="1:5" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A4" s="49"/>
+    </row>
+    <row r="5" spans="1:5" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A5" s="49"/>
+    </row>
+    <row r="6" spans="1:5" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A6" s="49"/>
+    </row>
+    <row r="7" spans="1:5" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A7" s="49"/>
+    </row>
+    <row r="8" spans="1:5" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A8" s="49"/>
+    </row>
+    <row r="9" spans="1:5" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A9" s="49"/>
+    </row>
+    <row r="10" spans="1:5" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A10" s="49"/>
+    </row>
+    <row r="11" spans="1:5" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A11" s="49"/>
+    </row>
+    <row r="12" spans="1:5" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A12" s="49"/>
+    </row>
+    <row r="13" spans="1:5" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A13" s="49"/>
+      <c r="B13" s="49"/>
+      <c r="C13" s="49"/>
+      <c r="D13" s="49"/>
+      <c r="E13" s="49"/>
+    </row>
+    <row r="14" spans="1:5" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A14" s="49"/>
+      <c r="B14" s="49"/>
+    </row>
+    <row r="15" spans="1:5" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A15" s="49"/>
+      <c r="B15" s="49"/>
+    </row>
+    <row r="16" spans="1:5" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A16" s="49"/>
+      <c r="B16" s="49"/>
+    </row>
+    <row r="17" spans="1:2" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A17" s="49"/>
+      <c r="B17" s="49"/>
+    </row>
+    <row r="18" spans="1:2" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A18" s="49"/>
+      <c r="B18" s="49"/>
+    </row>
+    <row r="19" spans="1:2" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A19" s="49"/>
+      <c r="B19" s="49"/>
+    </row>
+    <row r="20" spans="1:2" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A20" s="49"/>
+      <c r="B20" s="49"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{45F774DF-630E-4CCD-B16A-123A9D720A00}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:Z61"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="AD6" sqref="AD6"/>
     </sheetView>
   </sheetViews>
@@ -1854,23 +1964,23 @@
       <c r="H1" s="45"/>
       <c r="I1" s="45"/>
       <c r="J1" s="45"/>
-      <c r="K1" s="84" t="s">
+      <c r="K1" s="54" t="s">
         <v>72</v>
       </c>
-      <c r="L1" s="85"/>
-      <c r="M1" s="85"/>
-      <c r="N1" s="85"/>
-      <c r="O1" s="85"/>
-      <c r="P1" s="85"/>
-      <c r="Q1" s="85"/>
-      <c r="R1" s="85"/>
-      <c r="S1" s="85"/>
-      <c r="T1" s="85"/>
-      <c r="U1" s="85"/>
-      <c r="V1" s="85"/>
-      <c r="W1" s="85"/>
-      <c r="X1" s="85"/>
-      <c r="Y1" s="85"/>
+      <c r="L1" s="55"/>
+      <c r="M1" s="55"/>
+      <c r="N1" s="55"/>
+      <c r="O1" s="55"/>
+      <c r="P1" s="55"/>
+      <c r="Q1" s="55"/>
+      <c r="R1" s="55"/>
+      <c r="S1" s="55"/>
+      <c r="T1" s="55"/>
+      <c r="U1" s="55"/>
+      <c r="V1" s="55"/>
+      <c r="W1" s="55"/>
+      <c r="X1" s="55"/>
+      <c r="Y1" s="55"/>
       <c r="Z1" s="44"/>
     </row>
     <row r="2" spans="1:26" x14ac:dyDescent="0.2">
@@ -1879,24 +1989,24 @@
     </row>
     <row r="3" spans="1:26" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="43"/>
-      <c r="K3" s="86" t="s">
+      <c r="K3" s="56" t="s">
         <v>38</v>
       </c>
-      <c r="L3" s="86"/>
-      <c r="M3" s="86"/>
-      <c r="N3" s="86"/>
-      <c r="O3" s="86"/>
-      <c r="P3" s="86"/>
-      <c r="Q3" s="86"/>
-      <c r="S3" s="86" t="s">
+      <c r="L3" s="56"/>
+      <c r="M3" s="56"/>
+      <c r="N3" s="56"/>
+      <c r="O3" s="56"/>
+      <c r="P3" s="56"/>
+      <c r="Q3" s="56"/>
+      <c r="S3" s="56" t="s">
         <v>39</v>
       </c>
-      <c r="T3" s="86"/>
-      <c r="U3" s="86"/>
-      <c r="V3" s="86"/>
-      <c r="W3" s="86"/>
-      <c r="X3" s="86"/>
-      <c r="Y3" s="86"/>
+      <c r="T3" s="56"/>
+      <c r="U3" s="56"/>
+      <c r="V3" s="56"/>
+      <c r="W3" s="56"/>
+      <c r="X3" s="56"/>
+      <c r="Y3" s="56"/>
       <c r="Z3" s="42"/>
     </row>
     <row r="4" spans="1:26" ht="14.25" x14ac:dyDescent="0.2">
@@ -1910,25 +2020,25 @@
       <c r="H4" s="25"/>
       <c r="I4" s="25"/>
       <c r="J4" s="25"/>
-      <c r="K4" s="87" t="s">
+      <c r="K4" s="57" t="s">
         <v>18</v>
       </c>
-      <c r="L4" s="87"/>
-      <c r="M4" s="87"/>
-      <c r="N4" s="87"/>
-      <c r="O4" s="87"/>
-      <c r="P4" s="87"/>
-      <c r="Q4" s="87"/>
+      <c r="L4" s="57"/>
+      <c r="M4" s="57"/>
+      <c r="N4" s="57"/>
+      <c r="O4" s="57"/>
+      <c r="P4" s="57"/>
+      <c r="Q4" s="57"/>
       <c r="R4" s="26"/>
-      <c r="S4" s="87" t="s">
+      <c r="S4" s="57" t="s">
         <v>17</v>
       </c>
-      <c r="T4" s="87"/>
-      <c r="U4" s="87"/>
-      <c r="V4" s="87"/>
-      <c r="W4" s="87"/>
-      <c r="X4" s="87"/>
-      <c r="Y4" s="87"/>
+      <c r="T4" s="57"/>
+      <c r="U4" s="57"/>
+      <c r="V4" s="57"/>
+      <c r="W4" s="57"/>
+      <c r="X4" s="57"/>
+      <c r="Y4" s="57"/>
       <c r="Z4" s="40"/>
     </row>
     <row r="5" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
@@ -1942,25 +2052,25 @@
       <c r="H5" s="25"/>
       <c r="I5" s="25"/>
       <c r="J5" s="25"/>
-      <c r="K5" s="88" t="s">
+      <c r="K5" s="58" t="s">
         <v>44</v>
       </c>
-      <c r="L5" s="88"/>
-      <c r="M5" s="88"/>
-      <c r="N5" s="88"/>
-      <c r="O5" s="88"/>
-      <c r="P5" s="88"/>
-      <c r="Q5" s="88"/>
+      <c r="L5" s="58"/>
+      <c r="M5" s="58"/>
+      <c r="N5" s="58"/>
+      <c r="O5" s="58"/>
+      <c r="P5" s="58"/>
+      <c r="Q5" s="58"/>
       <c r="R5" s="26"/>
-      <c r="S5" s="88" t="s">
+      <c r="S5" s="58" t="s">
         <v>37</v>
       </c>
-      <c r="T5" s="88"/>
-      <c r="U5" s="88"/>
-      <c r="V5" s="88"/>
-      <c r="W5" s="88"/>
-      <c r="X5" s="88"/>
-      <c r="Y5" s="88"/>
+      <c r="T5" s="58"/>
+      <c r="U5" s="58"/>
+      <c r="V5" s="58"/>
+      <c r="W5" s="58"/>
+      <c r="X5" s="58"/>
+      <c r="Y5" s="58"/>
       <c r="Z5" s="40"/>
     </row>
     <row r="6" spans="1:26" x14ac:dyDescent="0.2">
@@ -1974,25 +2084,25 @@
       <c r="H6" s="25"/>
       <c r="I6" s="25"/>
       <c r="J6" s="25"/>
-      <c r="K6" s="89" t="s">
+      <c r="K6" s="59" t="s">
         <v>36</v>
       </c>
-      <c r="L6" s="89"/>
-      <c r="M6" s="89"/>
-      <c r="N6" s="89"/>
-      <c r="O6" s="89"/>
-      <c r="P6" s="89"/>
-      <c r="Q6" s="89"/>
+      <c r="L6" s="59"/>
+      <c r="M6" s="59"/>
+      <c r="N6" s="59"/>
+      <c r="O6" s="59"/>
+      <c r="P6" s="59"/>
+      <c r="Q6" s="59"/>
       <c r="R6" s="26"/>
-      <c r="S6" s="89" t="s">
+      <c r="S6" s="59" t="s">
         <v>35</v>
       </c>
-      <c r="T6" s="89"/>
-      <c r="U6" s="89"/>
-      <c r="V6" s="89"/>
-      <c r="W6" s="89"/>
-      <c r="X6" s="89"/>
-      <c r="Y6" s="89"/>
+      <c r="T6" s="59"/>
+      <c r="U6" s="59"/>
+      <c r="V6" s="59"/>
+      <c r="W6" s="59"/>
+      <c r="X6" s="59"/>
+      <c r="Y6" s="59"/>
       <c r="Z6" s="40"/>
     </row>
     <row r="7" spans="1:26" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
@@ -2007,18 +2117,18 @@
       <c r="I7" s="25"/>
       <c r="J7" s="25"/>
       <c r="K7" s="26"/>
-      <c r="L7" s="78" t="s">
+      <c r="L7" s="60" t="s">
         <v>45</v>
       </c>
-      <c r="M7" s="59"/>
-      <c r="N7" s="59"/>
-      <c r="O7" s="60"/>
+      <c r="M7" s="61"/>
+      <c r="N7" s="61"/>
+      <c r="O7" s="62"/>
       <c r="P7" s="26"/>
-      <c r="Q7" s="61" t="s">
+      <c r="Q7" s="63" t="s">
         <v>34</v>
       </c>
-      <c r="R7" s="59"/>
-      <c r="S7" s="60"/>
+      <c r="R7" s="61"/>
+      <c r="S7" s="62"/>
       <c r="T7" s="26"/>
       <c r="U7" s="26"/>
       <c r="V7" s="26"/>
@@ -2028,33 +2138,33 @@
       <c r="Z7" s="40"/>
     </row>
     <row r="8" spans="1:26" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="66" t="s">
+      <c r="A8" s="64" t="s">
         <v>18</v>
       </c>
-      <c r="B8" s="67"/>
-      <c r="C8" s="67"/>
-      <c r="D8" s="68" t="s">
+      <c r="B8" s="65"/>
+      <c r="C8" s="65"/>
+      <c r="D8" s="66" t="s">
         <v>33</v>
       </c>
-      <c r="E8" s="69"/>
-      <c r="F8" s="69"/>
-      <c r="G8" s="69"/>
-      <c r="H8" s="69"/>
-      <c r="I8" s="69"/>
-      <c r="J8" s="79"/>
+      <c r="E8" s="67"/>
+      <c r="F8" s="67"/>
+      <c r="G8" s="67"/>
+      <c r="H8" s="67"/>
+      <c r="I8" s="67"/>
+      <c r="J8" s="68"/>
       <c r="K8" s="26"/>
-      <c r="L8" s="80" t="s">
+      <c r="L8" s="69" t="s">
         <v>32</v>
       </c>
-      <c r="M8" s="80"/>
-      <c r="N8" s="80"/>
-      <c r="O8" s="80"/>
+      <c r="M8" s="69"/>
+      <c r="N8" s="69"/>
+      <c r="O8" s="69"/>
       <c r="P8" s="26"/>
-      <c r="Q8" s="80" t="s">
+      <c r="Q8" s="69" t="s">
         <v>31</v>
       </c>
-      <c r="R8" s="80"/>
-      <c r="S8" s="80"/>
+      <c r="R8" s="69"/>
+      <c r="S8" s="69"/>
       <c r="T8" s="26"/>
       <c r="U8" s="41"/>
       <c r="V8" s="26"/>
@@ -2078,24 +2188,24 @@
       <c r="H9" s="72"/>
       <c r="I9" s="72"/>
       <c r="J9" s="73"/>
-      <c r="K9" s="81" t="s">
+      <c r="K9" s="74" t="s">
         <v>30</v>
       </c>
-      <c r="L9" s="82"/>
-      <c r="M9" s="82"/>
-      <c r="N9" s="82"/>
-      <c r="O9" s="82"/>
-      <c r="P9" s="82"/>
-      <c r="Q9" s="82"/>
-      <c r="R9" s="82"/>
-      <c r="S9" s="82"/>
-      <c r="T9" s="82"/>
-      <c r="U9" s="82"/>
-      <c r="V9" s="82"/>
-      <c r="W9" s="82"/>
-      <c r="X9" s="82"/>
-      <c r="Y9" s="82"/>
-      <c r="Z9" s="83"/>
+      <c r="L9" s="75"/>
+      <c r="M9" s="75"/>
+      <c r="N9" s="75"/>
+      <c r="O9" s="75"/>
+      <c r="P9" s="75"/>
+      <c r="Q9" s="75"/>
+      <c r="R9" s="75"/>
+      <c r="S9" s="75"/>
+      <c r="T9" s="75"/>
+      <c r="U9" s="75"/>
+      <c r="V9" s="75"/>
+      <c r="W9" s="75"/>
+      <c r="X9" s="75"/>
+      <c r="Y9" s="75"/>
+      <c r="Z9" s="76"/>
     </row>
     <row r="10" spans="1:26" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" s="27"/>
@@ -2118,38 +2228,38 @@
         <v>4</v>
       </c>
       <c r="J10" s="25"/>
-      <c r="K10" s="74" t="s">
+      <c r="K10" s="77" t="s">
         <v>15</v>
       </c>
-      <c r="L10" s="75"/>
-      <c r="M10" s="75" t="s">
+      <c r="L10" s="78"/>
+      <c r="M10" s="78" t="s">
         <v>14</v>
       </c>
-      <c r="N10" s="76"/>
-      <c r="O10" s="74" t="s">
+      <c r="N10" s="79"/>
+      <c r="O10" s="77" t="s">
         <v>15</v>
       </c>
-      <c r="P10" s="75"/>
-      <c r="Q10" s="75" t="s">
+      <c r="P10" s="78"/>
+      <c r="Q10" s="78" t="s">
         <v>14</v>
       </c>
-      <c r="R10" s="76"/>
-      <c r="S10" s="74" t="s">
+      <c r="R10" s="79"/>
+      <c r="S10" s="77" t="s">
         <v>15</v>
       </c>
-      <c r="T10" s="75"/>
-      <c r="U10" s="75" t="s">
+      <c r="T10" s="78"/>
+      <c r="U10" s="78" t="s">
         <v>14</v>
       </c>
-      <c r="V10" s="76"/>
-      <c r="W10" s="74" t="s">
+      <c r="V10" s="79"/>
+      <c r="W10" s="77" t="s">
         <v>15</v>
       </c>
-      <c r="X10" s="75"/>
-      <c r="Y10" s="75" t="s">
+      <c r="X10" s="78"/>
+      <c r="Y10" s="78" t="s">
         <v>14</v>
       </c>
-      <c r="Z10" s="76"/>
+      <c r="Z10" s="79"/>
     </row>
     <row r="11" spans="1:26" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A11" s="27"/>
@@ -2356,18 +2466,18 @@
       <c r="Z14" s="18"/>
     </row>
     <row r="15" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A15" s="58"/>
-      <c r="B15" s="77"/>
+      <c r="A15" s="80"/>
+      <c r="B15" s="81"/>
       <c r="C15" s="26"/>
       <c r="D15" s="25"/>
       <c r="E15" s="25"/>
-      <c r="F15" s="61" t="s">
+      <c r="F15" s="63" t="s">
         <v>25</v>
       </c>
-      <c r="G15" s="59"/>
-      <c r="H15" s="59"/>
-      <c r="I15" s="59"/>
-      <c r="J15" s="59"/>
+      <c r="G15" s="61"/>
+      <c r="H15" s="61"/>
+      <c r="I15" s="61"/>
+      <c r="J15" s="61"/>
       <c r="K15" s="19"/>
       <c r="L15" s="10">
         <v>5</v>
@@ -2402,15 +2512,15 @@
       <c r="Z15" s="18"/>
     </row>
     <row r="16" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A16" s="61" t="s">
+      <c r="A16" s="63" t="s">
         <v>24</v>
       </c>
-      <c r="B16" s="59"/>
-      <c r="C16" s="60"/>
-      <c r="D16" s="64" t="s">
+      <c r="B16" s="61"/>
+      <c r="C16" s="62"/>
+      <c r="D16" s="82" t="s">
         <v>23</v>
       </c>
-      <c r="E16" s="65"/>
+      <c r="E16" s="83"/>
       <c r="F16" s="24">
         <v>1</v>
       </c>
@@ -2460,15 +2570,15 @@
       <c r="Z16" s="18"/>
     </row>
     <row r="17" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A17" s="58" t="s">
+      <c r="A17" s="80" t="s">
         <v>41</v>
       </c>
-      <c r="B17" s="59"/>
-      <c r="C17" s="60"/>
-      <c r="D17" s="61" t="s">
+      <c r="B17" s="61"/>
+      <c r="C17" s="62"/>
+      <c r="D17" s="63" t="s">
         <v>40</v>
       </c>
-      <c r="E17" s="60"/>
+      <c r="E17" s="62"/>
       <c r="F17" s="21"/>
       <c r="G17" s="11"/>
       <c r="H17" s="11"/>
@@ -2508,11 +2618,11 @@
       <c r="Z17" s="18"/>
     </row>
     <row r="18" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A18" s="58"/>
-      <c r="B18" s="59"/>
-      <c r="C18" s="60"/>
-      <c r="D18" s="61"/>
-      <c r="E18" s="60"/>
+      <c r="A18" s="80"/>
+      <c r="B18" s="61"/>
+      <c r="C18" s="62"/>
+      <c r="D18" s="63"/>
+      <c r="E18" s="62"/>
       <c r="F18" s="21"/>
       <c r="G18" s="11"/>
       <c r="H18" s="11"/>
@@ -2552,11 +2662,11 @@
       <c r="Z18" s="18"/>
     </row>
     <row r="19" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A19" s="58"/>
-      <c r="B19" s="59"/>
-      <c r="C19" s="60"/>
-      <c r="D19" s="61"/>
-      <c r="E19" s="60"/>
+      <c r="A19" s="80"/>
+      <c r="B19" s="61"/>
+      <c r="C19" s="62"/>
+      <c r="D19" s="63"/>
+      <c r="E19" s="62"/>
       <c r="F19" s="21"/>
       <c r="G19" s="11"/>
       <c r="H19" s="11"/>
@@ -2596,11 +2706,11 @@
       <c r="Z19" s="18"/>
     </row>
     <row r="20" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A20" s="58"/>
-      <c r="B20" s="59"/>
-      <c r="C20" s="60"/>
-      <c r="D20" s="61"/>
-      <c r="E20" s="60"/>
+      <c r="A20" s="80"/>
+      <c r="B20" s="61"/>
+      <c r="C20" s="62"/>
+      <c r="D20" s="63"/>
+      <c r="E20" s="62"/>
       <c r="F20" s="21"/>
       <c r="G20" s="11"/>
       <c r="H20" s="11"/>
@@ -2640,11 +2750,11 @@
       <c r="Z20" s="18"/>
     </row>
     <row r="21" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A21" s="58"/>
-      <c r="B21" s="59"/>
-      <c r="C21" s="60"/>
-      <c r="D21" s="61"/>
-      <c r="E21" s="60"/>
+      <c r="A21" s="80"/>
+      <c r="B21" s="61"/>
+      <c r="C21" s="62"/>
+      <c r="D21" s="63"/>
+      <c r="E21" s="62"/>
       <c r="F21" s="21"/>
       <c r="G21" s="11"/>
       <c r="H21" s="11"/>
@@ -2684,11 +2794,11 @@
       <c r="Z21" s="18"/>
     </row>
     <row r="22" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A22" s="58"/>
-      <c r="B22" s="59"/>
-      <c r="C22" s="60"/>
-      <c r="D22" s="61"/>
-      <c r="E22" s="60"/>
+      <c r="A22" s="80"/>
+      <c r="B22" s="61"/>
+      <c r="C22" s="62"/>
+      <c r="D22" s="63"/>
+      <c r="E22" s="62"/>
       <c r="F22" s="21"/>
       <c r="G22" s="11"/>
       <c r="H22" s="11"/>
@@ -2728,11 +2838,11 @@
       <c r="Z22" s="18"/>
     </row>
     <row r="23" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A23" s="58"/>
-      <c r="B23" s="59"/>
-      <c r="C23" s="60"/>
-      <c r="D23" s="61"/>
-      <c r="E23" s="60"/>
+      <c r="A23" s="80"/>
+      <c r="B23" s="61"/>
+      <c r="C23" s="62"/>
+      <c r="D23" s="63"/>
+      <c r="E23" s="62"/>
       <c r="F23" s="21"/>
       <c r="G23" s="11"/>
       <c r="H23" s="11"/>
@@ -2772,11 +2882,11 @@
       <c r="Z23" s="18"/>
     </row>
     <row r="24" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A24" s="58"/>
-      <c r="B24" s="59"/>
-      <c r="C24" s="60"/>
-      <c r="D24" s="61"/>
-      <c r="E24" s="60"/>
+      <c r="A24" s="80"/>
+      <c r="B24" s="61"/>
+      <c r="C24" s="62"/>
+      <c r="D24" s="63"/>
+      <c r="E24" s="62"/>
       <c r="F24" s="21"/>
       <c r="G24" s="11"/>
       <c r="H24" s="11"/>
@@ -2816,11 +2926,11 @@
       <c r="Z24" s="18"/>
     </row>
     <row r="25" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A25" s="58"/>
-      <c r="B25" s="59"/>
-      <c r="C25" s="60"/>
-      <c r="D25" s="61"/>
-      <c r="E25" s="60"/>
+      <c r="A25" s="80"/>
+      <c r="B25" s="61"/>
+      <c r="C25" s="62"/>
+      <c r="D25" s="63"/>
+      <c r="E25" s="62"/>
       <c r="F25" s="21"/>
       <c r="G25" s="11"/>
       <c r="H25" s="11"/>
@@ -2860,11 +2970,11 @@
       <c r="Z25" s="18"/>
     </row>
     <row r="26" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A26" s="58"/>
-      <c r="B26" s="59"/>
-      <c r="C26" s="60"/>
-      <c r="D26" s="61"/>
-      <c r="E26" s="60"/>
+      <c r="A26" s="80"/>
+      <c r="B26" s="61"/>
+      <c r="C26" s="62"/>
+      <c r="D26" s="63"/>
+      <c r="E26" s="62"/>
       <c r="F26" s="21"/>
       <c r="G26" s="11"/>
       <c r="H26" s="11"/>
@@ -2904,11 +3014,11 @@
       <c r="Z26" s="18"/>
     </row>
     <row r="27" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A27" s="58"/>
-      <c r="B27" s="59"/>
-      <c r="C27" s="60"/>
-      <c r="D27" s="61"/>
-      <c r="E27" s="60"/>
+      <c r="A27" s="80"/>
+      <c r="B27" s="61"/>
+      <c r="C27" s="62"/>
+      <c r="D27" s="63"/>
+      <c r="E27" s="62"/>
       <c r="F27" s="21"/>
       <c r="G27" s="11"/>
       <c r="H27" s="11"/>
@@ -2948,11 +3058,11 @@
       <c r="Z27" s="18"/>
     </row>
     <row r="28" spans="1:26" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="58"/>
-      <c r="B28" s="59"/>
-      <c r="C28" s="60"/>
-      <c r="D28" s="61"/>
-      <c r="E28" s="60"/>
+      <c r="A28" s="80"/>
+      <c r="B28" s="61"/>
+      <c r="C28" s="62"/>
+      <c r="D28" s="63"/>
+      <c r="E28" s="62"/>
       <c r="F28" s="21"/>
       <c r="G28" s="11"/>
       <c r="H28" s="11"/>
@@ -2992,20 +3102,20 @@
       <c r="Z28" s="18"/>
     </row>
     <row r="29" spans="1:26" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="66" t="s">
+      <c r="A29" s="64" t="s">
         <v>17</v>
       </c>
-      <c r="B29" s="67"/>
-      <c r="C29" s="67"/>
-      <c r="D29" s="68" t="s">
+      <c r="B29" s="65"/>
+      <c r="C29" s="65"/>
+      <c r="D29" s="66" t="s">
         <v>29</v>
       </c>
-      <c r="E29" s="69"/>
-      <c r="F29" s="69"/>
-      <c r="G29" s="69"/>
-      <c r="H29" s="69"/>
-      <c r="I29" s="69"/>
-      <c r="J29" s="69"/>
+      <c r="E29" s="67"/>
+      <c r="F29" s="67"/>
+      <c r="G29" s="67"/>
+      <c r="H29" s="67"/>
+      <c r="I29" s="67"/>
+      <c r="J29" s="67"/>
       <c r="K29" s="19"/>
       <c r="L29" s="10">
         <v>19</v>
@@ -3346,18 +3456,18 @@
       <c r="Z35" s="18"/>
     </row>
     <row r="36" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A36" s="58"/>
-      <c r="B36" s="63"/>
+      <c r="A36" s="80"/>
+      <c r="B36" s="84"/>
       <c r="C36" s="26"/>
       <c r="D36" s="25"/>
       <c r="E36" s="25"/>
-      <c r="F36" s="61" t="s">
+      <c r="F36" s="63" t="s">
         <v>25</v>
       </c>
-      <c r="G36" s="59"/>
-      <c r="H36" s="59"/>
-      <c r="I36" s="59"/>
-      <c r="J36" s="59"/>
+      <c r="G36" s="61"/>
+      <c r="H36" s="61"/>
+      <c r="I36" s="61"/>
+      <c r="J36" s="61"/>
       <c r="K36" s="19"/>
       <c r="L36" s="10">
         <v>26</v>
@@ -3392,15 +3502,15 @@
       <c r="Z36" s="18"/>
     </row>
     <row r="37" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A37" s="61" t="s">
+      <c r="A37" s="63" t="s">
         <v>24</v>
       </c>
-      <c r="B37" s="59"/>
-      <c r="C37" s="60"/>
-      <c r="D37" s="64" t="s">
+      <c r="B37" s="61"/>
+      <c r="C37" s="62"/>
+      <c r="D37" s="82" t="s">
         <v>23</v>
       </c>
-      <c r="E37" s="65"/>
+      <c r="E37" s="83"/>
       <c r="F37" s="24">
         <v>1</v>
       </c>
@@ -3450,15 +3560,15 @@
       <c r="Z37" s="18"/>
     </row>
     <row r="38" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A38" s="58" t="s">
+      <c r="A38" s="80" t="s">
         <v>42</v>
       </c>
-      <c r="B38" s="59"/>
-      <c r="C38" s="60"/>
-      <c r="D38" s="61" t="s">
+      <c r="B38" s="61"/>
+      <c r="C38" s="62"/>
+      <c r="D38" s="63" t="s">
         <v>43</v>
       </c>
-      <c r="E38" s="60"/>
+      <c r="E38" s="62"/>
       <c r="F38" s="21"/>
       <c r="G38" s="11"/>
       <c r="H38" s="11"/>
@@ -3498,11 +3608,11 @@
       <c r="Z38" s="18"/>
     </row>
     <row r="39" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A39" s="58"/>
-      <c r="B39" s="59"/>
-      <c r="C39" s="60"/>
-      <c r="D39" s="61"/>
-      <c r="E39" s="60"/>
+      <c r="A39" s="80"/>
+      <c r="B39" s="61"/>
+      <c r="C39" s="62"/>
+      <c r="D39" s="63"/>
+      <c r="E39" s="62"/>
       <c r="F39" s="21"/>
       <c r="G39" s="11"/>
       <c r="H39" s="11"/>
@@ -3542,11 +3652,11 @@
       <c r="Z39" s="18"/>
     </row>
     <row r="40" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A40" s="58"/>
-      <c r="B40" s="59"/>
-      <c r="C40" s="60"/>
-      <c r="D40" s="61"/>
-      <c r="E40" s="60"/>
+      <c r="A40" s="80"/>
+      <c r="B40" s="61"/>
+      <c r="C40" s="62"/>
+      <c r="D40" s="63"/>
+      <c r="E40" s="62"/>
       <c r="F40" s="21"/>
       <c r="G40" s="11"/>
       <c r="H40" s="11"/>
@@ -3586,11 +3696,11 @@
       <c r="Z40" s="18"/>
     </row>
     <row r="41" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A41" s="58"/>
-      <c r="B41" s="59"/>
-      <c r="C41" s="60"/>
-      <c r="D41" s="61"/>
-      <c r="E41" s="60"/>
+      <c r="A41" s="80"/>
+      <c r="B41" s="61"/>
+      <c r="C41" s="62"/>
+      <c r="D41" s="63"/>
+      <c r="E41" s="62"/>
       <c r="F41" s="21"/>
       <c r="G41" s="11"/>
       <c r="H41" s="11"/>
@@ -3630,11 +3740,11 @@
       <c r="Z41" s="18"/>
     </row>
     <row r="42" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A42" s="58"/>
-      <c r="B42" s="59"/>
-      <c r="C42" s="60"/>
-      <c r="D42" s="61"/>
-      <c r="E42" s="60"/>
+      <c r="A42" s="80"/>
+      <c r="B42" s="61"/>
+      <c r="C42" s="62"/>
+      <c r="D42" s="63"/>
+      <c r="E42" s="62"/>
       <c r="F42" s="21"/>
       <c r="G42" s="11"/>
       <c r="H42" s="11"/>
@@ -3674,11 +3784,11 @@
       <c r="Z42" s="18"/>
     </row>
     <row r="43" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A43" s="58"/>
-      <c r="B43" s="59"/>
-      <c r="C43" s="60"/>
-      <c r="D43" s="61"/>
-      <c r="E43" s="60"/>
+      <c r="A43" s="80"/>
+      <c r="B43" s="61"/>
+      <c r="C43" s="62"/>
+      <c r="D43" s="63"/>
+      <c r="E43" s="62"/>
       <c r="F43" s="21"/>
       <c r="G43" s="11"/>
       <c r="H43" s="11"/>
@@ -3718,11 +3828,11 @@
       <c r="Z43" s="18"/>
     </row>
     <row r="44" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A44" s="58"/>
-      <c r="B44" s="59"/>
-      <c r="C44" s="60"/>
-      <c r="D44" s="61"/>
-      <c r="E44" s="60"/>
+      <c r="A44" s="80"/>
+      <c r="B44" s="61"/>
+      <c r="C44" s="62"/>
+      <c r="D44" s="63"/>
+      <c r="E44" s="62"/>
       <c r="F44" s="21"/>
       <c r="G44" s="11"/>
       <c r="H44" s="11"/>
@@ -3762,11 +3872,11 @@
       <c r="Z44" s="18"/>
     </row>
     <row r="45" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A45" s="58"/>
-      <c r="B45" s="59"/>
-      <c r="C45" s="60"/>
-      <c r="D45" s="61"/>
-      <c r="E45" s="60"/>
+      <c r="A45" s="80"/>
+      <c r="B45" s="61"/>
+      <c r="C45" s="62"/>
+      <c r="D45" s="63"/>
+      <c r="E45" s="62"/>
       <c r="F45" s="21"/>
       <c r="G45" s="11"/>
       <c r="H45" s="11"/>
@@ -3806,11 +3916,11 @@
       <c r="Z45" s="18"/>
     </row>
     <row r="46" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A46" s="58"/>
-      <c r="B46" s="59"/>
-      <c r="C46" s="60"/>
-      <c r="D46" s="61"/>
-      <c r="E46" s="60"/>
+      <c r="A46" s="80"/>
+      <c r="B46" s="61"/>
+      <c r="C46" s="62"/>
+      <c r="D46" s="63"/>
+      <c r="E46" s="62"/>
       <c r="F46" s="21"/>
       <c r="G46" s="11"/>
       <c r="H46" s="11"/>
@@ -3850,11 +3960,11 @@
       <c r="Z46" s="18"/>
     </row>
     <row r="47" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A47" s="58"/>
-      <c r="B47" s="59"/>
-      <c r="C47" s="60"/>
-      <c r="D47" s="61"/>
-      <c r="E47" s="60"/>
+      <c r="A47" s="80"/>
+      <c r="B47" s="61"/>
+      <c r="C47" s="62"/>
+      <c r="D47" s="63"/>
+      <c r="E47" s="62"/>
       <c r="F47" s="21"/>
       <c r="G47" s="11"/>
       <c r="H47" s="11"/>
@@ -3894,11 +4004,11 @@
       <c r="Z47" s="18"/>
     </row>
     <row r="48" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A48" s="58"/>
-      <c r="B48" s="59"/>
-      <c r="C48" s="60"/>
-      <c r="D48" s="61"/>
-      <c r="E48" s="60"/>
+      <c r="A48" s="80"/>
+      <c r="B48" s="61"/>
+      <c r="C48" s="62"/>
+      <c r="D48" s="63"/>
+      <c r="E48" s="62"/>
       <c r="F48" s="21"/>
       <c r="G48" s="11"/>
       <c r="H48" s="11"/>
@@ -3938,11 +4048,11 @@
       <c r="Z48" s="18"/>
     </row>
     <row r="49" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A49" s="58"/>
-      <c r="B49" s="59"/>
-      <c r="C49" s="60"/>
-      <c r="D49" s="61"/>
-      <c r="E49" s="60"/>
+      <c r="A49" s="80"/>
+      <c r="B49" s="61"/>
+      <c r="C49" s="62"/>
+      <c r="D49" s="63"/>
+      <c r="E49" s="62"/>
       <c r="F49" s="21"/>
       <c r="G49" s="11"/>
       <c r="H49" s="11"/>
@@ -3983,11 +4093,11 @@
     </row>
     <row r="50" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A50" s="17"/>
-      <c r="B50" s="62" t="s">
+      <c r="B50" s="85" t="s">
         <v>22</v>
       </c>
-      <c r="C50" s="62"/>
-      <c r="D50" s="62"/>
+      <c r="C50" s="85"/>
+      <c r="D50" s="85"/>
       <c r="E50" s="17"/>
       <c r="F50" s="17"/>
       <c r="G50" s="17"/>
@@ -4029,21 +4139,21 @@
     </row>
     <row r="51" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A51" s="12"/>
-      <c r="B51" s="56" t="s">
+      <c r="B51" s="86" t="s">
         <v>21</v>
       </c>
-      <c r="C51" s="56"/>
-      <c r="D51" s="56"/>
+      <c r="C51" s="86"/>
+      <c r="D51" s="86"/>
       <c r="E51" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="F51" s="56"/>
-      <c r="G51" s="56"/>
+      <c r="F51" s="86"/>
+      <c r="G51" s="86"/>
       <c r="H51" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="I51" s="56"/>
-      <c r="J51" s="56"/>
+      <c r="I51" s="86"/>
+      <c r="J51" s="86"/>
       <c r="K51" s="10"/>
       <c r="L51" s="10"/>
       <c r="M51" s="10"/>
@@ -4063,78 +4173,78 @@
     </row>
     <row r="52" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A52" s="11"/>
-      <c r="B52" s="56" t="s">
+      <c r="B52" s="86" t="s">
         <v>20</v>
       </c>
-      <c r="C52" s="56"/>
-      <c r="D52" s="56"/>
+      <c r="C52" s="86"/>
+      <c r="D52" s="86"/>
       <c r="E52" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="F52" s="56"/>
-      <c r="G52" s="56"/>
+      <c r="F52" s="86"/>
+      <c r="G52" s="86"/>
       <c r="H52" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="I52" s="56"/>
-      <c r="J52" s="56"/>
+      <c r="I52" s="86"/>
+      <c r="J52" s="86"/>
       <c r="K52" s="10"/>
-      <c r="L52" s="57" t="s">
+      <c r="L52" s="87" t="s">
         <v>19</v>
       </c>
-      <c r="M52" s="57"/>
-      <c r="N52" s="57"/>
-      <c r="O52" s="57"/>
-      <c r="P52" s="56" t="s">
+      <c r="M52" s="87"/>
+      <c r="N52" s="87"/>
+      <c r="O52" s="87"/>
+      <c r="P52" s="86" t="s">
         <v>18</v>
       </c>
-      <c r="Q52" s="56"/>
-      <c r="R52" s="56"/>
-      <c r="S52" s="56"/>
-      <c r="T52" s="56"/>
-      <c r="U52" s="56" t="s">
+      <c r="Q52" s="86"/>
+      <c r="R52" s="86"/>
+      <c r="S52" s="86"/>
+      <c r="T52" s="86"/>
+      <c r="U52" s="86" t="s">
         <v>17</v>
       </c>
-      <c r="V52" s="56"/>
-      <c r="W52" s="56"/>
-      <c r="X52" s="56"/>
-      <c r="Y52" s="56"/>
+      <c r="V52" s="86"/>
+      <c r="W52" s="86"/>
+      <c r="X52" s="86"/>
+      <c r="Y52" s="86"/>
       <c r="Z52" s="10"/>
     </row>
     <row r="53" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A53" s="11"/>
-      <c r="B53" s="57" t="s">
+      <c r="B53" s="87" t="s">
         <v>16</v>
       </c>
-      <c r="C53" s="57"/>
-      <c r="D53" s="57"/>
+      <c r="C53" s="87"/>
+      <c r="D53" s="87"/>
       <c r="E53" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="F53" s="56"/>
-      <c r="G53" s="56"/>
+      <c r="F53" s="86"/>
+      <c r="G53" s="86"/>
       <c r="H53" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="I53" s="56"/>
-      <c r="J53" s="56"/>
-      <c r="K53" s="57" t="s">
+      <c r="I53" s="86"/>
+      <c r="J53" s="86"/>
+      <c r="K53" s="87" t="s">
         <v>13</v>
       </c>
-      <c r="L53" s="57"/>
-      <c r="M53" s="57"/>
-      <c r="N53" s="57"/>
-      <c r="O53" s="57"/>
-      <c r="P53" s="57"/>
-      <c r="Q53" s="57"/>
-      <c r="R53" s="56"/>
-      <c r="S53" s="56"/>
-      <c r="T53" s="56"/>
-      <c r="U53" s="56"/>
-      <c r="V53" s="56"/>
-      <c r="W53" s="56"/>
-      <c r="X53" s="56"/>
-      <c r="Y53" s="56"/>
+      <c r="L53" s="87"/>
+      <c r="M53" s="87"/>
+      <c r="N53" s="87"/>
+      <c r="O53" s="87"/>
+      <c r="P53" s="87"/>
+      <c r="Q53" s="87"/>
+      <c r="R53" s="86"/>
+      <c r="S53" s="86"/>
+      <c r="T53" s="86"/>
+      <c r="U53" s="86"/>
+      <c r="V53" s="86"/>
+      <c r="W53" s="86"/>
+      <c r="X53" s="86"/>
+      <c r="Y53" s="86"/>
       <c r="Z53" s="10"/>
     </row>
     <row r="55" spans="1:26" x14ac:dyDescent="0.2">
@@ -4266,93 +4376,6 @@
     </row>
   </sheetData>
   <mergeCells count="103">
-    <mergeCell ref="K1:Y1"/>
-    <mergeCell ref="K3:Q3"/>
-    <mergeCell ref="S3:Y3"/>
-    <mergeCell ref="K4:Q4"/>
-    <mergeCell ref="S4:Y4"/>
-    <mergeCell ref="K5:Q5"/>
-    <mergeCell ref="S5:Y5"/>
-    <mergeCell ref="K6:Q6"/>
-    <mergeCell ref="S6:Y6"/>
-    <mergeCell ref="L7:O7"/>
-    <mergeCell ref="Q7:S7"/>
-    <mergeCell ref="A8:C8"/>
-    <mergeCell ref="D8:J8"/>
-    <mergeCell ref="L8:O8"/>
-    <mergeCell ref="Q8:S8"/>
-    <mergeCell ref="A9:C9"/>
-    <mergeCell ref="E9:J9"/>
-    <mergeCell ref="K9:Z9"/>
-    <mergeCell ref="K10:L10"/>
-    <mergeCell ref="M10:N10"/>
-    <mergeCell ref="O10:P10"/>
-    <mergeCell ref="Q10:R10"/>
-    <mergeCell ref="S10:T10"/>
-    <mergeCell ref="U10:V10"/>
-    <mergeCell ref="W10:X10"/>
-    <mergeCell ref="Y10:Z10"/>
-    <mergeCell ref="A15:B15"/>
-    <mergeCell ref="F15:J15"/>
-    <mergeCell ref="A16:C16"/>
-    <mergeCell ref="D16:E16"/>
-    <mergeCell ref="A17:C17"/>
-    <mergeCell ref="D17:E17"/>
-    <mergeCell ref="A18:C18"/>
-    <mergeCell ref="D18:E18"/>
-    <mergeCell ref="A19:C19"/>
-    <mergeCell ref="D19:E19"/>
-    <mergeCell ref="A20:C20"/>
-    <mergeCell ref="D20:E20"/>
-    <mergeCell ref="A21:C21"/>
-    <mergeCell ref="D21:E21"/>
-    <mergeCell ref="A22:C22"/>
-    <mergeCell ref="D22:E22"/>
-    <mergeCell ref="A23:C23"/>
-    <mergeCell ref="D23:E23"/>
-    <mergeCell ref="A24:C24"/>
-    <mergeCell ref="D24:E24"/>
-    <mergeCell ref="A25:C25"/>
-    <mergeCell ref="D25:E25"/>
-    <mergeCell ref="A26:C26"/>
-    <mergeCell ref="D26:E26"/>
-    <mergeCell ref="A27:C27"/>
-    <mergeCell ref="D27:E27"/>
-    <mergeCell ref="A28:C28"/>
-    <mergeCell ref="D28:E28"/>
-    <mergeCell ref="A29:C29"/>
-    <mergeCell ref="D29:J29"/>
-    <mergeCell ref="A30:C30"/>
-    <mergeCell ref="E30:J30"/>
-    <mergeCell ref="A36:B36"/>
-    <mergeCell ref="F36:J36"/>
-    <mergeCell ref="A37:C37"/>
-    <mergeCell ref="D37:E37"/>
-    <mergeCell ref="A38:C38"/>
-    <mergeCell ref="D38:E38"/>
-    <mergeCell ref="A39:C39"/>
-    <mergeCell ref="D39:E39"/>
-    <mergeCell ref="A40:C40"/>
-    <mergeCell ref="D40:E40"/>
-    <mergeCell ref="A41:C41"/>
-    <mergeCell ref="D41:E41"/>
-    <mergeCell ref="A42:C42"/>
-    <mergeCell ref="D42:E42"/>
-    <mergeCell ref="A43:C43"/>
-    <mergeCell ref="D43:E43"/>
-    <mergeCell ref="A44:C44"/>
-    <mergeCell ref="D44:E44"/>
-    <mergeCell ref="A45:C45"/>
-    <mergeCell ref="D45:E45"/>
-    <mergeCell ref="A46:C46"/>
-    <mergeCell ref="D46:E46"/>
-    <mergeCell ref="A47:C47"/>
-    <mergeCell ref="D47:E47"/>
-    <mergeCell ref="A48:C48"/>
-    <mergeCell ref="D48:E48"/>
-    <mergeCell ref="A49:C49"/>
-    <mergeCell ref="D49:E49"/>
-    <mergeCell ref="B50:D50"/>
     <mergeCell ref="U52:W52"/>
     <mergeCell ref="X52:Y52"/>
     <mergeCell ref="B53:D53"/>
@@ -4369,6 +4392,93 @@
     <mergeCell ref="L52:O52"/>
     <mergeCell ref="P52:R52"/>
     <mergeCell ref="S52:T52"/>
+    <mergeCell ref="A46:C46"/>
+    <mergeCell ref="D46:E46"/>
+    <mergeCell ref="A47:C47"/>
+    <mergeCell ref="D47:E47"/>
+    <mergeCell ref="A48:C48"/>
+    <mergeCell ref="D48:E48"/>
+    <mergeCell ref="A49:C49"/>
+    <mergeCell ref="D49:E49"/>
+    <mergeCell ref="B50:D50"/>
+    <mergeCell ref="A41:C41"/>
+    <mergeCell ref="D41:E41"/>
+    <mergeCell ref="A42:C42"/>
+    <mergeCell ref="D42:E42"/>
+    <mergeCell ref="A43:C43"/>
+    <mergeCell ref="D43:E43"/>
+    <mergeCell ref="A44:C44"/>
+    <mergeCell ref="D44:E44"/>
+    <mergeCell ref="A45:C45"/>
+    <mergeCell ref="D45:E45"/>
+    <mergeCell ref="A36:B36"/>
+    <mergeCell ref="F36:J36"/>
+    <mergeCell ref="A37:C37"/>
+    <mergeCell ref="D37:E37"/>
+    <mergeCell ref="A38:C38"/>
+    <mergeCell ref="D38:E38"/>
+    <mergeCell ref="A39:C39"/>
+    <mergeCell ref="D39:E39"/>
+    <mergeCell ref="A40:C40"/>
+    <mergeCell ref="D40:E40"/>
+    <mergeCell ref="A26:C26"/>
+    <mergeCell ref="D26:E26"/>
+    <mergeCell ref="A27:C27"/>
+    <mergeCell ref="D27:E27"/>
+    <mergeCell ref="A28:C28"/>
+    <mergeCell ref="D28:E28"/>
+    <mergeCell ref="A29:C29"/>
+    <mergeCell ref="D29:J29"/>
+    <mergeCell ref="A30:C30"/>
+    <mergeCell ref="E30:J30"/>
+    <mergeCell ref="A21:C21"/>
+    <mergeCell ref="D21:E21"/>
+    <mergeCell ref="A22:C22"/>
+    <mergeCell ref="D22:E22"/>
+    <mergeCell ref="A23:C23"/>
+    <mergeCell ref="D23:E23"/>
+    <mergeCell ref="A24:C24"/>
+    <mergeCell ref="D24:E24"/>
+    <mergeCell ref="A25:C25"/>
+    <mergeCell ref="D25:E25"/>
+    <mergeCell ref="A16:C16"/>
+    <mergeCell ref="D16:E16"/>
+    <mergeCell ref="A17:C17"/>
+    <mergeCell ref="D17:E17"/>
+    <mergeCell ref="A18:C18"/>
+    <mergeCell ref="D18:E18"/>
+    <mergeCell ref="A19:C19"/>
+    <mergeCell ref="D19:E19"/>
+    <mergeCell ref="A20:C20"/>
+    <mergeCell ref="D20:E20"/>
+    <mergeCell ref="K10:L10"/>
+    <mergeCell ref="M10:N10"/>
+    <mergeCell ref="O10:P10"/>
+    <mergeCell ref="Q10:R10"/>
+    <mergeCell ref="S10:T10"/>
+    <mergeCell ref="U10:V10"/>
+    <mergeCell ref="W10:X10"/>
+    <mergeCell ref="Y10:Z10"/>
+    <mergeCell ref="A15:B15"/>
+    <mergeCell ref="F15:J15"/>
+    <mergeCell ref="L7:O7"/>
+    <mergeCell ref="Q7:S7"/>
+    <mergeCell ref="A8:C8"/>
+    <mergeCell ref="D8:J8"/>
+    <mergeCell ref="L8:O8"/>
+    <mergeCell ref="Q8:S8"/>
+    <mergeCell ref="A9:C9"/>
+    <mergeCell ref="E9:J9"/>
+    <mergeCell ref="K9:Z9"/>
+    <mergeCell ref="K1:Y1"/>
+    <mergeCell ref="K3:Q3"/>
+    <mergeCell ref="S3:Y3"/>
+    <mergeCell ref="K4:Q4"/>
+    <mergeCell ref="S4:Y4"/>
+    <mergeCell ref="K5:Q5"/>
+    <mergeCell ref="S5:Y5"/>
+    <mergeCell ref="K6:Q6"/>
+    <mergeCell ref="S6:Y6"/>
   </mergeCells>
   <pageMargins left="0.47" right="0.36" top="0.47" bottom="0.21" header="0.2" footer="0.21"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
page breaks in the template killing excel on error
</commit_message>
<xml_diff>
--- a/data/template.xlsx
+++ b/data/template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\me\Desktop\Development\nsbl-create-spreadsheets\src\nsblextracter\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCEE5E9E-2BE8-45CC-B809-88745C590258}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F1A473E-7E28-4118-A7E1-91B32965968E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2730" yWindow="2730" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{026AB82B-103F-4DF3-A0CA-05AA2F209D25}"/>
+    <workbookView xWindow="3465" yWindow="3465" windowWidth="21600" windowHeight="11385" xr2:uid="{026AB82B-103F-4DF3-A0CA-05AA2F209D25}"/>
   </bookViews>
   <sheets>
     <sheet name="runsheet-k" sheetId="5" r:id="rId1"/>
@@ -1034,6 +1034,90 @@
     <xf numFmtId="0" fontId="14" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="14" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="15" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="31" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="29" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="30" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="29" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="28" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="27" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="26" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="35" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="34" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="33" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="32" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="6" fillId="7" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="36" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="37" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="31" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="29" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="36" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="14" fontId="11" fillId="0" borderId="27" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -1050,90 +1134,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="7" borderId="27" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="6" fillId="7" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="31" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="29" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="30" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="29" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="36" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="37" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="28" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="27" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="26" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="31" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="29" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="36" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="35" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="34" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="33" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="32" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="15" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="14" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1532,8 +1532,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06001A37-2C87-4F4D-8D59-4864FA219C19}">
   <dimension ref="A1:G20"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="33.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1790,8 +1790,9 @@
       <c r="E20" s="49"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <printOptions horizontalCentered="1"/>
+  <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1799,8 +1800,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1BC4CC0-FE9D-498F-AEB1-D5F0C0522F79}">
   <dimension ref="A1:E20"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="E16" sqref="E15:E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="33.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1919,8 +1920,12 @@
       <c r="B20" s="49"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <printOptions horizontalCentered="1"/>
+  <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
+  <pageSetup paperSize="9" fitToWidth="0" fitToHeight="0" orientation="portrait" r:id="rId1"/>
+  <colBreaks count="1" manualBreakCount="1">
+    <brk id="2" max="2" man="1"/>
+  </colBreaks>
 </worksheet>
 </file>
 
@@ -1932,7 +1937,7 @@
   <dimension ref="A1:Z61"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="AD6" sqref="AD6"/>
+      <selection activeCell="AD20" sqref="AD20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1964,23 +1969,23 @@
       <c r="H1" s="45"/>
       <c r="I1" s="45"/>
       <c r="J1" s="45"/>
-      <c r="K1" s="54" t="s">
+      <c r="K1" s="82" t="s">
         <v>72</v>
       </c>
-      <c r="L1" s="55"/>
-      <c r="M1" s="55"/>
-      <c r="N1" s="55"/>
-      <c r="O1" s="55"/>
-      <c r="P1" s="55"/>
-      <c r="Q1" s="55"/>
-      <c r="R1" s="55"/>
-      <c r="S1" s="55"/>
-      <c r="T1" s="55"/>
-      <c r="U1" s="55"/>
-      <c r="V1" s="55"/>
-      <c r="W1" s="55"/>
-      <c r="X1" s="55"/>
-      <c r="Y1" s="55"/>
+      <c r="L1" s="83"/>
+      <c r="M1" s="83"/>
+      <c r="N1" s="83"/>
+      <c r="O1" s="83"/>
+      <c r="P1" s="83"/>
+      <c r="Q1" s="83"/>
+      <c r="R1" s="83"/>
+      <c r="S1" s="83"/>
+      <c r="T1" s="83"/>
+      <c r="U1" s="83"/>
+      <c r="V1" s="83"/>
+      <c r="W1" s="83"/>
+      <c r="X1" s="83"/>
+      <c r="Y1" s="83"/>
       <c r="Z1" s="44"/>
     </row>
     <row r="2" spans="1:26" x14ac:dyDescent="0.2">
@@ -1989,24 +1994,24 @@
     </row>
     <row r="3" spans="1:26" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="43"/>
-      <c r="K3" s="56" t="s">
+      <c r="K3" s="84" t="s">
         <v>38</v>
       </c>
-      <c r="L3" s="56"/>
-      <c r="M3" s="56"/>
-      <c r="N3" s="56"/>
-      <c r="O3" s="56"/>
-      <c r="P3" s="56"/>
-      <c r="Q3" s="56"/>
-      <c r="S3" s="56" t="s">
+      <c r="L3" s="84"/>
+      <c r="M3" s="84"/>
+      <c r="N3" s="84"/>
+      <c r="O3" s="84"/>
+      <c r="P3" s="84"/>
+      <c r="Q3" s="84"/>
+      <c r="S3" s="84" t="s">
         <v>39</v>
       </c>
-      <c r="T3" s="56"/>
-      <c r="U3" s="56"/>
-      <c r="V3" s="56"/>
-      <c r="W3" s="56"/>
-      <c r="X3" s="56"/>
-      <c r="Y3" s="56"/>
+      <c r="T3" s="84"/>
+      <c r="U3" s="84"/>
+      <c r="V3" s="84"/>
+      <c r="W3" s="84"/>
+      <c r="X3" s="84"/>
+      <c r="Y3" s="84"/>
       <c r="Z3" s="42"/>
     </row>
     <row r="4" spans="1:26" ht="14.25" x14ac:dyDescent="0.2">
@@ -2020,25 +2025,25 @@
       <c r="H4" s="25"/>
       <c r="I4" s="25"/>
       <c r="J4" s="25"/>
-      <c r="K4" s="57" t="s">
+      <c r="K4" s="85" t="s">
         <v>18</v>
       </c>
-      <c r="L4" s="57"/>
-      <c r="M4" s="57"/>
-      <c r="N4" s="57"/>
-      <c r="O4" s="57"/>
-      <c r="P4" s="57"/>
-      <c r="Q4" s="57"/>
+      <c r="L4" s="85"/>
+      <c r="M4" s="85"/>
+      <c r="N4" s="85"/>
+      <c r="O4" s="85"/>
+      <c r="P4" s="85"/>
+      <c r="Q4" s="85"/>
       <c r="R4" s="26"/>
-      <c r="S4" s="57" t="s">
+      <c r="S4" s="85" t="s">
         <v>17</v>
       </c>
-      <c r="T4" s="57"/>
-      <c r="U4" s="57"/>
-      <c r="V4" s="57"/>
-      <c r="W4" s="57"/>
-      <c r="X4" s="57"/>
-      <c r="Y4" s="57"/>
+      <c r="T4" s="85"/>
+      <c r="U4" s="85"/>
+      <c r="V4" s="85"/>
+      <c r="W4" s="85"/>
+      <c r="X4" s="85"/>
+      <c r="Y4" s="85"/>
       <c r="Z4" s="40"/>
     </row>
     <row r="5" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
@@ -2052,25 +2057,25 @@
       <c r="H5" s="25"/>
       <c r="I5" s="25"/>
       <c r="J5" s="25"/>
-      <c r="K5" s="58" t="s">
+      <c r="K5" s="86" t="s">
         <v>44</v>
       </c>
-      <c r="L5" s="58"/>
-      <c r="M5" s="58"/>
-      <c r="N5" s="58"/>
-      <c r="O5" s="58"/>
-      <c r="P5" s="58"/>
-      <c r="Q5" s="58"/>
+      <c r="L5" s="86"/>
+      <c r="M5" s="86"/>
+      <c r="N5" s="86"/>
+      <c r="O5" s="86"/>
+      <c r="P5" s="86"/>
+      <c r="Q5" s="86"/>
       <c r="R5" s="26"/>
-      <c r="S5" s="58" t="s">
+      <c r="S5" s="86" t="s">
         <v>37</v>
       </c>
-      <c r="T5" s="58"/>
-      <c r="U5" s="58"/>
-      <c r="V5" s="58"/>
-      <c r="W5" s="58"/>
-      <c r="X5" s="58"/>
-      <c r="Y5" s="58"/>
+      <c r="T5" s="86"/>
+      <c r="U5" s="86"/>
+      <c r="V5" s="86"/>
+      <c r="W5" s="86"/>
+      <c r="X5" s="86"/>
+      <c r="Y5" s="86"/>
       <c r="Z5" s="40"/>
     </row>
     <row r="6" spans="1:26" x14ac:dyDescent="0.2">
@@ -2084,25 +2089,25 @@
       <c r="H6" s="25"/>
       <c r="I6" s="25"/>
       <c r="J6" s="25"/>
-      <c r="K6" s="59" t="s">
+      <c r="K6" s="87" t="s">
         <v>36</v>
       </c>
-      <c r="L6" s="59"/>
-      <c r="M6" s="59"/>
-      <c r="N6" s="59"/>
-      <c r="O6" s="59"/>
-      <c r="P6" s="59"/>
-      <c r="Q6" s="59"/>
+      <c r="L6" s="87"/>
+      <c r="M6" s="87"/>
+      <c r="N6" s="87"/>
+      <c r="O6" s="87"/>
+      <c r="P6" s="87"/>
+      <c r="Q6" s="87"/>
       <c r="R6" s="26"/>
-      <c r="S6" s="59" t="s">
+      <c r="S6" s="87" t="s">
         <v>35</v>
       </c>
-      <c r="T6" s="59"/>
-      <c r="U6" s="59"/>
-      <c r="V6" s="59"/>
-      <c r="W6" s="59"/>
-      <c r="X6" s="59"/>
-      <c r="Y6" s="59"/>
+      <c r="T6" s="87"/>
+      <c r="U6" s="87"/>
+      <c r="V6" s="87"/>
+      <c r="W6" s="87"/>
+      <c r="X6" s="87"/>
+      <c r="Y6" s="87"/>
       <c r="Z6" s="40"/>
     </row>
     <row r="7" spans="1:26" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
@@ -2117,18 +2122,18 @@
       <c r="I7" s="25"/>
       <c r="J7" s="25"/>
       <c r="K7" s="26"/>
-      <c r="L7" s="60" t="s">
+      <c r="L7" s="76" t="s">
         <v>45</v>
       </c>
-      <c r="M7" s="61"/>
-      <c r="N7" s="61"/>
-      <c r="O7" s="62"/>
+      <c r="M7" s="57"/>
+      <c r="N7" s="57"/>
+      <c r="O7" s="58"/>
       <c r="P7" s="26"/>
-      <c r="Q7" s="63" t="s">
+      <c r="Q7" s="59" t="s">
         <v>34</v>
       </c>
-      <c r="R7" s="61"/>
-      <c r="S7" s="62"/>
+      <c r="R7" s="57"/>
+      <c r="S7" s="58"/>
       <c r="T7" s="26"/>
       <c r="U7" s="26"/>
       <c r="V7" s="26"/>
@@ -2151,20 +2156,20 @@
       <c r="G8" s="67"/>
       <c r="H8" s="67"/>
       <c r="I8" s="67"/>
-      <c r="J8" s="68"/>
+      <c r="J8" s="77"/>
       <c r="K8" s="26"/>
-      <c r="L8" s="69" t="s">
+      <c r="L8" s="78" t="s">
         <v>32</v>
       </c>
-      <c r="M8" s="69"/>
-      <c r="N8" s="69"/>
-      <c r="O8" s="69"/>
+      <c r="M8" s="78"/>
+      <c r="N8" s="78"/>
+      <c r="O8" s="78"/>
       <c r="P8" s="26"/>
-      <c r="Q8" s="69" t="s">
+      <c r="Q8" s="78" t="s">
         <v>31</v>
       </c>
-      <c r="R8" s="69"/>
-      <c r="S8" s="69"/>
+      <c r="R8" s="78"/>
+      <c r="S8" s="78"/>
       <c r="T8" s="26"/>
       <c r="U8" s="41"/>
       <c r="V8" s="26"/>
@@ -2174,38 +2179,38 @@
       <c r="Z8" s="40"/>
     </row>
     <row r="9" spans="1:26" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="70" t="s">
+      <c r="A9" s="68" t="s">
         <v>28</v>
       </c>
-      <c r="B9" s="71"/>
-      <c r="C9" s="71"/>
+      <c r="B9" s="69"/>
+      <c r="C9" s="69"/>
       <c r="D9" s="25"/>
-      <c r="E9" s="72" t="s">
+      <c r="E9" s="70" t="s">
         <v>27</v>
       </c>
-      <c r="F9" s="72"/>
-      <c r="G9" s="72"/>
-      <c r="H9" s="72"/>
-      <c r="I9" s="72"/>
-      <c r="J9" s="73"/>
-      <c r="K9" s="74" t="s">
+      <c r="F9" s="70"/>
+      <c r="G9" s="70"/>
+      <c r="H9" s="70"/>
+      <c r="I9" s="70"/>
+      <c r="J9" s="71"/>
+      <c r="K9" s="79" t="s">
         <v>30</v>
       </c>
-      <c r="L9" s="75"/>
-      <c r="M9" s="75"/>
-      <c r="N9" s="75"/>
-      <c r="O9" s="75"/>
-      <c r="P9" s="75"/>
-      <c r="Q9" s="75"/>
-      <c r="R9" s="75"/>
-      <c r="S9" s="75"/>
-      <c r="T9" s="75"/>
-      <c r="U9" s="75"/>
-      <c r="V9" s="75"/>
-      <c r="W9" s="75"/>
-      <c r="X9" s="75"/>
-      <c r="Y9" s="75"/>
-      <c r="Z9" s="76"/>
+      <c r="L9" s="80"/>
+      <c r="M9" s="80"/>
+      <c r="N9" s="80"/>
+      <c r="O9" s="80"/>
+      <c r="P9" s="80"/>
+      <c r="Q9" s="80"/>
+      <c r="R9" s="80"/>
+      <c r="S9" s="80"/>
+      <c r="T9" s="80"/>
+      <c r="U9" s="80"/>
+      <c r="V9" s="80"/>
+      <c r="W9" s="80"/>
+      <c r="X9" s="80"/>
+      <c r="Y9" s="80"/>
+      <c r="Z9" s="81"/>
     </row>
     <row r="10" spans="1:26" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" s="27"/>
@@ -2228,38 +2233,38 @@
         <v>4</v>
       </c>
       <c r="J10" s="25"/>
-      <c r="K10" s="77" t="s">
+      <c r="K10" s="72" t="s">
         <v>15</v>
       </c>
-      <c r="L10" s="78"/>
-      <c r="M10" s="78" t="s">
+      <c r="L10" s="73"/>
+      <c r="M10" s="73" t="s">
         <v>14</v>
       </c>
-      <c r="N10" s="79"/>
-      <c r="O10" s="77" t="s">
+      <c r="N10" s="74"/>
+      <c r="O10" s="72" t="s">
         <v>15</v>
       </c>
-      <c r="P10" s="78"/>
-      <c r="Q10" s="78" t="s">
+      <c r="P10" s="73"/>
+      <c r="Q10" s="73" t="s">
         <v>14</v>
       </c>
-      <c r="R10" s="79"/>
-      <c r="S10" s="77" t="s">
+      <c r="R10" s="74"/>
+      <c r="S10" s="72" t="s">
         <v>15</v>
       </c>
-      <c r="T10" s="78"/>
-      <c r="U10" s="78" t="s">
+      <c r="T10" s="73"/>
+      <c r="U10" s="73" t="s">
         <v>14</v>
       </c>
-      <c r="V10" s="79"/>
-      <c r="W10" s="77" t="s">
+      <c r="V10" s="74"/>
+      <c r="W10" s="72" t="s">
         <v>15</v>
       </c>
-      <c r="X10" s="78"/>
-      <c r="Y10" s="78" t="s">
+      <c r="X10" s="73"/>
+      <c r="Y10" s="73" t="s">
         <v>14</v>
       </c>
-      <c r="Z10" s="79"/>
+      <c r="Z10" s="74"/>
     </row>
     <row r="11" spans="1:26" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A11" s="27"/>
@@ -2466,18 +2471,18 @@
       <c r="Z14" s="18"/>
     </row>
     <row r="15" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A15" s="80"/>
-      <c r="B15" s="81"/>
+      <c r="A15" s="56"/>
+      <c r="B15" s="75"/>
       <c r="C15" s="26"/>
       <c r="D15" s="25"/>
       <c r="E15" s="25"/>
-      <c r="F15" s="63" t="s">
+      <c r="F15" s="59" t="s">
         <v>25</v>
       </c>
-      <c r="G15" s="61"/>
-      <c r="H15" s="61"/>
-      <c r="I15" s="61"/>
-      <c r="J15" s="61"/>
+      <c r="G15" s="57"/>
+      <c r="H15" s="57"/>
+      <c r="I15" s="57"/>
+      <c r="J15" s="57"/>
       <c r="K15" s="19"/>
       <c r="L15" s="10">
         <v>5</v>
@@ -2512,15 +2517,15 @@
       <c r="Z15" s="18"/>
     </row>
     <row r="16" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A16" s="63" t="s">
+      <c r="A16" s="59" t="s">
         <v>24</v>
       </c>
-      <c r="B16" s="61"/>
-      <c r="C16" s="62"/>
-      <c r="D16" s="82" t="s">
+      <c r="B16" s="57"/>
+      <c r="C16" s="58"/>
+      <c r="D16" s="62" t="s">
         <v>23</v>
       </c>
-      <c r="E16" s="83"/>
+      <c r="E16" s="63"/>
       <c r="F16" s="24">
         <v>1</v>
       </c>
@@ -2570,15 +2575,15 @@
       <c r="Z16" s="18"/>
     </row>
     <row r="17" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A17" s="80" t="s">
+      <c r="A17" s="56" t="s">
         <v>41</v>
       </c>
-      <c r="B17" s="61"/>
-      <c r="C17" s="62"/>
-      <c r="D17" s="63" t="s">
+      <c r="B17" s="57"/>
+      <c r="C17" s="58"/>
+      <c r="D17" s="59" t="s">
         <v>40</v>
       </c>
-      <c r="E17" s="62"/>
+      <c r="E17" s="58"/>
       <c r="F17" s="21"/>
       <c r="G17" s="11"/>
       <c r="H17" s="11"/>
@@ -2618,11 +2623,11 @@
       <c r="Z17" s="18"/>
     </row>
     <row r="18" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A18" s="80"/>
-      <c r="B18" s="61"/>
-      <c r="C18" s="62"/>
-      <c r="D18" s="63"/>
-      <c r="E18" s="62"/>
+      <c r="A18" s="56"/>
+      <c r="B18" s="57"/>
+      <c r="C18" s="58"/>
+      <c r="D18" s="59"/>
+      <c r="E18" s="58"/>
       <c r="F18" s="21"/>
       <c r="G18" s="11"/>
       <c r="H18" s="11"/>
@@ -2662,11 +2667,11 @@
       <c r="Z18" s="18"/>
     </row>
     <row r="19" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A19" s="80"/>
-      <c r="B19" s="61"/>
-      <c r="C19" s="62"/>
-      <c r="D19" s="63"/>
-      <c r="E19" s="62"/>
+      <c r="A19" s="56"/>
+      <c r="B19" s="57"/>
+      <c r="C19" s="58"/>
+      <c r="D19" s="59"/>
+      <c r="E19" s="58"/>
       <c r="F19" s="21"/>
       <c r="G19" s="11"/>
       <c r="H19" s="11"/>
@@ -2706,11 +2711,11 @@
       <c r="Z19" s="18"/>
     </row>
     <row r="20" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A20" s="80"/>
-      <c r="B20" s="61"/>
-      <c r="C20" s="62"/>
-      <c r="D20" s="63"/>
-      <c r="E20" s="62"/>
+      <c r="A20" s="56"/>
+      <c r="B20" s="57"/>
+      <c r="C20" s="58"/>
+      <c r="D20" s="59"/>
+      <c r="E20" s="58"/>
       <c r="F20" s="21"/>
       <c r="G20" s="11"/>
       <c r="H20" s="11"/>
@@ -2750,11 +2755,11 @@
       <c r="Z20" s="18"/>
     </row>
     <row r="21" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A21" s="80"/>
-      <c r="B21" s="61"/>
-      <c r="C21" s="62"/>
-      <c r="D21" s="63"/>
-      <c r="E21" s="62"/>
+      <c r="A21" s="56"/>
+      <c r="B21" s="57"/>
+      <c r="C21" s="58"/>
+      <c r="D21" s="59"/>
+      <c r="E21" s="58"/>
       <c r="F21" s="21"/>
       <c r="G21" s="11"/>
       <c r="H21" s="11"/>
@@ -2794,11 +2799,11 @@
       <c r="Z21" s="18"/>
     </row>
     <row r="22" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A22" s="80"/>
-      <c r="B22" s="61"/>
-      <c r="C22" s="62"/>
-      <c r="D22" s="63"/>
-      <c r="E22" s="62"/>
+      <c r="A22" s="56"/>
+      <c r="B22" s="57"/>
+      <c r="C22" s="58"/>
+      <c r="D22" s="59"/>
+      <c r="E22" s="58"/>
       <c r="F22" s="21"/>
       <c r="G22" s="11"/>
       <c r="H22" s="11"/>
@@ -2838,11 +2843,11 @@
       <c r="Z22" s="18"/>
     </row>
     <row r="23" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A23" s="80"/>
-      <c r="B23" s="61"/>
-      <c r="C23" s="62"/>
-      <c r="D23" s="63"/>
-      <c r="E23" s="62"/>
+      <c r="A23" s="56"/>
+      <c r="B23" s="57"/>
+      <c r="C23" s="58"/>
+      <c r="D23" s="59"/>
+      <c r="E23" s="58"/>
       <c r="F23" s="21"/>
       <c r="G23" s="11"/>
       <c r="H23" s="11"/>
@@ -2882,11 +2887,11 @@
       <c r="Z23" s="18"/>
     </row>
     <row r="24" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A24" s="80"/>
-      <c r="B24" s="61"/>
-      <c r="C24" s="62"/>
-      <c r="D24" s="63"/>
-      <c r="E24" s="62"/>
+      <c r="A24" s="56"/>
+      <c r="B24" s="57"/>
+      <c r="C24" s="58"/>
+      <c r="D24" s="59"/>
+      <c r="E24" s="58"/>
       <c r="F24" s="21"/>
       <c r="G24" s="11"/>
       <c r="H24" s="11"/>
@@ -2926,11 +2931,11 @@
       <c r="Z24" s="18"/>
     </row>
     <row r="25" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A25" s="80"/>
-      <c r="B25" s="61"/>
-      <c r="C25" s="62"/>
-      <c r="D25" s="63"/>
-      <c r="E25" s="62"/>
+      <c r="A25" s="56"/>
+      <c r="B25" s="57"/>
+      <c r="C25" s="58"/>
+      <c r="D25" s="59"/>
+      <c r="E25" s="58"/>
       <c r="F25" s="21"/>
       <c r="G25" s="11"/>
       <c r="H25" s="11"/>
@@ -2970,11 +2975,11 @@
       <c r="Z25" s="18"/>
     </row>
     <row r="26" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A26" s="80"/>
-      <c r="B26" s="61"/>
-      <c r="C26" s="62"/>
-      <c r="D26" s="63"/>
-      <c r="E26" s="62"/>
+      <c r="A26" s="56"/>
+      <c r="B26" s="57"/>
+      <c r="C26" s="58"/>
+      <c r="D26" s="59"/>
+      <c r="E26" s="58"/>
       <c r="F26" s="21"/>
       <c r="G26" s="11"/>
       <c r="H26" s="11"/>
@@ -3014,11 +3019,11 @@
       <c r="Z26" s="18"/>
     </row>
     <row r="27" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A27" s="80"/>
-      <c r="B27" s="61"/>
-      <c r="C27" s="62"/>
-      <c r="D27" s="63"/>
-      <c r="E27" s="62"/>
+      <c r="A27" s="56"/>
+      <c r="B27" s="57"/>
+      <c r="C27" s="58"/>
+      <c r="D27" s="59"/>
+      <c r="E27" s="58"/>
       <c r="F27" s="21"/>
       <c r="G27" s="11"/>
       <c r="H27" s="11"/>
@@ -3058,11 +3063,11 @@
       <c r="Z27" s="18"/>
     </row>
     <row r="28" spans="1:26" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="80"/>
-      <c r="B28" s="61"/>
-      <c r="C28" s="62"/>
-      <c r="D28" s="63"/>
-      <c r="E28" s="62"/>
+      <c r="A28" s="56"/>
+      <c r="B28" s="57"/>
+      <c r="C28" s="58"/>
+      <c r="D28" s="59"/>
+      <c r="E28" s="58"/>
       <c r="F28" s="21"/>
       <c r="G28" s="11"/>
       <c r="H28" s="11"/>
@@ -3150,20 +3155,20 @@
       <c r="Z29" s="18"/>
     </row>
     <row r="30" spans="1:26" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="70" t="s">
+      <c r="A30" s="68" t="s">
         <v>28</v>
       </c>
-      <c r="B30" s="71"/>
-      <c r="C30" s="71"/>
+      <c r="B30" s="69"/>
+      <c r="C30" s="69"/>
       <c r="D30" s="25"/>
-      <c r="E30" s="72" t="s">
+      <c r="E30" s="70" t="s">
         <v>27</v>
       </c>
-      <c r="F30" s="72"/>
-      <c r="G30" s="72"/>
-      <c r="H30" s="72"/>
-      <c r="I30" s="72"/>
-      <c r="J30" s="73"/>
+      <c r="F30" s="70"/>
+      <c r="G30" s="70"/>
+      <c r="H30" s="70"/>
+      <c r="I30" s="70"/>
+      <c r="J30" s="71"/>
       <c r="K30" s="19"/>
       <c r="L30" s="10">
         <v>20</v>
@@ -3456,18 +3461,18 @@
       <c r="Z35" s="18"/>
     </row>
     <row r="36" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A36" s="80"/>
-      <c r="B36" s="84"/>
+      <c r="A36" s="56"/>
+      <c r="B36" s="61"/>
       <c r="C36" s="26"/>
       <c r="D36" s="25"/>
       <c r="E36" s="25"/>
-      <c r="F36" s="63" t="s">
+      <c r="F36" s="59" t="s">
         <v>25</v>
       </c>
-      <c r="G36" s="61"/>
-      <c r="H36" s="61"/>
-      <c r="I36" s="61"/>
-      <c r="J36" s="61"/>
+      <c r="G36" s="57"/>
+      <c r="H36" s="57"/>
+      <c r="I36" s="57"/>
+      <c r="J36" s="57"/>
       <c r="K36" s="19"/>
       <c r="L36" s="10">
         <v>26</v>
@@ -3502,15 +3507,15 @@
       <c r="Z36" s="18"/>
     </row>
     <row r="37" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A37" s="63" t="s">
+      <c r="A37" s="59" t="s">
         <v>24</v>
       </c>
-      <c r="B37" s="61"/>
-      <c r="C37" s="62"/>
-      <c r="D37" s="82" t="s">
+      <c r="B37" s="57"/>
+      <c r="C37" s="58"/>
+      <c r="D37" s="62" t="s">
         <v>23</v>
       </c>
-      <c r="E37" s="83"/>
+      <c r="E37" s="63"/>
       <c r="F37" s="24">
         <v>1</v>
       </c>
@@ -3560,15 +3565,15 @@
       <c r="Z37" s="18"/>
     </row>
     <row r="38" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A38" s="80" t="s">
+      <c r="A38" s="56" t="s">
         <v>42</v>
       </c>
-      <c r="B38" s="61"/>
-      <c r="C38" s="62"/>
-      <c r="D38" s="63" t="s">
+      <c r="B38" s="57"/>
+      <c r="C38" s="58"/>
+      <c r="D38" s="59" t="s">
         <v>43</v>
       </c>
-      <c r="E38" s="62"/>
+      <c r="E38" s="58"/>
       <c r="F38" s="21"/>
       <c r="G38" s="11"/>
       <c r="H38" s="11"/>
@@ -3608,11 +3613,11 @@
       <c r="Z38" s="18"/>
     </row>
     <row r="39" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A39" s="80"/>
-      <c r="B39" s="61"/>
-      <c r="C39" s="62"/>
-      <c r="D39" s="63"/>
-      <c r="E39" s="62"/>
+      <c r="A39" s="56"/>
+      <c r="B39" s="57"/>
+      <c r="C39" s="58"/>
+      <c r="D39" s="59"/>
+      <c r="E39" s="58"/>
       <c r="F39" s="21"/>
       <c r="G39" s="11"/>
       <c r="H39" s="11"/>
@@ -3652,11 +3657,11 @@
       <c r="Z39" s="18"/>
     </row>
     <row r="40" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A40" s="80"/>
-      <c r="B40" s="61"/>
-      <c r="C40" s="62"/>
-      <c r="D40" s="63"/>
-      <c r="E40" s="62"/>
+      <c r="A40" s="56"/>
+      <c r="B40" s="57"/>
+      <c r="C40" s="58"/>
+      <c r="D40" s="59"/>
+      <c r="E40" s="58"/>
       <c r="F40" s="21"/>
       <c r="G40" s="11"/>
       <c r="H40" s="11"/>
@@ -3696,11 +3701,11 @@
       <c r="Z40" s="18"/>
     </row>
     <row r="41" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A41" s="80"/>
-      <c r="B41" s="61"/>
-      <c r="C41" s="62"/>
-      <c r="D41" s="63"/>
-      <c r="E41" s="62"/>
+      <c r="A41" s="56"/>
+      <c r="B41" s="57"/>
+      <c r="C41" s="58"/>
+      <c r="D41" s="59"/>
+      <c r="E41" s="58"/>
       <c r="F41" s="21"/>
       <c r="G41" s="11"/>
       <c r="H41" s="11"/>
@@ -3740,11 +3745,11 @@
       <c r="Z41" s="18"/>
     </row>
     <row r="42" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A42" s="80"/>
-      <c r="B42" s="61"/>
-      <c r="C42" s="62"/>
-      <c r="D42" s="63"/>
-      <c r="E42" s="62"/>
+      <c r="A42" s="56"/>
+      <c r="B42" s="57"/>
+      <c r="C42" s="58"/>
+      <c r="D42" s="59"/>
+      <c r="E42" s="58"/>
       <c r="F42" s="21"/>
       <c r="G42" s="11"/>
       <c r="H42" s="11"/>
@@ -3784,11 +3789,11 @@
       <c r="Z42" s="18"/>
     </row>
     <row r="43" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A43" s="80"/>
-      <c r="B43" s="61"/>
-      <c r="C43" s="62"/>
-      <c r="D43" s="63"/>
-      <c r="E43" s="62"/>
+      <c r="A43" s="56"/>
+      <c r="B43" s="57"/>
+      <c r="C43" s="58"/>
+      <c r="D43" s="59"/>
+      <c r="E43" s="58"/>
       <c r="F43" s="21"/>
       <c r="G43" s="11"/>
       <c r="H43" s="11"/>
@@ -3828,11 +3833,11 @@
       <c r="Z43" s="18"/>
     </row>
     <row r="44" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A44" s="80"/>
-      <c r="B44" s="61"/>
-      <c r="C44" s="62"/>
-      <c r="D44" s="63"/>
-      <c r="E44" s="62"/>
+      <c r="A44" s="56"/>
+      <c r="B44" s="57"/>
+      <c r="C44" s="58"/>
+      <c r="D44" s="59"/>
+      <c r="E44" s="58"/>
       <c r="F44" s="21"/>
       <c r="G44" s="11"/>
       <c r="H44" s="11"/>
@@ -3872,11 +3877,11 @@
       <c r="Z44" s="18"/>
     </row>
     <row r="45" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A45" s="80"/>
-      <c r="B45" s="61"/>
-      <c r="C45" s="62"/>
-      <c r="D45" s="63"/>
-      <c r="E45" s="62"/>
+      <c r="A45" s="56"/>
+      <c r="B45" s="57"/>
+      <c r="C45" s="58"/>
+      <c r="D45" s="59"/>
+      <c r="E45" s="58"/>
       <c r="F45" s="21"/>
       <c r="G45" s="11"/>
       <c r="H45" s="11"/>
@@ -3916,11 +3921,11 @@
       <c r="Z45" s="18"/>
     </row>
     <row r="46" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A46" s="80"/>
-      <c r="B46" s="61"/>
-      <c r="C46" s="62"/>
-      <c r="D46" s="63"/>
-      <c r="E46" s="62"/>
+      <c r="A46" s="56"/>
+      <c r="B46" s="57"/>
+      <c r="C46" s="58"/>
+      <c r="D46" s="59"/>
+      <c r="E46" s="58"/>
       <c r="F46" s="21"/>
       <c r="G46" s="11"/>
       <c r="H46" s="11"/>
@@ -3960,11 +3965,11 @@
       <c r="Z46" s="18"/>
     </row>
     <row r="47" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A47" s="80"/>
-      <c r="B47" s="61"/>
-      <c r="C47" s="62"/>
-      <c r="D47" s="63"/>
-      <c r="E47" s="62"/>
+      <c r="A47" s="56"/>
+      <c r="B47" s="57"/>
+      <c r="C47" s="58"/>
+      <c r="D47" s="59"/>
+      <c r="E47" s="58"/>
       <c r="F47" s="21"/>
       <c r="G47" s="11"/>
       <c r="H47" s="11"/>
@@ -4004,11 +4009,11 @@
       <c r="Z47" s="18"/>
     </row>
     <row r="48" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A48" s="80"/>
-      <c r="B48" s="61"/>
-      <c r="C48" s="62"/>
-      <c r="D48" s="63"/>
-      <c r="E48" s="62"/>
+      <c r="A48" s="56"/>
+      <c r="B48" s="57"/>
+      <c r="C48" s="58"/>
+      <c r="D48" s="59"/>
+      <c r="E48" s="58"/>
       <c r="F48" s="21"/>
       <c r="G48" s="11"/>
       <c r="H48" s="11"/>
@@ -4048,11 +4053,11 @@
       <c r="Z48" s="18"/>
     </row>
     <row r="49" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A49" s="80"/>
-      <c r="B49" s="61"/>
-      <c r="C49" s="62"/>
-      <c r="D49" s="63"/>
-      <c r="E49" s="62"/>
+      <c r="A49" s="56"/>
+      <c r="B49" s="57"/>
+      <c r="C49" s="58"/>
+      <c r="D49" s="59"/>
+      <c r="E49" s="58"/>
       <c r="F49" s="21"/>
       <c r="G49" s="11"/>
       <c r="H49" s="11"/>
@@ -4093,11 +4098,11 @@
     </row>
     <row r="50" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A50" s="17"/>
-      <c r="B50" s="85" t="s">
+      <c r="B50" s="60" t="s">
         <v>22</v>
       </c>
-      <c r="C50" s="85"/>
-      <c r="D50" s="85"/>
+      <c r="C50" s="60"/>
+      <c r="D50" s="60"/>
       <c r="E50" s="17"/>
       <c r="F50" s="17"/>
       <c r="G50" s="17"/>
@@ -4139,21 +4144,21 @@
     </row>
     <row r="51" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A51" s="12"/>
-      <c r="B51" s="86" t="s">
+      <c r="B51" s="54" t="s">
         <v>21</v>
       </c>
-      <c r="C51" s="86"/>
-      <c r="D51" s="86"/>
+      <c r="C51" s="54"/>
+      <c r="D51" s="54"/>
       <c r="E51" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="F51" s="86"/>
-      <c r="G51" s="86"/>
+      <c r="F51" s="54"/>
+      <c r="G51" s="54"/>
       <c r="H51" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="I51" s="86"/>
-      <c r="J51" s="86"/>
+      <c r="I51" s="54"/>
+      <c r="J51" s="54"/>
       <c r="K51" s="10"/>
       <c r="L51" s="10"/>
       <c r="M51" s="10"/>
@@ -4173,78 +4178,78 @@
     </row>
     <row r="52" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A52" s="11"/>
-      <c r="B52" s="86" t="s">
+      <c r="B52" s="54" t="s">
         <v>20</v>
       </c>
-      <c r="C52" s="86"/>
-      <c r="D52" s="86"/>
+      <c r="C52" s="54"/>
+      <c r="D52" s="54"/>
       <c r="E52" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="F52" s="86"/>
-      <c r="G52" s="86"/>
+      <c r="F52" s="54"/>
+      <c r="G52" s="54"/>
       <c r="H52" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="I52" s="86"/>
-      <c r="J52" s="86"/>
+      <c r="I52" s="54"/>
+      <c r="J52" s="54"/>
       <c r="K52" s="10"/>
-      <c r="L52" s="87" t="s">
+      <c r="L52" s="55" t="s">
         <v>19</v>
       </c>
-      <c r="M52" s="87"/>
-      <c r="N52" s="87"/>
-      <c r="O52" s="87"/>
-      <c r="P52" s="86" t="s">
+      <c r="M52" s="55"/>
+      <c r="N52" s="55"/>
+      <c r="O52" s="55"/>
+      <c r="P52" s="54" t="s">
         <v>18</v>
       </c>
-      <c r="Q52" s="86"/>
-      <c r="R52" s="86"/>
-      <c r="S52" s="86"/>
-      <c r="T52" s="86"/>
-      <c r="U52" s="86" t="s">
+      <c r="Q52" s="54"/>
+      <c r="R52" s="54"/>
+      <c r="S52" s="54"/>
+      <c r="T52" s="54"/>
+      <c r="U52" s="54" t="s">
         <v>17</v>
       </c>
-      <c r="V52" s="86"/>
-      <c r="W52" s="86"/>
-      <c r="X52" s="86"/>
-      <c r="Y52" s="86"/>
+      <c r="V52" s="54"/>
+      <c r="W52" s="54"/>
+      <c r="X52" s="54"/>
+      <c r="Y52" s="54"/>
       <c r="Z52" s="10"/>
     </row>
     <row r="53" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A53" s="11"/>
-      <c r="B53" s="87" t="s">
+      <c r="B53" s="55" t="s">
         <v>16</v>
       </c>
-      <c r="C53" s="87"/>
-      <c r="D53" s="87"/>
+      <c r="C53" s="55"/>
+      <c r="D53" s="55"/>
       <c r="E53" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="F53" s="86"/>
-      <c r="G53" s="86"/>
+      <c r="F53" s="54"/>
+      <c r="G53" s="54"/>
       <c r="H53" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="I53" s="86"/>
-      <c r="J53" s="86"/>
-      <c r="K53" s="87" t="s">
+      <c r="I53" s="54"/>
+      <c r="J53" s="54"/>
+      <c r="K53" s="55" t="s">
         <v>13</v>
       </c>
-      <c r="L53" s="87"/>
-      <c r="M53" s="87"/>
-      <c r="N53" s="87"/>
-      <c r="O53" s="87"/>
-      <c r="P53" s="87"/>
-      <c r="Q53" s="87"/>
-      <c r="R53" s="86"/>
-      <c r="S53" s="86"/>
-      <c r="T53" s="86"/>
-      <c r="U53" s="86"/>
-      <c r="V53" s="86"/>
-      <c r="W53" s="86"/>
-      <c r="X53" s="86"/>
-      <c r="Y53" s="86"/>
+      <c r="L53" s="55"/>
+      <c r="M53" s="55"/>
+      <c r="N53" s="55"/>
+      <c r="O53" s="55"/>
+      <c r="P53" s="55"/>
+      <c r="Q53" s="55"/>
+      <c r="R53" s="54"/>
+      <c r="S53" s="54"/>
+      <c r="T53" s="54"/>
+      <c r="U53" s="54"/>
+      <c r="V53" s="54"/>
+      <c r="W53" s="54"/>
+      <c r="X53" s="54"/>
+      <c r="Y53" s="54"/>
       <c r="Z53" s="10"/>
     </row>
     <row r="55" spans="1:26" x14ac:dyDescent="0.2">
@@ -4376,6 +4381,93 @@
     </row>
   </sheetData>
   <mergeCells count="103">
+    <mergeCell ref="K1:Y1"/>
+    <mergeCell ref="K3:Q3"/>
+    <mergeCell ref="S3:Y3"/>
+    <mergeCell ref="K4:Q4"/>
+    <mergeCell ref="S4:Y4"/>
+    <mergeCell ref="K5:Q5"/>
+    <mergeCell ref="S5:Y5"/>
+    <mergeCell ref="K6:Q6"/>
+    <mergeCell ref="S6:Y6"/>
+    <mergeCell ref="L7:O7"/>
+    <mergeCell ref="Q7:S7"/>
+    <mergeCell ref="A8:C8"/>
+    <mergeCell ref="D8:J8"/>
+    <mergeCell ref="L8:O8"/>
+    <mergeCell ref="Q8:S8"/>
+    <mergeCell ref="A9:C9"/>
+    <mergeCell ref="E9:J9"/>
+    <mergeCell ref="K9:Z9"/>
+    <mergeCell ref="K10:L10"/>
+    <mergeCell ref="M10:N10"/>
+    <mergeCell ref="O10:P10"/>
+    <mergeCell ref="Q10:R10"/>
+    <mergeCell ref="S10:T10"/>
+    <mergeCell ref="U10:V10"/>
+    <mergeCell ref="W10:X10"/>
+    <mergeCell ref="Y10:Z10"/>
+    <mergeCell ref="A15:B15"/>
+    <mergeCell ref="F15:J15"/>
+    <mergeCell ref="A16:C16"/>
+    <mergeCell ref="D16:E16"/>
+    <mergeCell ref="A17:C17"/>
+    <mergeCell ref="D17:E17"/>
+    <mergeCell ref="A18:C18"/>
+    <mergeCell ref="D18:E18"/>
+    <mergeCell ref="A19:C19"/>
+    <mergeCell ref="D19:E19"/>
+    <mergeCell ref="A20:C20"/>
+    <mergeCell ref="D20:E20"/>
+    <mergeCell ref="A21:C21"/>
+    <mergeCell ref="D21:E21"/>
+    <mergeCell ref="A22:C22"/>
+    <mergeCell ref="D22:E22"/>
+    <mergeCell ref="A23:C23"/>
+    <mergeCell ref="D23:E23"/>
+    <mergeCell ref="A24:C24"/>
+    <mergeCell ref="D24:E24"/>
+    <mergeCell ref="A25:C25"/>
+    <mergeCell ref="D25:E25"/>
+    <mergeCell ref="A26:C26"/>
+    <mergeCell ref="D26:E26"/>
+    <mergeCell ref="A27:C27"/>
+    <mergeCell ref="D27:E27"/>
+    <mergeCell ref="A28:C28"/>
+    <mergeCell ref="D28:E28"/>
+    <mergeCell ref="A29:C29"/>
+    <mergeCell ref="D29:J29"/>
+    <mergeCell ref="A30:C30"/>
+    <mergeCell ref="E30:J30"/>
+    <mergeCell ref="A36:B36"/>
+    <mergeCell ref="F36:J36"/>
+    <mergeCell ref="A37:C37"/>
+    <mergeCell ref="D37:E37"/>
+    <mergeCell ref="A38:C38"/>
+    <mergeCell ref="D38:E38"/>
+    <mergeCell ref="A39:C39"/>
+    <mergeCell ref="D39:E39"/>
+    <mergeCell ref="A40:C40"/>
+    <mergeCell ref="D40:E40"/>
+    <mergeCell ref="A41:C41"/>
+    <mergeCell ref="D41:E41"/>
+    <mergeCell ref="A42:C42"/>
+    <mergeCell ref="D42:E42"/>
+    <mergeCell ref="A43:C43"/>
+    <mergeCell ref="D43:E43"/>
+    <mergeCell ref="A44:C44"/>
+    <mergeCell ref="D44:E44"/>
+    <mergeCell ref="A45:C45"/>
+    <mergeCell ref="D45:E45"/>
+    <mergeCell ref="A46:C46"/>
+    <mergeCell ref="D46:E46"/>
+    <mergeCell ref="A47:C47"/>
+    <mergeCell ref="D47:E47"/>
+    <mergeCell ref="A48:C48"/>
+    <mergeCell ref="D48:E48"/>
+    <mergeCell ref="A49:C49"/>
+    <mergeCell ref="D49:E49"/>
+    <mergeCell ref="B50:D50"/>
     <mergeCell ref="U52:W52"/>
     <mergeCell ref="X52:Y52"/>
     <mergeCell ref="B53:D53"/>
@@ -4392,95 +4484,9 @@
     <mergeCell ref="L52:O52"/>
     <mergeCell ref="P52:R52"/>
     <mergeCell ref="S52:T52"/>
-    <mergeCell ref="A46:C46"/>
-    <mergeCell ref="D46:E46"/>
-    <mergeCell ref="A47:C47"/>
-    <mergeCell ref="D47:E47"/>
-    <mergeCell ref="A48:C48"/>
-    <mergeCell ref="D48:E48"/>
-    <mergeCell ref="A49:C49"/>
-    <mergeCell ref="D49:E49"/>
-    <mergeCell ref="B50:D50"/>
-    <mergeCell ref="A41:C41"/>
-    <mergeCell ref="D41:E41"/>
-    <mergeCell ref="A42:C42"/>
-    <mergeCell ref="D42:E42"/>
-    <mergeCell ref="A43:C43"/>
-    <mergeCell ref="D43:E43"/>
-    <mergeCell ref="A44:C44"/>
-    <mergeCell ref="D44:E44"/>
-    <mergeCell ref="A45:C45"/>
-    <mergeCell ref="D45:E45"/>
-    <mergeCell ref="A36:B36"/>
-    <mergeCell ref="F36:J36"/>
-    <mergeCell ref="A37:C37"/>
-    <mergeCell ref="D37:E37"/>
-    <mergeCell ref="A38:C38"/>
-    <mergeCell ref="D38:E38"/>
-    <mergeCell ref="A39:C39"/>
-    <mergeCell ref="D39:E39"/>
-    <mergeCell ref="A40:C40"/>
-    <mergeCell ref="D40:E40"/>
-    <mergeCell ref="A26:C26"/>
-    <mergeCell ref="D26:E26"/>
-    <mergeCell ref="A27:C27"/>
-    <mergeCell ref="D27:E27"/>
-    <mergeCell ref="A28:C28"/>
-    <mergeCell ref="D28:E28"/>
-    <mergeCell ref="A29:C29"/>
-    <mergeCell ref="D29:J29"/>
-    <mergeCell ref="A30:C30"/>
-    <mergeCell ref="E30:J30"/>
-    <mergeCell ref="A21:C21"/>
-    <mergeCell ref="D21:E21"/>
-    <mergeCell ref="A22:C22"/>
-    <mergeCell ref="D22:E22"/>
-    <mergeCell ref="A23:C23"/>
-    <mergeCell ref="D23:E23"/>
-    <mergeCell ref="A24:C24"/>
-    <mergeCell ref="D24:E24"/>
-    <mergeCell ref="A25:C25"/>
-    <mergeCell ref="D25:E25"/>
-    <mergeCell ref="A16:C16"/>
-    <mergeCell ref="D16:E16"/>
-    <mergeCell ref="A17:C17"/>
-    <mergeCell ref="D17:E17"/>
-    <mergeCell ref="A18:C18"/>
-    <mergeCell ref="D18:E18"/>
-    <mergeCell ref="A19:C19"/>
-    <mergeCell ref="D19:E19"/>
-    <mergeCell ref="A20:C20"/>
-    <mergeCell ref="D20:E20"/>
-    <mergeCell ref="K10:L10"/>
-    <mergeCell ref="M10:N10"/>
-    <mergeCell ref="O10:P10"/>
-    <mergeCell ref="Q10:R10"/>
-    <mergeCell ref="S10:T10"/>
-    <mergeCell ref="U10:V10"/>
-    <mergeCell ref="W10:X10"/>
-    <mergeCell ref="Y10:Z10"/>
-    <mergeCell ref="A15:B15"/>
-    <mergeCell ref="F15:J15"/>
-    <mergeCell ref="L7:O7"/>
-    <mergeCell ref="Q7:S7"/>
-    <mergeCell ref="A8:C8"/>
-    <mergeCell ref="D8:J8"/>
-    <mergeCell ref="L8:O8"/>
-    <mergeCell ref="Q8:S8"/>
-    <mergeCell ref="A9:C9"/>
-    <mergeCell ref="E9:J9"/>
-    <mergeCell ref="K9:Z9"/>
-    <mergeCell ref="K1:Y1"/>
-    <mergeCell ref="K3:Q3"/>
-    <mergeCell ref="S3:Y3"/>
-    <mergeCell ref="K4:Q4"/>
-    <mergeCell ref="S4:Y4"/>
-    <mergeCell ref="K5:Q5"/>
-    <mergeCell ref="S5:Y5"/>
-    <mergeCell ref="K6:Q6"/>
-    <mergeCell ref="S6:Y6"/>
   </mergeCells>
-  <pageMargins left="0.47" right="0.36" top="0.47" bottom="0.21" header="0.2" footer="0.21"/>
+  <printOptions horizontalCentered="1" verticalCentered="1"/>
+  <pageMargins left="0.47244094488188981" right="0.35433070866141736" top="0.47244094488188981" bottom="0.19685039370078741" header="0.19685039370078741" footer="0.19685039370078741"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <headerFooter alignWithMargins="0"/>
   <drawing r:id="rId2"/>

</xml_diff>

<commit_message>
updating template and removing adults runsheet
</commit_message>
<xml_diff>
--- a/data/template.xlsx
+++ b/data/template.xlsx
@@ -1,23 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27004"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\baske\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADFA6EA3-AC68-4EA1-8CDA-E3C50F55C081}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{83CBDB96-6E83-47F4-A584-BAFA1E89E030}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{026AB82B-103F-4DF3-A0CA-05AA2F209D25}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="1" xr2:uid="{026AB82B-103F-4DF3-A0CA-05AA2F209D25}"/>
   </bookViews>
   <sheets>
     <sheet name="runsheet-k" sheetId="5" r:id="rId1"/>
-    <sheet name="runsheet-a" sheetId="11" r:id="rId2"/>
-    <sheet name="scoresheet" sheetId="10" r:id="rId3"/>
+    <sheet name="scoresheet" sheetId="10" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -29,6 +28,8 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -36,7 +37,10 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="75">
+  <si>
+    <t>Time &amp; Grade/Year</t>
+  </si>
   <si>
     <t>COURT 1</t>
   </si>
@@ -47,136 +51,19 @@
     <t>9am Years 3/4</t>
   </si>
   <si>
-    <t>10am Years 3/4</t>
+    <t>_9_c1_s_</t>
   </si>
   <si>
-    <t>12pm Years 5/6</t>
-  </si>
-  <si>
-    <t>2pm Years 7/8</t>
-  </si>
-  <si>
-    <t>4pm Years 9-12</t>
-  </si>
-  <si>
-    <t>5pm Years 9-12</t>
-  </si>
-  <si>
-    <t>6pm Years 9-12</t>
-  </si>
-  <si>
-    <t>11am Years 5/6</t>
+    <t>_9_c2_s_</t>
   </si>
   <si>
     <t>1pm Years 7/8</t>
   </si>
   <si>
-    <t>3pm Years 9-12</t>
+    <t>_1_c1_b_</t>
   </si>
   <si>
-    <t>Time &amp; Grade/Year</t>
-  </si>
-  <si>
-    <t>WINNING TEAM:</t>
-  </si>
-  <si>
-    <t>B</t>
-  </si>
-  <si>
-    <t>A</t>
-  </si>
-  <si>
-    <t>Full Time</t>
-  </si>
-  <si>
-    <t>Team B</t>
-  </si>
-  <si>
-    <t>Team A</t>
-  </si>
-  <si>
-    <t>FINAL SCORE:</t>
-  </si>
-  <si>
-    <t>Second Half</t>
-  </si>
-  <si>
-    <t>First Half</t>
-  </si>
-  <si>
-    <t>SCORES</t>
-  </si>
-  <si>
-    <t>Name of Player</t>
-  </si>
-  <si>
-    <t>No.</t>
-  </si>
-  <si>
-    <t>FOULS</t>
-  </si>
-  <si>
-    <t>Team Fouls</t>
-  </si>
-  <si>
-    <t>Time Outs</t>
-  </si>
-  <si>
-    <t>_team_black_</t>
-  </si>
-  <si>
-    <t>RUNNING SCORE</t>
-  </si>
-  <si>
-    <t>Time</t>
-  </si>
-  <si>
-    <t>Date</t>
-  </si>
-  <si>
-    <t>_team_white_</t>
-  </si>
-  <si>
-    <t>_time_</t>
-  </si>
-  <si>
-    <t>Court</t>
-  </si>
-  <si>
-    <t>Venue</t>
-  </si>
-  <si>
-    <t>_court_</t>
-  </si>
-  <si>
-    <t>_team_white_title_</t>
-  </si>
-  <si>
-    <t>_team_black_title_</t>
-  </si>
-  <si>
-    <t>_a_player_name_</t>
-  </si>
-  <si>
-    <t>_a_player_num_</t>
-  </si>
-  <si>
-    <t>_b_player_num_</t>
-  </si>
-  <si>
-    <t>_b_player_name_</t>
-  </si>
-  <si>
-    <t>_venue_</t>
-  </si>
-  <si>
-    <t>_date_</t>
-  </si>
-  <si>
-    <t>_9_c1_s_</t>
-  </si>
-  <si>
-    <t>_9_c2_s_</t>
+    <t>10am Years 3/4</t>
   </si>
   <si>
     <t>_10_c1_s_</t>
@@ -185,13 +72,25 @@
     <t>_10_c2_s_</t>
   </si>
   <si>
+    <t>2pm Years 7/8</t>
+  </si>
+  <si>
+    <t>_2_c1_b_</t>
+  </si>
+  <si>
     <t>11am Years 3/4</t>
   </si>
   <si>
     <t>_11_c1_s_</t>
   </si>
   <si>
+    <t>11am Years 5/6</t>
+  </si>
+  <si>
     <t>_11_c2_s_</t>
+  </si>
+  <si>
+    <t>12pm Years 5/6</t>
   </si>
   <si>
     <t>_12_c1_s_</t>
@@ -209,16 +108,34 @@
     <t>_1_c2_s_</t>
   </si>
   <si>
+    <t>_1_c2_b_</t>
+  </si>
+  <si>
+    <t>2pm Years 5/6</t>
+  </si>
+  <si>
     <t>_2_c1_s_</t>
   </si>
   <si>
     <t>_2_c2_s_</t>
   </si>
   <si>
+    <t>_2_c2_b_</t>
+  </si>
+  <si>
+    <t>3pm Years 7/8</t>
+  </si>
+  <si>
     <t>_3_c1_s_</t>
   </si>
   <si>
+    <t>3pm Years 9-12</t>
+  </si>
+  <si>
     <t>_3_c2_s_</t>
+  </si>
+  <si>
+    <t>4pm Years 9-12</t>
   </si>
   <si>
     <t>_4_c1_s_</t>
@@ -227,10 +144,16 @@
     <t>_4_c2_s_</t>
   </si>
   <si>
+    <t>5pm Years 9-12</t>
+  </si>
+  <si>
     <t>_5_c1_s_</t>
   </si>
   <si>
     <t>_5_c2_s_</t>
+  </si>
+  <si>
+    <t>6pm Years 9-12</t>
   </si>
   <si>
     <t>_6_c1_s_</t>
@@ -239,47 +162,113 @@
     <t>_6_c2_s_</t>
   </si>
   <si>
-    <t>_1_c1_b_</t>
-  </si>
-  <si>
-    <t>_2_c1_b_</t>
-  </si>
-  <si>
-    <t>_1_c2_b_</t>
-  </si>
-  <si>
-    <t>_2_c2_b_</t>
-  </si>
-  <si>
     <t>GRADES _year_group_</t>
   </si>
   <si>
-    <t>7pm</t>
+    <t>_team_white_title_</t>
   </si>
   <si>
-    <t>745pm</t>
+    <t>_team_black_title_</t>
   </si>
   <si>
-    <t>_7_c1_s_</t>
+    <t>Team A</t>
   </si>
   <si>
-    <t>_7_c2_s_</t>
+    <t>Team B</t>
   </si>
   <si>
-    <t>_745_c1_s_</t>
+    <t>_venue_</t>
   </si>
   <si>
-    <t>_745_c2_s_</t>
+    <t>_court_</t>
+  </si>
+  <si>
+    <t>Venue</t>
+  </si>
+  <si>
+    <t>Court</t>
+  </si>
+  <si>
+    <t>_date_</t>
+  </si>
+  <si>
+    <t>_time_</t>
+  </si>
+  <si>
+    <t>_team_white_</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>Time</t>
+  </si>
+  <si>
+    <t>Time Outs</t>
+  </si>
+  <si>
+    <t>Team Fouls</t>
+  </si>
+  <si>
+    <t>RUNNING SCORE</t>
+  </si>
+  <si>
+    <t>First Half</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>Second Half</t>
   </si>
   <si>
     <t>Extra Periods</t>
+  </si>
+  <si>
+    <t>FOULS</t>
+  </si>
+  <si>
+    <t>No.</t>
+  </si>
+  <si>
+    <t>Name of Player</t>
+  </si>
+  <si>
+    <t>_a_player_num_</t>
+  </si>
+  <si>
+    <t>_a_player_name_</t>
+  </si>
+  <si>
+    <t>_team_black_</t>
+  </si>
+  <si>
+    <t>_b_player_num_</t>
+  </si>
+  <si>
+    <t>_b_player_name_</t>
+  </si>
+  <si>
+    <t>SCORES</t>
+  </si>
+  <si>
+    <t>FINAL SCORE:</t>
+  </si>
+  <si>
+    <t>Full Time</t>
+  </si>
+  <si>
+    <t>WINNING TEAM:</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="19" x14ac:knownFonts="1">
+  <fonts count="15">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -378,37 +367,6 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <i/>
-      <sz val="28"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="28"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="28"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="28"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="8">
     <fill>
@@ -943,7 +901,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="95">
+  <cellXfs count="91">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1090,6 +1048,39 @@
     <xf numFmtId="0" fontId="6" fillId="7" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="15" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="7" borderId="31" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1100,6 +1091,27 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="7" borderId="29" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="27" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="34" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="33" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="28" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="27" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="32" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="6" fillId="7" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="7" borderId="35" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1115,15 +1127,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="7" borderId="35" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="27" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="28" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="27" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="14" fontId="11" fillId="0" borderId="27" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1143,63 +1146,6 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="7" borderId="27" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="33" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="32" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="34" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="6" fillId="7" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="15" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1321,8 +1267,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="305566" y="3198865"/>
-          <a:ext cx="417183" cy="108000"/>
+          <a:off x="300803" y="3141715"/>
+          <a:ext cx="407658" cy="108000"/>
           <a:chOff x="408650" y="3345734"/>
           <a:chExt cx="322695" cy="108000"/>
         </a:xfrm>
@@ -1560,8 +1506,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="305566" y="3365553"/>
-          <a:ext cx="417183" cy="108000"/>
+          <a:off x="300803" y="3303640"/>
+          <a:ext cx="407658" cy="108000"/>
           <a:chOff x="408650" y="3345734"/>
           <a:chExt cx="322695" cy="108000"/>
         </a:xfrm>
@@ -1748,8 +1694,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="305566" y="3532240"/>
-          <a:ext cx="417183" cy="108000"/>
+          <a:off x="300803" y="3465565"/>
+          <a:ext cx="407658" cy="108000"/>
           <a:chOff x="408650" y="3345734"/>
           <a:chExt cx="322695" cy="108000"/>
         </a:xfrm>
@@ -1936,8 +1882,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="305566" y="3698928"/>
-          <a:ext cx="417183" cy="108000"/>
+          <a:off x="300803" y="3627490"/>
+          <a:ext cx="407658" cy="108000"/>
           <a:chOff x="408650" y="3345734"/>
           <a:chExt cx="322695" cy="108000"/>
         </a:xfrm>
@@ -2124,8 +2070,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="305566" y="3865615"/>
-          <a:ext cx="417183" cy="108000"/>
+          <a:off x="300803" y="3789415"/>
+          <a:ext cx="407658" cy="108000"/>
           <a:chOff x="408650" y="3345734"/>
           <a:chExt cx="322695" cy="108000"/>
         </a:xfrm>
@@ -2312,8 +2258,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="305566" y="4032303"/>
-          <a:ext cx="417183" cy="108000"/>
+          <a:off x="300803" y="3951340"/>
+          <a:ext cx="407658" cy="108000"/>
           <a:chOff x="408650" y="3345734"/>
           <a:chExt cx="322695" cy="108000"/>
         </a:xfrm>
@@ -2500,8 +2446,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="305566" y="4198990"/>
-          <a:ext cx="417183" cy="108000"/>
+          <a:off x="300803" y="4113265"/>
+          <a:ext cx="407658" cy="108000"/>
           <a:chOff x="408650" y="3345734"/>
           <a:chExt cx="322695" cy="108000"/>
         </a:xfrm>
@@ -2688,8 +2634,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="305566" y="4365678"/>
-          <a:ext cx="417183" cy="108000"/>
+          <a:off x="300803" y="4275190"/>
+          <a:ext cx="407658" cy="108000"/>
           <a:chOff x="408650" y="3345734"/>
           <a:chExt cx="322695" cy="108000"/>
         </a:xfrm>
@@ -2876,8 +2822,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="305566" y="4532365"/>
-          <a:ext cx="417183" cy="108000"/>
+          <a:off x="300803" y="4437115"/>
+          <a:ext cx="407658" cy="108000"/>
           <a:chOff x="408650" y="3345734"/>
           <a:chExt cx="322695" cy="108000"/>
         </a:xfrm>
@@ -3064,8 +3010,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="305566" y="4699053"/>
-          <a:ext cx="417183" cy="108000"/>
+          <a:off x="300803" y="4599040"/>
+          <a:ext cx="407658" cy="108000"/>
           <a:chOff x="408650" y="3345734"/>
           <a:chExt cx="322695" cy="108000"/>
         </a:xfrm>
@@ -3252,8 +3198,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="305566" y="4865740"/>
-          <a:ext cx="417183" cy="108000"/>
+          <a:off x="300803" y="4760965"/>
+          <a:ext cx="407658" cy="108000"/>
           <a:chOff x="408650" y="3345734"/>
           <a:chExt cx="322695" cy="108000"/>
         </a:xfrm>
@@ -3440,8 +3386,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="305566" y="5032428"/>
-          <a:ext cx="417183" cy="108000"/>
+          <a:off x="300803" y="4922890"/>
+          <a:ext cx="407658" cy="108000"/>
           <a:chOff x="408650" y="3345734"/>
           <a:chExt cx="322695" cy="108000"/>
         </a:xfrm>
@@ -3628,8 +3574,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="305566" y="6961240"/>
-          <a:ext cx="417183" cy="108000"/>
+          <a:off x="300803" y="6799315"/>
+          <a:ext cx="407658" cy="108000"/>
           <a:chOff x="408650" y="3345734"/>
           <a:chExt cx="322695" cy="108000"/>
         </a:xfrm>
@@ -3816,8 +3762,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="305566" y="6794553"/>
-          <a:ext cx="417183" cy="108000"/>
+          <a:off x="300803" y="6637390"/>
+          <a:ext cx="407658" cy="108000"/>
           <a:chOff x="408650" y="3345734"/>
           <a:chExt cx="322695" cy="108000"/>
         </a:xfrm>
@@ -4004,8 +3950,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="305566" y="7127928"/>
-          <a:ext cx="417183" cy="108000"/>
+          <a:off x="300803" y="6961240"/>
+          <a:ext cx="407658" cy="108000"/>
           <a:chOff x="408650" y="3345734"/>
           <a:chExt cx="322695" cy="108000"/>
         </a:xfrm>
@@ -4192,8 +4138,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="305566" y="7294615"/>
-          <a:ext cx="417183" cy="108000"/>
+          <a:off x="300803" y="7123165"/>
+          <a:ext cx="407658" cy="108000"/>
           <a:chOff x="408650" y="3345734"/>
           <a:chExt cx="322695" cy="108000"/>
         </a:xfrm>
@@ -4380,8 +4326,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="305566" y="7461303"/>
-          <a:ext cx="417183" cy="108000"/>
+          <a:off x="300803" y="7285090"/>
+          <a:ext cx="407658" cy="108000"/>
           <a:chOff x="408650" y="3345734"/>
           <a:chExt cx="322695" cy="108000"/>
         </a:xfrm>
@@ -4568,8 +4514,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="305566" y="7627990"/>
-          <a:ext cx="417183" cy="108000"/>
+          <a:off x="300803" y="7447015"/>
+          <a:ext cx="407658" cy="108000"/>
           <a:chOff x="408650" y="3345734"/>
           <a:chExt cx="322695" cy="108000"/>
         </a:xfrm>
@@ -4756,8 +4702,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="305566" y="7794678"/>
-          <a:ext cx="417183" cy="108000"/>
+          <a:off x="300803" y="7608940"/>
+          <a:ext cx="407658" cy="108000"/>
           <a:chOff x="408650" y="3345734"/>
           <a:chExt cx="322695" cy="108000"/>
         </a:xfrm>
@@ -4944,8 +4890,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="305566" y="7961365"/>
-          <a:ext cx="417183" cy="108000"/>
+          <a:off x="300803" y="7770865"/>
+          <a:ext cx="407658" cy="108000"/>
           <a:chOff x="408650" y="3345734"/>
           <a:chExt cx="322695" cy="108000"/>
         </a:xfrm>
@@ -5132,8 +5078,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="305566" y="8128053"/>
-          <a:ext cx="417183" cy="108000"/>
+          <a:off x="300803" y="7932790"/>
+          <a:ext cx="407658" cy="108000"/>
           <a:chOff x="408650" y="3345734"/>
           <a:chExt cx="322695" cy="108000"/>
         </a:xfrm>
@@ -5320,8 +5266,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="305566" y="8294740"/>
-          <a:ext cx="417183" cy="108000"/>
+          <a:off x="300803" y="8094715"/>
+          <a:ext cx="407658" cy="108000"/>
           <a:chOff x="408650" y="3345734"/>
           <a:chExt cx="322695" cy="108000"/>
         </a:xfrm>
@@ -5508,8 +5454,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="305566" y="8461428"/>
-          <a:ext cx="417183" cy="108000"/>
+          <a:off x="300803" y="8256640"/>
+          <a:ext cx="407658" cy="108000"/>
           <a:chOff x="408650" y="3345734"/>
           <a:chExt cx="322695" cy="108000"/>
         </a:xfrm>
@@ -5696,8 +5642,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="305566" y="8628115"/>
-          <a:ext cx="417183" cy="108000"/>
+          <a:off x="300803" y="8418565"/>
+          <a:ext cx="407658" cy="108000"/>
           <a:chOff x="408650" y="3345734"/>
           <a:chExt cx="322695" cy="108000"/>
         </a:xfrm>
@@ -6160,260 +6106,260 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06001A37-2C87-4F4D-8D59-4864FA219C19}">
   <dimension ref="A1:G20"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="33.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="33.7109375" defaultRowHeight="14.45"/>
   <cols>
-    <col min="1" max="1" width="29.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="56.88671875" customWidth="1"/>
-    <col min="3" max="3" width="29.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="56.88671875" customWidth="1"/>
+    <col min="1" max="1" width="29.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="56.85546875" customWidth="1"/>
+    <col min="3" max="3" width="29.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="56.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="23.4" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:7" ht="23.45">
       <c r="A1" s="1" t="s">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>12</v>
-      </c>
       <c r="D1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F1" s="2" t="s">
         <v>1</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>0</v>
       </c>
       <c r="G1" s="34"/>
     </row>
-    <row r="2" spans="1:7" ht="23.4" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:7" ht="23.45">
       <c r="A2" s="3" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B2" s="35" t="s">
-        <v>45</v>
+        <v>4</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D2" s="35" t="s">
-        <v>46</v>
+        <v>5</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="F2" s="37" t="s">
-        <v>67</v>
+        <v>7</v>
       </c>
       <c r="G2" s="34"/>
     </row>
-    <row r="3" spans="1:7" ht="23.4" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:7" ht="23.45">
       <c r="A3" s="3" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="B3" s="35" t="s">
-        <v>47</v>
+        <v>9</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="D3" s="35" t="s">
-        <v>48</v>
+        <v>10</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="F3" s="37" t="s">
-        <v>68</v>
+        <v>12</v>
       </c>
       <c r="G3" s="34"/>
     </row>
-    <row r="4" spans="1:7" ht="23.4" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:7" ht="23.45">
       <c r="A4" s="3" t="s">
-        <v>49</v>
+        <v>13</v>
       </c>
       <c r="B4" s="35" t="s">
-        <v>50</v>
+        <v>14</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="D4" s="36" t="s">
-        <v>51</v>
+        <v>16</v>
       </c>
       <c r="E4" s="34"/>
       <c r="F4" s="34"/>
       <c r="G4" s="34"/>
     </row>
-    <row r="5" spans="1:7" ht="23.4" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:7" ht="23.45">
       <c r="A5" s="4" t="s">
-        <v>4</v>
+        <v>17</v>
       </c>
       <c r="B5" s="36" t="s">
-        <v>52</v>
+        <v>18</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>4</v>
+        <v>17</v>
       </c>
       <c r="D5" s="36" t="s">
-        <v>53</v>
+        <v>19</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G5" s="34"/>
     </row>
-    <row r="6" spans="1:7" ht="23.4" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:7" ht="23.45">
       <c r="A6" s="4" t="s">
-        <v>54</v>
+        <v>20</v>
       </c>
       <c r="B6" s="36" t="s">
-        <v>55</v>
+        <v>21</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>54</v>
+        <v>20</v>
       </c>
       <c r="D6" s="36" t="s">
-        <v>56</v>
+        <v>22</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="F6" s="37" t="s">
-        <v>69</v>
+        <v>23</v>
       </c>
       <c r="G6" s="34"/>
     </row>
-    <row r="7" spans="1:7" ht="23.4" x14ac:dyDescent="0.45">
-      <c r="A7" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="B7" s="37" t="s">
-        <v>57</v>
+    <row r="7" spans="1:7" ht="23.25">
+      <c r="A7" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B7" s="36" t="s">
+        <v>25</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="D7" s="37" t="s">
-        <v>58</v>
+        <v>26</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="F7" s="37" t="s">
-        <v>70</v>
+        <v>27</v>
       </c>
       <c r="G7" s="34"/>
     </row>
-    <row r="8" spans="1:7" ht="23.4" x14ac:dyDescent="0.45">
-      <c r="A8" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="B8" s="38" t="s">
-        <v>59</v>
+    <row r="8" spans="1:7" ht="23.25">
+      <c r="A8" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="B8" s="37" t="s">
+        <v>29</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>11</v>
+        <v>30</v>
       </c>
       <c r="D8" s="38" t="s">
-        <v>60</v>
+        <v>31</v>
       </c>
       <c r="E8" s="34"/>
     </row>
-    <row r="9" spans="1:7" ht="23.4" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:7" ht="23.45">
       <c r="A9" s="6" t="s">
-        <v>6</v>
+        <v>32</v>
       </c>
       <c r="B9" s="38" t="s">
-        <v>61</v>
+        <v>33</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>6</v>
+        <v>32</v>
       </c>
       <c r="D9" s="38" t="s">
-        <v>62</v>
+        <v>34</v>
       </c>
       <c r="E9" s="34"/>
     </row>
-    <row r="10" spans="1:7" ht="23.4" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:7" ht="23.45">
       <c r="A10" s="6" t="s">
-        <v>7</v>
+        <v>35</v>
       </c>
       <c r="B10" s="38" t="s">
-        <v>63</v>
+        <v>36</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>7</v>
+        <v>35</v>
       </c>
       <c r="D10" s="38" t="s">
-        <v>64</v>
+        <v>37</v>
       </c>
       <c r="E10" s="34"/>
     </row>
-    <row r="11" spans="1:7" ht="23.4" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:7" ht="23.45">
       <c r="A11" s="6" t="s">
-        <v>8</v>
+        <v>38</v>
       </c>
       <c r="B11" s="38" t="s">
-        <v>65</v>
+        <v>39</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>8</v>
+        <v>38</v>
       </c>
       <c r="D11" s="38" t="s">
-        <v>66</v>
+        <v>40</v>
       </c>
       <c r="E11" s="34"/>
     </row>
-    <row r="12" spans="1:7" ht="22.8" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:7" ht="22.9">
       <c r="A12" s="34"/>
       <c r="B12" s="34"/>
       <c r="C12" s="34"/>
       <c r="D12" s="34"/>
       <c r="E12" s="34"/>
     </row>
-    <row r="13" spans="1:7" ht="22.8" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:7" ht="22.9">
       <c r="A13" s="34"/>
       <c r="B13" s="34"/>
       <c r="C13" s="34"/>
       <c r="D13" s="34"/>
       <c r="E13" s="34"/>
     </row>
-    <row r="14" spans="1:7" ht="22.8" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:7" ht="22.9">
       <c r="D14" s="34"/>
       <c r="E14" s="34"/>
     </row>
-    <row r="15" spans="1:7" ht="22.8" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:7" ht="22.9">
       <c r="D15" s="34"/>
       <c r="E15" s="34"/>
     </row>
-    <row r="16" spans="1:7" ht="22.8" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:7" ht="22.9">
       <c r="D16" s="34"/>
       <c r="E16" s="34"/>
     </row>
-    <row r="17" spans="4:5" ht="22.8" x14ac:dyDescent="0.4">
+    <row r="17" spans="4:5" ht="22.9">
       <c r="D17" s="34"/>
       <c r="E17" s="34"/>
     </row>
-    <row r="18" spans="4:5" ht="22.8" x14ac:dyDescent="0.4">
+    <row r="18" spans="4:5" ht="22.9">
       <c r="D18" s="34"/>
       <c r="E18" s="34"/>
     </row>
-    <row r="19" spans="4:5" ht="22.8" x14ac:dyDescent="0.4">
+    <row r="19" spans="4:5" ht="22.9">
       <c r="D19" s="34"/>
       <c r="E19" s="34"/>
     </row>
-    <row r="20" spans="4:5" ht="22.8" x14ac:dyDescent="0.4">
+    <row r="20" spans="4:5" ht="22.9">
       <c r="D20" s="34"/>
       <c r="E20" s="34"/>
     </row>
@@ -6425,132 +6371,6 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1BC4CC0-FE9D-498F-AEB1-D5F0C0522F79}">
-  <dimension ref="A1:E20"/>
-  <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="33.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="17.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="27.77734375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.44140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="27.77734375" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" ht="36.6" x14ac:dyDescent="0.7">
-      <c r="A1" s="91"/>
-      <c r="B1" s="92" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="91"/>
-      <c r="D1" s="92" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1" s="34"/>
-    </row>
-    <row r="2" spans="1:5" ht="36.6" x14ac:dyDescent="0.7">
-      <c r="A2" s="93" t="s">
-        <v>72</v>
-      </c>
-      <c r="B2" s="94" t="s">
-        <v>74</v>
-      </c>
-      <c r="C2" s="93" t="s">
-        <v>72</v>
-      </c>
-      <c r="D2" s="94" t="s">
-        <v>75</v>
-      </c>
-      <c r="E2" s="34"/>
-    </row>
-    <row r="3" spans="1:5" ht="36.6" x14ac:dyDescent="0.7">
-      <c r="A3" s="93" t="s">
-        <v>73</v>
-      </c>
-      <c r="B3" s="94" t="s">
-        <v>76</v>
-      </c>
-      <c r="C3" s="93" t="s">
-        <v>73</v>
-      </c>
-      <c r="D3" s="94" t="s">
-        <v>77</v>
-      </c>
-      <c r="E3" s="34"/>
-    </row>
-    <row r="4" spans="1:5" ht="22.8" x14ac:dyDescent="0.4">
-      <c r="A4" s="34"/>
-    </row>
-    <row r="5" spans="1:5" ht="22.8" x14ac:dyDescent="0.4">
-      <c r="A5" s="34"/>
-    </row>
-    <row r="6" spans="1:5" ht="22.8" x14ac:dyDescent="0.4">
-      <c r="A6" s="34"/>
-    </row>
-    <row r="7" spans="1:5" ht="22.8" x14ac:dyDescent="0.4">
-      <c r="A7" s="34"/>
-    </row>
-    <row r="8" spans="1:5" ht="22.8" x14ac:dyDescent="0.4">
-      <c r="A8" s="34"/>
-    </row>
-    <row r="9" spans="1:5" ht="22.8" x14ac:dyDescent="0.4">
-      <c r="A9" s="34"/>
-    </row>
-    <row r="10" spans="1:5" ht="22.8" x14ac:dyDescent="0.4">
-      <c r="A10" s="34"/>
-    </row>
-    <row r="11" spans="1:5" ht="22.8" x14ac:dyDescent="0.4">
-      <c r="A11" s="34"/>
-    </row>
-    <row r="12" spans="1:5" ht="22.8" x14ac:dyDescent="0.4">
-      <c r="A12" s="34"/>
-    </row>
-    <row r="13" spans="1:5" ht="22.8" x14ac:dyDescent="0.4">
-      <c r="A13" s="34"/>
-      <c r="B13" s="34"/>
-      <c r="C13" s="34"/>
-      <c r="D13" s="34"/>
-      <c r="E13" s="34"/>
-    </row>
-    <row r="14" spans="1:5" ht="22.8" x14ac:dyDescent="0.4">
-      <c r="A14" s="34"/>
-      <c r="B14" s="34"/>
-    </row>
-    <row r="15" spans="1:5" ht="22.8" x14ac:dyDescent="0.4">
-      <c r="A15" s="34"/>
-      <c r="B15" s="34"/>
-    </row>
-    <row r="16" spans="1:5" ht="22.8" x14ac:dyDescent="0.4">
-      <c r="A16" s="34"/>
-      <c r="B16" s="34"/>
-    </row>
-    <row r="17" spans="1:2" ht="22.8" x14ac:dyDescent="0.4">
-      <c r="A17" s="34"/>
-      <c r="B17" s="34"/>
-    </row>
-    <row r="18" spans="1:2" ht="22.8" x14ac:dyDescent="0.4">
-      <c r="A18" s="34"/>
-      <c r="B18" s="34"/>
-    </row>
-    <row r="19" spans="1:2" ht="22.8" x14ac:dyDescent="0.4">
-      <c r="A19" s="34"/>
-      <c r="B19" s="34"/>
-    </row>
-    <row r="20" spans="1:2" ht="22.8" x14ac:dyDescent="0.4">
-      <c r="A20" s="34"/>
-      <c r="B20" s="34"/>
-    </row>
-  </sheetData>
-  <printOptions horizontalCentered="1"/>
-  <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
-  <pageSetup paperSize="9" fitToWidth="0" fitToHeight="0" orientation="landscape" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{45F774DF-630E-4CCD-B16A-123A9D720A00}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
@@ -6561,23 +6381,23 @@
       <selection activeCell="AF9" sqref="AF9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="13.15"/>
   <cols>
-    <col min="1" max="1" width="2.6640625" style="7" customWidth="1"/>
-    <col min="2" max="2" width="1.44140625" style="7" customWidth="1"/>
+    <col min="1" max="1" width="2.7109375" style="7" customWidth="1"/>
+    <col min="2" max="2" width="1.42578125" style="7" customWidth="1"/>
     <col min="3" max="3" width="4" style="8" customWidth="1"/>
-    <col min="4" max="4" width="3.109375" style="7" customWidth="1"/>
-    <col min="5" max="5" width="14.33203125" style="7" customWidth="1"/>
+    <col min="4" max="4" width="3.140625" style="7" customWidth="1"/>
+    <col min="5" max="5" width="14.28515625" style="7" customWidth="1"/>
     <col min="6" max="10" width="2" style="7" customWidth="1"/>
-    <col min="11" max="19" width="3.109375" style="8" customWidth="1"/>
+    <col min="11" max="19" width="3.140625" style="8" customWidth="1"/>
     <col min="20" max="21" width="4" style="8" bestFit="1" customWidth="1"/>
-    <col min="22" max="23" width="3.109375" style="8" customWidth="1"/>
+    <col min="22" max="23" width="3.140625" style="8" customWidth="1"/>
     <col min="24" max="25" width="4" style="8" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="3.109375" style="8" customWidth="1"/>
-    <col min="27" max="16384" width="9.109375" style="7"/>
+    <col min="26" max="26" width="3.140625" style="8" customWidth="1"/>
+    <col min="27" max="16384" width="9.140625" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:26" ht="33" customHeight="1">
       <c r="A1" s="33"/>
       <c r="B1" s="31"/>
       <c r="C1" s="32"/>
@@ -6588,52 +6408,52 @@
       <c r="H1" s="30"/>
       <c r="I1" s="30"/>
       <c r="J1" s="30"/>
-      <c r="K1" s="70" t="s">
-        <v>71</v>
-      </c>
-      <c r="L1" s="71"/>
-      <c r="M1" s="71"/>
-      <c r="N1" s="71"/>
-      <c r="O1" s="71"/>
-      <c r="P1" s="71"/>
-      <c r="Q1" s="71"/>
-      <c r="R1" s="71"/>
-      <c r="S1" s="71"/>
-      <c r="T1" s="71"/>
-      <c r="U1" s="71"/>
-      <c r="V1" s="71"/>
-      <c r="W1" s="71"/>
-      <c r="X1" s="71"/>
-      <c r="Y1" s="71"/>
+      <c r="K1" s="85" t="s">
+        <v>41</v>
+      </c>
+      <c r="L1" s="86"/>
+      <c r="M1" s="86"/>
+      <c r="N1" s="86"/>
+      <c r="O1" s="86"/>
+      <c r="P1" s="86"/>
+      <c r="Q1" s="86"/>
+      <c r="R1" s="86"/>
+      <c r="S1" s="86"/>
+      <c r="T1" s="86"/>
+      <c r="U1" s="86"/>
+      <c r="V1" s="86"/>
+      <c r="W1" s="86"/>
+      <c r="X1" s="86"/>
+      <c r="Y1" s="86"/>
       <c r="Z1" s="29"/>
     </row>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:26">
       <c r="A2" s="28"/>
       <c r="Z2" s="27"/>
     </row>
-    <row r="3" spans="1:26" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:26" ht="13.9" thickBot="1">
       <c r="A3" s="28"/>
-      <c r="K3" s="72" t="s">
-        <v>37</v>
-      </c>
-      <c r="L3" s="72"/>
-      <c r="M3" s="72"/>
-      <c r="N3" s="72"/>
-      <c r="O3" s="72"/>
-      <c r="P3" s="72"/>
-      <c r="Q3" s="72"/>
-      <c r="S3" s="72" t="s">
-        <v>38</v>
-      </c>
-      <c r="T3" s="72"/>
-      <c r="U3" s="72"/>
-      <c r="V3" s="72"/>
-      <c r="W3" s="72"/>
-      <c r="X3" s="72"/>
-      <c r="Y3" s="72"/>
+      <c r="K3" s="87" t="s">
+        <v>42</v>
+      </c>
+      <c r="L3" s="87"/>
+      <c r="M3" s="87"/>
+      <c r="N3" s="87"/>
+      <c r="O3" s="87"/>
+      <c r="P3" s="87"/>
+      <c r="Q3" s="87"/>
+      <c r="S3" s="87" t="s">
+        <v>43</v>
+      </c>
+      <c r="T3" s="87"/>
+      <c r="U3" s="87"/>
+      <c r="V3" s="87"/>
+      <c r="W3" s="87"/>
+      <c r="X3" s="87"/>
+      <c r="Y3" s="87"/>
       <c r="Z3" s="27"/>
     </row>
-    <row r="4" spans="1:26" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:26" ht="13.9">
       <c r="A4" s="21"/>
       <c r="B4" s="19"/>
       <c r="C4" s="20"/>
@@ -6644,28 +6464,28 @@
       <c r="H4" s="19"/>
       <c r="I4" s="19"/>
       <c r="J4" s="19"/>
-      <c r="K4" s="73" t="s">
-        <v>18</v>
-      </c>
-      <c r="L4" s="73"/>
-      <c r="M4" s="73"/>
-      <c r="N4" s="73"/>
-      <c r="O4" s="73"/>
-      <c r="P4" s="73"/>
-      <c r="Q4" s="73"/>
+      <c r="K4" s="88" t="s">
+        <v>44</v>
+      </c>
+      <c r="L4" s="88"/>
+      <c r="M4" s="88"/>
+      <c r="N4" s="88"/>
+      <c r="O4" s="88"/>
+      <c r="P4" s="88"/>
+      <c r="Q4" s="88"/>
       <c r="R4" s="20"/>
-      <c r="S4" s="73" t="s">
-        <v>17</v>
-      </c>
-      <c r="T4" s="73"/>
-      <c r="U4" s="73"/>
-      <c r="V4" s="73"/>
-      <c r="W4" s="73"/>
-      <c r="X4" s="73"/>
-      <c r="Y4" s="73"/>
+      <c r="S4" s="88" t="s">
+        <v>45</v>
+      </c>
+      <c r="T4" s="88"/>
+      <c r="U4" s="88"/>
+      <c r="V4" s="88"/>
+      <c r="W4" s="88"/>
+      <c r="X4" s="88"/>
+      <c r="Y4" s="88"/>
       <c r="Z4" s="25"/>
     </row>
-    <row r="5" spans="1:26" ht="15.6" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:26" ht="15.6" thickBot="1">
       <c r="A5" s="21"/>
       <c r="B5" s="19"/>
       <c r="C5" s="20"/>
@@ -6676,28 +6496,28 @@
       <c r="H5" s="19"/>
       <c r="I5" s="19"/>
       <c r="J5" s="19"/>
-      <c r="K5" s="74" t="s">
-        <v>43</v>
-      </c>
-      <c r="L5" s="74"/>
-      <c r="M5" s="74"/>
-      <c r="N5" s="74"/>
-      <c r="O5" s="74"/>
-      <c r="P5" s="74"/>
-      <c r="Q5" s="74"/>
+      <c r="K5" s="89" t="s">
+        <v>46</v>
+      </c>
+      <c r="L5" s="89"/>
+      <c r="M5" s="89"/>
+      <c r="N5" s="89"/>
+      <c r="O5" s="89"/>
+      <c r="P5" s="89"/>
+      <c r="Q5" s="89"/>
       <c r="R5" s="20"/>
-      <c r="S5" s="74" t="s">
-        <v>36</v>
-      </c>
-      <c r="T5" s="74"/>
-      <c r="U5" s="74"/>
-      <c r="V5" s="74"/>
-      <c r="W5" s="74"/>
-      <c r="X5" s="74"/>
-      <c r="Y5" s="74"/>
+      <c r="S5" s="89" t="s">
+        <v>47</v>
+      </c>
+      <c r="T5" s="89"/>
+      <c r="U5" s="89"/>
+      <c r="V5" s="89"/>
+      <c r="W5" s="89"/>
+      <c r="X5" s="89"/>
+      <c r="Y5" s="89"/>
       <c r="Z5" s="25"/>
     </row>
-    <row r="6" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:26">
       <c r="A6" s="21"/>
       <c r="B6" s="19"/>
       <c r="C6" s="20"/>
@@ -6708,28 +6528,28 @@
       <c r="H6" s="19"/>
       <c r="I6" s="19"/>
       <c r="J6" s="19"/>
-      <c r="K6" s="75" t="s">
-        <v>35</v>
-      </c>
-      <c r="L6" s="75"/>
-      <c r="M6" s="75"/>
-      <c r="N6" s="75"/>
-      <c r="O6" s="75"/>
-      <c r="P6" s="75"/>
-      <c r="Q6" s="75"/>
+      <c r="K6" s="90" t="s">
+        <v>48</v>
+      </c>
+      <c r="L6" s="90"/>
+      <c r="M6" s="90"/>
+      <c r="N6" s="90"/>
+      <c r="O6" s="90"/>
+      <c r="P6" s="90"/>
+      <c r="Q6" s="90"/>
       <c r="R6" s="20"/>
-      <c r="S6" s="75" t="s">
-        <v>34</v>
-      </c>
-      <c r="T6" s="75"/>
-      <c r="U6" s="75"/>
-      <c r="V6" s="75"/>
-      <c r="W6" s="75"/>
-      <c r="X6" s="75"/>
-      <c r="Y6" s="75"/>
+      <c r="S6" s="90" t="s">
+        <v>49</v>
+      </c>
+      <c r="T6" s="90"/>
+      <c r="U6" s="90"/>
+      <c r="V6" s="90"/>
+      <c r="W6" s="90"/>
+      <c r="X6" s="90"/>
+      <c r="Y6" s="90"/>
       <c r="Z6" s="25"/>
     </row>
-    <row r="7" spans="1:26" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:26" ht="13.9" thickBot="1">
       <c r="A7" s="21"/>
       <c r="B7" s="19"/>
       <c r="C7" s="20"/>
@@ -6741,18 +6561,18 @@
       <c r="I7" s="19"/>
       <c r="J7" s="19"/>
       <c r="K7" s="20"/>
-      <c r="L7" s="81" t="s">
-        <v>44</v>
-      </c>
-      <c r="M7" s="80"/>
-      <c r="N7" s="80"/>
-      <c r="O7" s="82"/>
+      <c r="L7" s="79" t="s">
+        <v>50</v>
+      </c>
+      <c r="M7" s="63"/>
+      <c r="N7" s="63"/>
+      <c r="O7" s="62"/>
       <c r="P7" s="20"/>
-      <c r="Q7" s="79" t="s">
-        <v>33</v>
-      </c>
-      <c r="R7" s="80"/>
-      <c r="S7" s="82"/>
+      <c r="Q7" s="61" t="s">
+        <v>51</v>
+      </c>
+      <c r="R7" s="63"/>
+      <c r="S7" s="62"/>
       <c r="T7" s="20"/>
       <c r="U7" s="20"/>
       <c r="V7" s="20"/>
@@ -6761,34 +6581,34 @@
       <c r="Y7" s="20"/>
       <c r="Z7" s="25"/>
     </row>
-    <row r="8" spans="1:26" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="58" t="s">
-        <v>18</v>
-      </c>
-      <c r="B8" s="59"/>
-      <c r="C8" s="59"/>
-      <c r="D8" s="60" t="s">
-        <v>32</v>
-      </c>
-      <c r="E8" s="61"/>
-      <c r="F8" s="61"/>
-      <c r="G8" s="61"/>
-      <c r="H8" s="61"/>
-      <c r="I8" s="61"/>
-      <c r="J8" s="62"/>
+    <row r="8" spans="1:26" ht="16.149999999999999" thickBot="1">
+      <c r="A8" s="69" t="s">
+        <v>44</v>
+      </c>
+      <c r="B8" s="70"/>
+      <c r="C8" s="70"/>
+      <c r="D8" s="71" t="s">
+        <v>52</v>
+      </c>
+      <c r="E8" s="72"/>
+      <c r="F8" s="72"/>
+      <c r="G8" s="72"/>
+      <c r="H8" s="72"/>
+      <c r="I8" s="72"/>
+      <c r="J8" s="80"/>
       <c r="K8" s="20"/>
-      <c r="L8" s="63" t="s">
-        <v>31</v>
-      </c>
-      <c r="M8" s="63"/>
-      <c r="N8" s="63"/>
-      <c r="O8" s="63"/>
+      <c r="L8" s="81" t="s">
+        <v>53</v>
+      </c>
+      <c r="M8" s="81"/>
+      <c r="N8" s="81"/>
+      <c r="O8" s="81"/>
       <c r="P8" s="20"/>
-      <c r="Q8" s="63" t="s">
-        <v>30</v>
-      </c>
-      <c r="R8" s="63"/>
-      <c r="S8" s="63"/>
+      <c r="Q8" s="81" t="s">
+        <v>54</v>
+      </c>
+      <c r="R8" s="81"/>
+      <c r="S8" s="81"/>
       <c r="T8" s="20"/>
       <c r="U8" s="26"/>
       <c r="V8" s="20"/>
@@ -6797,47 +6617,47 @@
       <c r="Y8" s="20"/>
       <c r="Z8" s="25"/>
     </row>
-    <row r="9" spans="1:26" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="68" t="s">
-        <v>27</v>
-      </c>
-      <c r="B9" s="69"/>
-      <c r="C9" s="69"/>
-      <c r="D9" s="69"/>
-      <c r="E9" s="67" t="s">
-        <v>26</v>
-      </c>
-      <c r="F9" s="67"/>
-      <c r="G9" s="67"/>
-      <c r="H9" s="67"/>
-      <c r="I9" s="67"/>
+    <row r="9" spans="1:26" ht="15.75" customHeight="1" thickBot="1">
+      <c r="A9" s="76" t="s">
+        <v>55</v>
+      </c>
+      <c r="B9" s="77"/>
+      <c r="C9" s="77"/>
+      <c r="D9" s="77"/>
+      <c r="E9" s="73" t="s">
+        <v>56</v>
+      </c>
+      <c r="F9" s="73"/>
+      <c r="G9" s="73"/>
+      <c r="H9" s="73"/>
+      <c r="I9" s="73"/>
       <c r="J9" s="40"/>
-      <c r="K9" s="64" t="s">
-        <v>29</v>
-      </c>
-      <c r="L9" s="65"/>
-      <c r="M9" s="65"/>
-      <c r="N9" s="65"/>
-      <c r="O9" s="65"/>
-      <c r="P9" s="65"/>
-      <c r="Q9" s="65"/>
-      <c r="R9" s="65"/>
-      <c r="S9" s="65"/>
-      <c r="T9" s="65"/>
-      <c r="U9" s="65"/>
-      <c r="V9" s="65"/>
-      <c r="W9" s="65"/>
-      <c r="X9" s="65"/>
-      <c r="Y9" s="65"/>
-      <c r="Z9" s="66"/>
+      <c r="K9" s="82" t="s">
+        <v>57</v>
+      </c>
+      <c r="L9" s="83"/>
+      <c r="M9" s="83"/>
+      <c r="N9" s="83"/>
+      <c r="O9" s="83"/>
+      <c r="P9" s="83"/>
+      <c r="Q9" s="83"/>
+      <c r="R9" s="83"/>
+      <c r="S9" s="83"/>
+      <c r="T9" s="83"/>
+      <c r="U9" s="83"/>
+      <c r="V9" s="83"/>
+      <c r="W9" s="83"/>
+      <c r="X9" s="83"/>
+      <c r="Y9" s="83"/>
+      <c r="Z9" s="84"/>
     </row>
-    <row r="10" spans="1:26" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:26" ht="15.75" customHeight="1" thickBot="1">
       <c r="A10" s="21"/>
-      <c r="B10" s="79"/>
-      <c r="C10" s="82"/>
+      <c r="B10" s="61"/>
+      <c r="C10" s="62"/>
       <c r="D10" s="19"/>
       <c r="E10" s="39" t="s">
-        <v>21</v>
+        <v>58</v>
       </c>
       <c r="F10" s="41">
         <v>1</v>
@@ -6852,43 +6672,43 @@
         <v>4</v>
       </c>
       <c r="J10" s="19"/>
-      <c r="K10" s="78" t="s">
-        <v>15</v>
-      </c>
-      <c r="L10" s="76"/>
-      <c r="M10" s="76" t="s">
-        <v>14</v>
-      </c>
-      <c r="N10" s="77"/>
-      <c r="O10" s="78" t="s">
-        <v>15</v>
-      </c>
-      <c r="P10" s="76"/>
-      <c r="Q10" s="76" t="s">
-        <v>14</v>
-      </c>
-      <c r="R10" s="77"/>
-      <c r="S10" s="78" t="s">
-        <v>15</v>
-      </c>
-      <c r="T10" s="76"/>
-      <c r="U10" s="76" t="s">
-        <v>14</v>
-      </c>
-      <c r="V10" s="77"/>
-      <c r="W10" s="78" t="s">
-        <v>15</v>
-      </c>
-      <c r="X10" s="76"/>
-      <c r="Y10" s="76" t="s">
-        <v>14</v>
-      </c>
-      <c r="Z10" s="77"/>
+      <c r="K10" s="74" t="s">
+        <v>59</v>
+      </c>
+      <c r="L10" s="75"/>
+      <c r="M10" s="75" t="s">
+        <v>60</v>
+      </c>
+      <c r="N10" s="78"/>
+      <c r="O10" s="74" t="s">
+        <v>59</v>
+      </c>
+      <c r="P10" s="75"/>
+      <c r="Q10" s="75" t="s">
+        <v>60</v>
+      </c>
+      <c r="R10" s="78"/>
+      <c r="S10" s="74" t="s">
+        <v>59</v>
+      </c>
+      <c r="T10" s="75"/>
+      <c r="U10" s="75" t="s">
+        <v>60</v>
+      </c>
+      <c r="V10" s="78"/>
+      <c r="W10" s="74" t="s">
+        <v>59</v>
+      </c>
+      <c r="X10" s="75"/>
+      <c r="Y10" s="75" t="s">
+        <v>60</v>
+      </c>
+      <c r="Z10" s="78"/>
     </row>
-    <row r="11" spans="1:26" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:26" ht="13.9" thickBot="1">
       <c r="A11" s="21"/>
-      <c r="B11" s="79"/>
-      <c r="C11" s="82"/>
+      <c r="B11" s="61"/>
+      <c r="C11" s="62"/>
       <c r="D11" s="20"/>
       <c r="E11" s="20"/>
       <c r="F11" s="44">
@@ -6937,13 +6757,13 @@
       </c>
       <c r="Z11" s="15"/>
     </row>
-    <row r="12" spans="1:26" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:26" ht="15.75" customHeight="1" thickBot="1">
       <c r="A12" s="21"/>
-      <c r="B12" s="79"/>
-      <c r="C12" s="82"/>
+      <c r="B12" s="61"/>
+      <c r="C12" s="62"/>
       <c r="D12" s="19"/>
       <c r="E12" s="39" t="s">
-        <v>20</v>
+        <v>61</v>
       </c>
       <c r="F12" s="47">
         <v>1</v>
@@ -6991,10 +6811,10 @@
       </c>
       <c r="Z12" s="15"/>
     </row>
-    <row r="13" spans="1:26" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:26" ht="13.9" thickBot="1">
       <c r="A13" s="21"/>
-      <c r="B13" s="79"/>
-      <c r="C13" s="82"/>
+      <c r="B13" s="61"/>
+      <c r="C13" s="62"/>
       <c r="D13" s="20"/>
       <c r="E13" s="20"/>
       <c r="F13" s="41">
@@ -7043,13 +6863,13 @@
       </c>
       <c r="Z13" s="15"/>
     </row>
-    <row r="14" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:26" ht="15" customHeight="1">
       <c r="A14" s="21"/>
-      <c r="B14" s="79"/>
-      <c r="C14" s="82"/>
+      <c r="B14" s="61"/>
+      <c r="C14" s="62"/>
       <c r="D14" s="11"/>
       <c r="E14" s="19" t="s">
-        <v>78</v>
+        <v>62</v>
       </c>
       <c r="F14" s="20"/>
       <c r="G14" s="19"/>
@@ -7089,19 +6909,19 @@
       </c>
       <c r="Z14" s="15"/>
     </row>
-    <row r="15" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A15" s="79"/>
-      <c r="B15" s="80"/>
-      <c r="C15" s="82"/>
+    <row r="15" spans="1:26">
+      <c r="A15" s="61"/>
+      <c r="B15" s="63"/>
+      <c r="C15" s="62"/>
       <c r="D15" s="19"/>
       <c r="E15" s="19"/>
-      <c r="F15" s="79" t="s">
-        <v>25</v>
-      </c>
-      <c r="G15" s="80"/>
-      <c r="H15" s="80"/>
-      <c r="I15" s="80"/>
-      <c r="J15" s="80"/>
+      <c r="F15" s="61" t="s">
+        <v>63</v>
+      </c>
+      <c r="G15" s="63"/>
+      <c r="H15" s="63"/>
+      <c r="I15" s="63"/>
+      <c r="J15" s="63"/>
       <c r="K15" s="16"/>
       <c r="L15" s="22">
         <v>5</v>
@@ -7135,16 +6955,16 @@
       </c>
       <c r="Z15" s="15"/>
     </row>
-    <row r="16" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A16" s="79" t="s">
-        <v>24</v>
-      </c>
-      <c r="B16" s="80"/>
-      <c r="C16" s="82"/>
-      <c r="D16" s="83" t="s">
-        <v>23</v>
-      </c>
-      <c r="E16" s="84"/>
+    <row r="16" spans="1:26">
+      <c r="A16" s="61" t="s">
+        <v>64</v>
+      </c>
+      <c r="B16" s="63"/>
+      <c r="C16" s="62"/>
+      <c r="D16" s="67" t="s">
+        <v>65</v>
+      </c>
+      <c r="E16" s="68"/>
       <c r="F16" s="50">
         <v>1</v>
       </c>
@@ -7193,15 +7013,15 @@
       </c>
       <c r="Z16" s="15"/>
     </row>
-    <row r="17" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A17" s="85" t="s">
-        <v>40</v>
-      </c>
-      <c r="B17" s="82"/>
-      <c r="C17" s="79"/>
-      <c r="D17" s="82"/>
+    <row r="17" spans="1:26">
+      <c r="A17" s="64" t="s">
+        <v>66</v>
+      </c>
+      <c r="B17" s="62"/>
+      <c r="C17" s="61"/>
+      <c r="D17" s="62"/>
       <c r="E17" s="18" t="s">
-        <v>39</v>
+        <v>67</v>
       </c>
       <c r="F17" s="11"/>
       <c r="G17" s="11"/>
@@ -7241,11 +7061,11 @@
       </c>
       <c r="Z17" s="15"/>
     </row>
-    <row r="18" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A18" s="85"/>
-      <c r="B18" s="82"/>
-      <c r="C18" s="79"/>
-      <c r="D18" s="82"/>
+    <row r="18" spans="1:26">
+      <c r="A18" s="64"/>
+      <c r="B18" s="62"/>
+      <c r="C18" s="61"/>
+      <c r="D18" s="62"/>
       <c r="E18" s="18"/>
       <c r="F18" s="18"/>
       <c r="G18" s="11"/>
@@ -7285,11 +7105,11 @@
       </c>
       <c r="Z18" s="15"/>
     </row>
-    <row r="19" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A19" s="85"/>
-      <c r="B19" s="82"/>
-      <c r="C19" s="79"/>
-      <c r="D19" s="82"/>
+    <row r="19" spans="1:26">
+      <c r="A19" s="64"/>
+      <c r="B19" s="62"/>
+      <c r="C19" s="61"/>
+      <c r="D19" s="62"/>
       <c r="E19" s="18"/>
       <c r="F19" s="18"/>
       <c r="G19" s="11"/>
@@ -7329,11 +7149,11 @@
       </c>
       <c r="Z19" s="15"/>
     </row>
-    <row r="20" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A20" s="85"/>
-      <c r="B20" s="82"/>
-      <c r="C20" s="79"/>
-      <c r="D20" s="82"/>
+    <row r="20" spans="1:26">
+      <c r="A20" s="64"/>
+      <c r="B20" s="62"/>
+      <c r="C20" s="61"/>
+      <c r="D20" s="62"/>
       <c r="E20" s="18"/>
       <c r="F20" s="18"/>
       <c r="G20" s="11"/>
@@ -7373,11 +7193,11 @@
       </c>
       <c r="Z20" s="15"/>
     </row>
-    <row r="21" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A21" s="85"/>
-      <c r="B21" s="82"/>
-      <c r="C21" s="79"/>
-      <c r="D21" s="82"/>
+    <row r="21" spans="1:26">
+      <c r="A21" s="64"/>
+      <c r="B21" s="62"/>
+      <c r="C21" s="61"/>
+      <c r="D21" s="62"/>
       <c r="E21" s="18"/>
       <c r="F21" s="18"/>
       <c r="G21" s="11"/>
@@ -7417,11 +7237,11 @@
       </c>
       <c r="Z21" s="15"/>
     </row>
-    <row r="22" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A22" s="85"/>
-      <c r="B22" s="82"/>
-      <c r="C22" s="79"/>
-      <c r="D22" s="82"/>
+    <row r="22" spans="1:26">
+      <c r="A22" s="64"/>
+      <c r="B22" s="62"/>
+      <c r="C22" s="61"/>
+      <c r="D22" s="62"/>
       <c r="E22" s="18"/>
       <c r="F22" s="18"/>
       <c r="G22" s="11"/>
@@ -7461,11 +7281,11 @@
       </c>
       <c r="Z22" s="15"/>
     </row>
-    <row r="23" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A23" s="85"/>
-      <c r="B23" s="82"/>
-      <c r="C23" s="79"/>
-      <c r="D23" s="82"/>
+    <row r="23" spans="1:26">
+      <c r="A23" s="64"/>
+      <c r="B23" s="62"/>
+      <c r="C23" s="61"/>
+      <c r="D23" s="62"/>
       <c r="E23" s="18"/>
       <c r="F23" s="18"/>
       <c r="G23" s="11"/>
@@ -7505,11 +7325,11 @@
       </c>
       <c r="Z23" s="15"/>
     </row>
-    <row r="24" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A24" s="85"/>
-      <c r="B24" s="82"/>
-      <c r="C24" s="79"/>
-      <c r="D24" s="82"/>
+    <row r="24" spans="1:26">
+      <c r="A24" s="64"/>
+      <c r="B24" s="62"/>
+      <c r="C24" s="61"/>
+      <c r="D24" s="62"/>
       <c r="E24" s="18"/>
       <c r="F24" s="18"/>
       <c r="G24" s="11"/>
@@ -7549,11 +7369,11 @@
       </c>
       <c r="Z24" s="15"/>
     </row>
-    <row r="25" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A25" s="85"/>
-      <c r="B25" s="82"/>
-      <c r="C25" s="79"/>
-      <c r="D25" s="82"/>
+    <row r="25" spans="1:26">
+      <c r="A25" s="64"/>
+      <c r="B25" s="62"/>
+      <c r="C25" s="61"/>
+      <c r="D25" s="62"/>
       <c r="E25" s="18"/>
       <c r="F25" s="18"/>
       <c r="G25" s="11"/>
@@ -7593,11 +7413,11 @@
       </c>
       <c r="Z25" s="15"/>
     </row>
-    <row r="26" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A26" s="85"/>
-      <c r="B26" s="82"/>
-      <c r="C26" s="79"/>
-      <c r="D26" s="82"/>
+    <row r="26" spans="1:26">
+      <c r="A26" s="64"/>
+      <c r="B26" s="62"/>
+      <c r="C26" s="61"/>
+      <c r="D26" s="62"/>
       <c r="E26" s="18"/>
       <c r="F26" s="18"/>
       <c r="G26" s="11"/>
@@ -7637,11 +7457,11 @@
       </c>
       <c r="Z26" s="15"/>
     </row>
-    <row r="27" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A27" s="85"/>
-      <c r="B27" s="82"/>
-      <c r="C27" s="79"/>
-      <c r="D27" s="82"/>
+    <row r="27" spans="1:26">
+      <c r="A27" s="64"/>
+      <c r="B27" s="62"/>
+      <c r="C27" s="61"/>
+      <c r="D27" s="62"/>
       <c r="E27" s="18"/>
       <c r="F27" s="18"/>
       <c r="G27" s="11"/>
@@ -7681,11 +7501,11 @@
       </c>
       <c r="Z27" s="15"/>
     </row>
-    <row r="28" spans="1:26" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="85"/>
-      <c r="B28" s="82"/>
-      <c r="C28" s="79"/>
-      <c r="D28" s="82"/>
+    <row r="28" spans="1:26" ht="13.9" thickBot="1">
+      <c r="A28" s="64"/>
+      <c r="B28" s="62"/>
+      <c r="C28" s="61"/>
+      <c r="D28" s="62"/>
       <c r="E28" s="18"/>
       <c r="F28" s="18"/>
       <c r="G28" s="11"/>
@@ -7725,21 +7545,21 @@
       </c>
       <c r="Z28" s="15"/>
     </row>
-    <row r="29" spans="1:26" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A29" s="58" t="s">
-        <v>17</v>
-      </c>
-      <c r="B29" s="59"/>
-      <c r="C29" s="59"/>
-      <c r="D29" s="60" t="s">
-        <v>28</v>
-      </c>
-      <c r="E29" s="61"/>
-      <c r="F29" s="61"/>
-      <c r="G29" s="61"/>
-      <c r="H29" s="61"/>
-      <c r="I29" s="61"/>
-      <c r="J29" s="61"/>
+    <row r="29" spans="1:26" ht="16.149999999999999" thickBot="1">
+      <c r="A29" s="69" t="s">
+        <v>45</v>
+      </c>
+      <c r="B29" s="70"/>
+      <c r="C29" s="70"/>
+      <c r="D29" s="71" t="s">
+        <v>68</v>
+      </c>
+      <c r="E29" s="72"/>
+      <c r="F29" s="72"/>
+      <c r="G29" s="72"/>
+      <c r="H29" s="72"/>
+      <c r="I29" s="72"/>
+      <c r="J29" s="72"/>
       <c r="K29" s="16"/>
       <c r="L29" s="22">
         <v>19</v>
@@ -7773,20 +7593,20 @@
       </c>
       <c r="Z29" s="15"/>
     </row>
-    <row r="30" spans="1:26" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="68" t="s">
-        <v>27</v>
-      </c>
-      <c r="B30" s="69"/>
-      <c r="C30" s="69"/>
-      <c r="D30" s="69"/>
-      <c r="E30" s="67" t="s">
-        <v>26</v>
-      </c>
-      <c r="F30" s="67"/>
-      <c r="G30" s="67"/>
-      <c r="H30" s="67"/>
-      <c r="I30" s="67"/>
+    <row r="30" spans="1:26" ht="13.9" thickBot="1">
+      <c r="A30" s="76" t="s">
+        <v>55</v>
+      </c>
+      <c r="B30" s="77"/>
+      <c r="C30" s="77"/>
+      <c r="D30" s="77"/>
+      <c r="E30" s="73" t="s">
+        <v>56</v>
+      </c>
+      <c r="F30" s="73"/>
+      <c r="G30" s="73"/>
+      <c r="H30" s="73"/>
+      <c r="I30" s="73"/>
       <c r="J30" s="40"/>
       <c r="K30" s="16"/>
       <c r="L30" s="22">
@@ -7821,13 +7641,13 @@
       </c>
       <c r="Z30" s="15"/>
     </row>
-    <row r="31" spans="1:26" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:26" ht="13.9" thickBot="1">
       <c r="A31" s="21"/>
-      <c r="B31" s="79"/>
-      <c r="C31" s="82"/>
+      <c r="B31" s="61"/>
+      <c r="C31" s="62"/>
       <c r="D31" s="19"/>
       <c r="E31" s="39" t="s">
-        <v>21</v>
+        <v>58</v>
       </c>
       <c r="F31" s="41">
         <v>1</v>
@@ -7875,10 +7695,10 @@
       </c>
       <c r="Z31" s="15"/>
     </row>
-    <row r="32" spans="1:26" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:26" ht="13.9" thickBot="1">
       <c r="A32" s="21"/>
-      <c r="B32" s="79"/>
-      <c r="C32" s="82"/>
+      <c r="B32" s="61"/>
+      <c r="C32" s="62"/>
       <c r="D32" s="20"/>
       <c r="E32" s="20"/>
       <c r="F32" s="44">
@@ -7927,13 +7747,13 @@
       </c>
       <c r="Z32" s="15"/>
     </row>
-    <row r="33" spans="1:26" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:26" ht="13.9" thickBot="1">
       <c r="A33" s="21"/>
-      <c r="B33" s="79"/>
-      <c r="C33" s="82"/>
+      <c r="B33" s="61"/>
+      <c r="C33" s="62"/>
       <c r="D33" s="19"/>
       <c r="E33" s="39" t="s">
-        <v>20</v>
+        <v>61</v>
       </c>
       <c r="F33" s="47">
         <v>1</v>
@@ -7981,10 +7801,10 @@
       </c>
       <c r="Z33" s="15"/>
     </row>
-    <row r="34" spans="1:26" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:26" ht="13.9" thickBot="1">
       <c r="A34" s="21"/>
-      <c r="B34" s="79"/>
-      <c r="C34" s="82"/>
+      <c r="B34" s="61"/>
+      <c r="C34" s="62"/>
       <c r="D34" s="20"/>
       <c r="E34" s="20"/>
       <c r="F34" s="41">
@@ -8033,13 +7853,13 @@
       </c>
       <c r="Z34" s="15"/>
     </row>
-    <row r="35" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:26">
       <c r="A35" s="21"/>
-      <c r="B35" s="79"/>
-      <c r="C35" s="82"/>
+      <c r="B35" s="61"/>
+      <c r="C35" s="62"/>
       <c r="D35" s="11"/>
       <c r="E35" s="19" t="s">
-        <v>78</v>
+        <v>62</v>
       </c>
       <c r="F35" s="20"/>
       <c r="G35" s="19"/>
@@ -8079,19 +7899,19 @@
       </c>
       <c r="Z35" s="15"/>
     </row>
-    <row r="36" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A36" s="79"/>
-      <c r="B36" s="80"/>
-      <c r="C36" s="82"/>
+    <row r="36" spans="1:26">
+      <c r="A36" s="61"/>
+      <c r="B36" s="63"/>
+      <c r="C36" s="62"/>
       <c r="D36" s="19"/>
       <c r="E36" s="19"/>
-      <c r="F36" s="79" t="s">
-        <v>25</v>
-      </c>
-      <c r="G36" s="80"/>
-      <c r="H36" s="80"/>
-      <c r="I36" s="80"/>
-      <c r="J36" s="80"/>
+      <c r="F36" s="61" t="s">
+        <v>63</v>
+      </c>
+      <c r="G36" s="63"/>
+      <c r="H36" s="63"/>
+      <c r="I36" s="63"/>
+      <c r="J36" s="63"/>
       <c r="K36" s="16"/>
       <c r="L36" s="22">
         <v>26</v>
@@ -8125,16 +7945,16 @@
       </c>
       <c r="Z36" s="15"/>
     </row>
-    <row r="37" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A37" s="79" t="s">
-        <v>24</v>
-      </c>
-      <c r="B37" s="80"/>
-      <c r="C37" s="82"/>
-      <c r="D37" s="83" t="s">
-        <v>23</v>
-      </c>
-      <c r="E37" s="84"/>
+    <row r="37" spans="1:26">
+      <c r="A37" s="61" t="s">
+        <v>64</v>
+      </c>
+      <c r="B37" s="63"/>
+      <c r="C37" s="62"/>
+      <c r="D37" s="67" t="s">
+        <v>65</v>
+      </c>
+      <c r="E37" s="68"/>
       <c r="F37" s="50">
         <v>1</v>
       </c>
@@ -8183,15 +8003,15 @@
       </c>
       <c r="Z37" s="15"/>
     </row>
-    <row r="38" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A38" s="85" t="s">
-        <v>41</v>
-      </c>
-      <c r="B38" s="82"/>
-      <c r="C38" s="79"/>
-      <c r="D38" s="82"/>
+    <row r="38" spans="1:26">
+      <c r="A38" s="64" t="s">
+        <v>69</v>
+      </c>
+      <c r="B38" s="62"/>
+      <c r="C38" s="61"/>
+      <c r="D38" s="62"/>
       <c r="E38" s="18" t="s">
-        <v>42</v>
+        <v>70</v>
       </c>
       <c r="F38" s="18"/>
       <c r="G38" s="11"/>
@@ -8231,11 +8051,11 @@
       </c>
       <c r="Z38" s="15"/>
     </row>
-    <row r="39" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A39" s="85"/>
-      <c r="B39" s="82"/>
-      <c r="C39" s="79"/>
-      <c r="D39" s="82"/>
+    <row r="39" spans="1:26">
+      <c r="A39" s="64"/>
+      <c r="B39" s="62"/>
+      <c r="C39" s="61"/>
+      <c r="D39" s="62"/>
       <c r="E39" s="18"/>
       <c r="F39" s="18"/>
       <c r="G39" s="11"/>
@@ -8275,11 +8095,11 @@
       </c>
       <c r="Z39" s="15"/>
     </row>
-    <row r="40" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A40" s="85"/>
-      <c r="B40" s="82"/>
-      <c r="C40" s="79"/>
-      <c r="D40" s="82"/>
+    <row r="40" spans="1:26">
+      <c r="A40" s="64"/>
+      <c r="B40" s="62"/>
+      <c r="C40" s="61"/>
+      <c r="D40" s="62"/>
       <c r="E40" s="18"/>
       <c r="F40" s="18"/>
       <c r="G40" s="11"/>
@@ -8319,11 +8139,11 @@
       </c>
       <c r="Z40" s="15"/>
     </row>
-    <row r="41" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A41" s="85"/>
-      <c r="B41" s="82"/>
-      <c r="C41" s="79"/>
-      <c r="D41" s="82"/>
+    <row r="41" spans="1:26">
+      <c r="A41" s="64"/>
+      <c r="B41" s="62"/>
+      <c r="C41" s="61"/>
+      <c r="D41" s="62"/>
       <c r="E41" s="18"/>
       <c r="F41" s="18"/>
       <c r="G41" s="11"/>
@@ -8363,11 +8183,11 @@
       </c>
       <c r="Z41" s="15"/>
     </row>
-    <row r="42" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A42" s="85"/>
-      <c r="B42" s="82"/>
-      <c r="C42" s="79"/>
-      <c r="D42" s="82"/>
+    <row r="42" spans="1:26">
+      <c r="A42" s="64"/>
+      <c r="B42" s="62"/>
+      <c r="C42" s="61"/>
+      <c r="D42" s="62"/>
       <c r="E42" s="18"/>
       <c r="F42" s="18"/>
       <c r="G42" s="11"/>
@@ -8407,11 +8227,11 @@
       </c>
       <c r="Z42" s="15"/>
     </row>
-    <row r="43" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A43" s="85"/>
-      <c r="B43" s="82"/>
-      <c r="C43" s="79"/>
-      <c r="D43" s="82"/>
+    <row r="43" spans="1:26">
+      <c r="A43" s="64"/>
+      <c r="B43" s="62"/>
+      <c r="C43" s="61"/>
+      <c r="D43" s="62"/>
       <c r="E43" s="18"/>
       <c r="F43" s="18"/>
       <c r="G43" s="11"/>
@@ -8451,11 +8271,11 @@
       </c>
       <c r="Z43" s="15"/>
     </row>
-    <row r="44" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A44" s="85"/>
-      <c r="B44" s="82"/>
-      <c r="C44" s="79"/>
-      <c r="D44" s="82"/>
+    <row r="44" spans="1:26">
+      <c r="A44" s="64"/>
+      <c r="B44" s="62"/>
+      <c r="C44" s="61"/>
+      <c r="D44" s="62"/>
       <c r="E44" s="18"/>
       <c r="F44" s="18"/>
       <c r="G44" s="11"/>
@@ -8495,11 +8315,11 @@
       </c>
       <c r="Z44" s="15"/>
     </row>
-    <row r="45" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A45" s="85"/>
-      <c r="B45" s="82"/>
-      <c r="C45" s="79"/>
-      <c r="D45" s="82"/>
+    <row r="45" spans="1:26">
+      <c r="A45" s="64"/>
+      <c r="B45" s="62"/>
+      <c r="C45" s="61"/>
+      <c r="D45" s="62"/>
       <c r="E45" s="18"/>
       <c r="F45" s="18"/>
       <c r="G45" s="11"/>
@@ -8539,11 +8359,11 @@
       </c>
       <c r="Z45" s="15"/>
     </row>
-    <row r="46" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A46" s="85"/>
-      <c r="B46" s="82"/>
-      <c r="C46" s="79"/>
-      <c r="D46" s="82"/>
+    <row r="46" spans="1:26">
+      <c r="A46" s="64"/>
+      <c r="B46" s="62"/>
+      <c r="C46" s="61"/>
+      <c r="D46" s="62"/>
       <c r="E46" s="18"/>
       <c r="F46" s="18"/>
       <c r="G46" s="11"/>
@@ -8583,11 +8403,11 @@
       </c>
       <c r="Z46" s="15"/>
     </row>
-    <row r="47" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A47" s="85"/>
-      <c r="B47" s="82"/>
-      <c r="C47" s="79"/>
-      <c r="D47" s="82"/>
+    <row r="47" spans="1:26">
+      <c r="A47" s="64"/>
+      <c r="B47" s="62"/>
+      <c r="C47" s="61"/>
+      <c r="D47" s="62"/>
       <c r="E47" s="18"/>
       <c r="F47" s="18"/>
       <c r="G47" s="11"/>
@@ -8627,11 +8447,11 @@
       </c>
       <c r="Z47" s="15"/>
     </row>
-    <row r="48" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A48" s="85"/>
-      <c r="B48" s="82"/>
-      <c r="C48" s="79"/>
-      <c r="D48" s="82"/>
+    <row r="48" spans="1:26">
+      <c r="A48" s="64"/>
+      <c r="B48" s="62"/>
+      <c r="C48" s="61"/>
+      <c r="D48" s="62"/>
       <c r="E48" s="18"/>
       <c r="F48" s="18"/>
       <c r="G48" s="11"/>
@@ -8671,11 +8491,11 @@
       </c>
       <c r="Z48" s="15"/>
     </row>
-    <row r="49" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A49" s="85"/>
-      <c r="B49" s="82"/>
-      <c r="C49" s="79"/>
-      <c r="D49" s="82"/>
+    <row r="49" spans="1:26">
+      <c r="A49" s="64"/>
+      <c r="B49" s="62"/>
+      <c r="C49" s="61"/>
+      <c r="D49" s="62"/>
       <c r="E49" s="18"/>
       <c r="F49" s="18"/>
       <c r="G49" s="11"/>
@@ -8715,13 +8535,13 @@
       </c>
       <c r="Z49" s="15"/>
     </row>
-    <row r="50" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="88" t="s">
-        <v>22</v>
-      </c>
-      <c r="B50" s="89"/>
-      <c r="C50" s="89"/>
-      <c r="D50" s="90"/>
+    <row r="50" spans="1:26" ht="15" customHeight="1">
+      <c r="A50" s="58" t="s">
+        <v>71</v>
+      </c>
+      <c r="B50" s="59"/>
+      <c r="C50" s="59"/>
+      <c r="D50" s="60"/>
       <c r="E50" s="14"/>
       <c r="F50" s="14"/>
       <c r="G50" s="14"/>
@@ -8761,23 +8581,23 @@
       </c>
       <c r="Z50" s="12"/>
     </row>
-    <row r="51" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="79" t="s">
-        <v>21</v>
-      </c>
-      <c r="B51" s="80"/>
-      <c r="C51" s="80"/>
-      <c r="D51" s="82"/>
+    <row r="51" spans="1:26" ht="15" customHeight="1">
+      <c r="A51" s="61" t="s">
+        <v>58</v>
+      </c>
+      <c r="B51" s="63"/>
+      <c r="C51" s="63"/>
+      <c r="D51" s="62"/>
       <c r="E51" s="57" t="s">
-        <v>15</v>
-      </c>
-      <c r="F51" s="86"/>
-      <c r="G51" s="86"/>
+        <v>59</v>
+      </c>
+      <c r="F51" s="65"/>
+      <c r="G51" s="65"/>
       <c r="H51" s="56" t="s">
-        <v>14</v>
-      </c>
-      <c r="I51" s="86"/>
-      <c r="J51" s="86"/>
+        <v>60</v>
+      </c>
+      <c r="I51" s="65"/>
+      <c r="J51" s="65"/>
       <c r="K51" s="10"/>
       <c r="L51" s="10"/>
       <c r="M51" s="10"/>
@@ -8795,83 +8615,83 @@
       <c r="Y51" s="10"/>
       <c r="Z51" s="10"/>
     </row>
-    <row r="52" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="79" t="s">
-        <v>20</v>
-      </c>
-      <c r="B52" s="80"/>
-      <c r="C52" s="80"/>
-      <c r="D52" s="82"/>
+    <row r="52" spans="1:26" ht="15" customHeight="1">
+      <c r="A52" s="61" t="s">
+        <v>61</v>
+      </c>
+      <c r="B52" s="63"/>
+      <c r="C52" s="63"/>
+      <c r="D52" s="62"/>
       <c r="E52" s="57" t="s">
-        <v>15</v>
-      </c>
-      <c r="F52" s="86"/>
-      <c r="G52" s="86"/>
+        <v>59</v>
+      </c>
+      <c r="F52" s="65"/>
+      <c r="G52" s="65"/>
       <c r="H52" s="56" t="s">
-        <v>14</v>
-      </c>
-      <c r="I52" s="86"/>
-      <c r="J52" s="86"/>
-      <c r="K52" s="88" t="s">
-        <v>19</v>
-      </c>
-      <c r="L52" s="89"/>
-      <c r="M52" s="89"/>
-      <c r="N52" s="89"/>
-      <c r="O52" s="90"/>
-      <c r="P52" s="86" t="s">
-        <v>18</v>
-      </c>
-      <c r="Q52" s="86"/>
-      <c r="R52" s="86"/>
-      <c r="S52" s="86"/>
-      <c r="T52" s="86"/>
-      <c r="U52" s="86" t="s">
-        <v>17</v>
-      </c>
-      <c r="V52" s="86"/>
-      <c r="W52" s="86"/>
-      <c r="X52" s="86"/>
-      <c r="Y52" s="86"/>
+        <v>60</v>
+      </c>
+      <c r="I52" s="65"/>
+      <c r="J52" s="65"/>
+      <c r="K52" s="58" t="s">
+        <v>72</v>
+      </c>
+      <c r="L52" s="59"/>
+      <c r="M52" s="59"/>
+      <c r="N52" s="59"/>
+      <c r="O52" s="60"/>
+      <c r="P52" s="65" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q52" s="65"/>
+      <c r="R52" s="65"/>
+      <c r="S52" s="65"/>
+      <c r="T52" s="65"/>
+      <c r="U52" s="65" t="s">
+        <v>45</v>
+      </c>
+      <c r="V52" s="65"/>
+      <c r="W52" s="65"/>
+      <c r="X52" s="65"/>
+      <c r="Y52" s="65"/>
       <c r="Z52" s="10"/>
     </row>
-    <row r="53" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="88" t="s">
-        <v>16</v>
-      </c>
-      <c r="B53" s="89"/>
-      <c r="C53" s="89"/>
-      <c r="D53" s="90"/>
+    <row r="53" spans="1:26" ht="15" customHeight="1">
+      <c r="A53" s="58" t="s">
+        <v>73</v>
+      </c>
+      <c r="B53" s="59"/>
+      <c r="C53" s="59"/>
+      <c r="D53" s="60"/>
       <c r="E53" s="57" t="s">
-        <v>15</v>
-      </c>
-      <c r="F53" s="86"/>
-      <c r="G53" s="86"/>
+        <v>59</v>
+      </c>
+      <c r="F53" s="65"/>
+      <c r="G53" s="65"/>
       <c r="H53" s="56" t="s">
-        <v>14</v>
-      </c>
-      <c r="I53" s="86"/>
-      <c r="J53" s="86"/>
-      <c r="K53" s="87" t="s">
-        <v>13</v>
-      </c>
-      <c r="L53" s="87"/>
-      <c r="M53" s="87"/>
-      <c r="N53" s="87"/>
-      <c r="O53" s="87"/>
-      <c r="P53" s="87"/>
-      <c r="Q53" s="87"/>
-      <c r="R53" s="86"/>
-      <c r="S53" s="86"/>
-      <c r="T53" s="86"/>
-      <c r="U53" s="86"/>
-      <c r="V53" s="86"/>
-      <c r="W53" s="86"/>
-      <c r="X53" s="86"/>
-      <c r="Y53" s="86"/>
+        <v>60</v>
+      </c>
+      <c r="I53" s="65"/>
+      <c r="J53" s="65"/>
+      <c r="K53" s="66" t="s">
+        <v>74</v>
+      </c>
+      <c r="L53" s="66"/>
+      <c r="M53" s="66"/>
+      <c r="N53" s="66"/>
+      <c r="O53" s="66"/>
+      <c r="P53" s="66"/>
+      <c r="Q53" s="66"/>
+      <c r="R53" s="65"/>
+      <c r="S53" s="65"/>
+      <c r="T53" s="65"/>
+      <c r="U53" s="65"/>
+      <c r="V53" s="65"/>
+      <c r="W53" s="65"/>
+      <c r="X53" s="65"/>
+      <c r="Y53" s="65"/>
       <c r="Z53" s="10"/>
     </row>
-    <row r="55" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:26">
       <c r="D55" s="9"/>
       <c r="K55" s="7"/>
       <c r="L55" s="7"/>
@@ -8890,7 +8710,7 @@
       <c r="Y55" s="7"/>
       <c r="Z55" s="7"/>
     </row>
-    <row r="56" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:26">
       <c r="K56" s="7"/>
       <c r="L56" s="7"/>
       <c r="M56" s="7"/>
@@ -8908,7 +8728,7 @@
       <c r="Y56" s="7"/>
       <c r="Z56" s="7"/>
     </row>
-    <row r="57" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:26">
       <c r="K57" s="7"/>
       <c r="L57" s="7"/>
       <c r="M57" s="7"/>
@@ -8926,7 +8746,7 @@
       <c r="Y57" s="7"/>
       <c r="Z57" s="7"/>
     </row>
-    <row r="58" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:26">
       <c r="K58" s="7"/>
       <c r="L58" s="7"/>
       <c r="M58" s="7"/>
@@ -8944,7 +8764,7 @@
       <c r="Y58" s="7"/>
       <c r="Z58" s="7"/>
     </row>
-    <row r="59" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:26">
       <c r="K59" s="7"/>
       <c r="L59" s="7"/>
       <c r="M59" s="7"/>
@@ -8962,7 +8782,7 @@
       <c r="Y59" s="7"/>
       <c r="Z59" s="7"/>
     </row>
-    <row r="60" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:26">
       <c r="K60" s="7"/>
       <c r="L60" s="7"/>
       <c r="M60" s="7"/>
@@ -8980,7 +8800,7 @@
       <c r="Y60" s="7"/>
       <c r="Z60" s="7"/>
     </row>
-    <row r="61" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:26">
       <c r="K61" s="7"/>
       <c r="L61" s="7"/>
       <c r="M61" s="7"/>
@@ -9000,6 +8820,95 @@
     </row>
   </sheetData>
   <mergeCells count="113">
+    <mergeCell ref="A8:C8"/>
+    <mergeCell ref="D8:J8"/>
+    <mergeCell ref="L8:O8"/>
+    <mergeCell ref="Q8:S8"/>
+    <mergeCell ref="K9:Z9"/>
+    <mergeCell ref="E9:I9"/>
+    <mergeCell ref="A9:D9"/>
+    <mergeCell ref="K1:Y1"/>
+    <mergeCell ref="K3:Q3"/>
+    <mergeCell ref="S3:Y3"/>
+    <mergeCell ref="K4:Q4"/>
+    <mergeCell ref="S4:Y4"/>
+    <mergeCell ref="K5:Q5"/>
+    <mergeCell ref="S5:Y5"/>
+    <mergeCell ref="K6:Q6"/>
+    <mergeCell ref="S6:Y6"/>
+    <mergeCell ref="M10:N10"/>
+    <mergeCell ref="O10:P10"/>
+    <mergeCell ref="Q10:R10"/>
+    <mergeCell ref="S10:T10"/>
+    <mergeCell ref="U10:V10"/>
+    <mergeCell ref="W10:X10"/>
+    <mergeCell ref="Y10:Z10"/>
+    <mergeCell ref="F15:J15"/>
+    <mergeCell ref="L7:O7"/>
+    <mergeCell ref="Q7:S7"/>
+    <mergeCell ref="K10:L10"/>
+    <mergeCell ref="A20:B20"/>
+    <mergeCell ref="C20:D20"/>
+    <mergeCell ref="A21:B21"/>
+    <mergeCell ref="C21:D21"/>
+    <mergeCell ref="A30:D30"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="A15:C15"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="C38:D38"/>
+    <mergeCell ref="A39:B39"/>
+    <mergeCell ref="C39:D39"/>
+    <mergeCell ref="A40:B40"/>
+    <mergeCell ref="C40:D40"/>
+    <mergeCell ref="A29:C29"/>
+    <mergeCell ref="D29:J29"/>
+    <mergeCell ref="E30:I30"/>
+    <mergeCell ref="A16:C16"/>
+    <mergeCell ref="D16:E16"/>
+    <mergeCell ref="A17:B17"/>
+    <mergeCell ref="A18:B18"/>
+    <mergeCell ref="C18:D18"/>
+    <mergeCell ref="F53:G53"/>
+    <mergeCell ref="I53:J53"/>
+    <mergeCell ref="K53:Q53"/>
+    <mergeCell ref="R53:Y53"/>
+    <mergeCell ref="F51:G51"/>
+    <mergeCell ref="I51:J51"/>
+    <mergeCell ref="F52:G52"/>
+    <mergeCell ref="I52:J52"/>
+    <mergeCell ref="P52:R52"/>
+    <mergeCell ref="S52:T52"/>
+    <mergeCell ref="K52:O52"/>
+    <mergeCell ref="B31:C31"/>
+    <mergeCell ref="B32:C32"/>
+    <mergeCell ref="U52:W52"/>
+    <mergeCell ref="X52:Y52"/>
+    <mergeCell ref="A46:B46"/>
+    <mergeCell ref="C46:D46"/>
+    <mergeCell ref="A47:B47"/>
+    <mergeCell ref="C47:D47"/>
+    <mergeCell ref="A48:B48"/>
+    <mergeCell ref="C48:D48"/>
+    <mergeCell ref="A49:B49"/>
+    <mergeCell ref="C49:D49"/>
+    <mergeCell ref="A41:B41"/>
+    <mergeCell ref="C41:D41"/>
+    <mergeCell ref="A42:B42"/>
+    <mergeCell ref="C42:D42"/>
+    <mergeCell ref="A43:B43"/>
+    <mergeCell ref="C43:D43"/>
+    <mergeCell ref="A44:B44"/>
+    <mergeCell ref="C45:D45"/>
+    <mergeCell ref="F36:J36"/>
+    <mergeCell ref="A37:C37"/>
+    <mergeCell ref="D37:E37"/>
+    <mergeCell ref="A38:B38"/>
     <mergeCell ref="A53:D53"/>
     <mergeCell ref="B33:C33"/>
     <mergeCell ref="B34:C34"/>
@@ -9024,95 +8933,6 @@
     <mergeCell ref="A52:D52"/>
     <mergeCell ref="C44:D44"/>
     <mergeCell ref="A45:B45"/>
-    <mergeCell ref="B31:C31"/>
-    <mergeCell ref="B32:C32"/>
-    <mergeCell ref="U52:W52"/>
-    <mergeCell ref="X52:Y52"/>
-    <mergeCell ref="A46:B46"/>
-    <mergeCell ref="C46:D46"/>
-    <mergeCell ref="A47:B47"/>
-    <mergeCell ref="C47:D47"/>
-    <mergeCell ref="A48:B48"/>
-    <mergeCell ref="C48:D48"/>
-    <mergeCell ref="A49:B49"/>
-    <mergeCell ref="C49:D49"/>
-    <mergeCell ref="A41:B41"/>
-    <mergeCell ref="C41:D41"/>
-    <mergeCell ref="A42:B42"/>
-    <mergeCell ref="C42:D42"/>
-    <mergeCell ref="A43:B43"/>
-    <mergeCell ref="C43:D43"/>
-    <mergeCell ref="A44:B44"/>
-    <mergeCell ref="F53:G53"/>
-    <mergeCell ref="I53:J53"/>
-    <mergeCell ref="K53:Q53"/>
-    <mergeCell ref="R53:Y53"/>
-    <mergeCell ref="F51:G51"/>
-    <mergeCell ref="I51:J51"/>
-    <mergeCell ref="F52:G52"/>
-    <mergeCell ref="I52:J52"/>
-    <mergeCell ref="P52:R52"/>
-    <mergeCell ref="S52:T52"/>
-    <mergeCell ref="K52:O52"/>
-    <mergeCell ref="C45:D45"/>
-    <mergeCell ref="F36:J36"/>
-    <mergeCell ref="A37:C37"/>
-    <mergeCell ref="D37:E37"/>
-    <mergeCell ref="A38:B38"/>
-    <mergeCell ref="C38:D38"/>
-    <mergeCell ref="A39:B39"/>
-    <mergeCell ref="C39:D39"/>
-    <mergeCell ref="A40:B40"/>
-    <mergeCell ref="C40:D40"/>
-    <mergeCell ref="A29:C29"/>
-    <mergeCell ref="D29:J29"/>
-    <mergeCell ref="E30:I30"/>
-    <mergeCell ref="A16:C16"/>
-    <mergeCell ref="D16:E16"/>
-    <mergeCell ref="A17:B17"/>
-    <mergeCell ref="A18:B18"/>
-    <mergeCell ref="C18:D18"/>
-    <mergeCell ref="K10:L10"/>
-    <mergeCell ref="A20:B20"/>
-    <mergeCell ref="C20:D20"/>
-    <mergeCell ref="A21:B21"/>
-    <mergeCell ref="C21:D21"/>
-    <mergeCell ref="A30:D30"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="B13:C13"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="A15:C15"/>
-    <mergeCell ref="C17:D17"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="C19:D19"/>
-    <mergeCell ref="M10:N10"/>
-    <mergeCell ref="O10:P10"/>
-    <mergeCell ref="Q10:R10"/>
-    <mergeCell ref="S10:T10"/>
-    <mergeCell ref="U10:V10"/>
-    <mergeCell ref="W10:X10"/>
-    <mergeCell ref="Y10:Z10"/>
-    <mergeCell ref="F15:J15"/>
-    <mergeCell ref="L7:O7"/>
-    <mergeCell ref="Q7:S7"/>
-    <mergeCell ref="A8:C8"/>
-    <mergeCell ref="D8:J8"/>
-    <mergeCell ref="L8:O8"/>
-    <mergeCell ref="Q8:S8"/>
-    <mergeCell ref="K9:Z9"/>
-    <mergeCell ref="E9:I9"/>
-    <mergeCell ref="A9:D9"/>
-    <mergeCell ref="K1:Y1"/>
-    <mergeCell ref="K3:Q3"/>
-    <mergeCell ref="S3:Y3"/>
-    <mergeCell ref="K4:Q4"/>
-    <mergeCell ref="S4:Y4"/>
-    <mergeCell ref="K5:Q5"/>
-    <mergeCell ref="S5:Y5"/>
-    <mergeCell ref="K6:Q6"/>
-    <mergeCell ref="S6:Y6"/>
   </mergeCells>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
   <pageMargins left="0.47244094488188981" right="0.35433070866141736" top="0.47244094488188981" bottom="0.19685039370078741" header="0.19685039370078741" footer="0.19685039370078741"/>

</xml_diff>

<commit_message>
updating template for consistency
</commit_message>
<xml_diff>
--- a/data/template.xlsx
+++ b/data/template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27004"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27016"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\baske\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{83CBDB96-6E83-47F4-A584-BAFA1E89E030}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{9E65F298-6809-4F8A-9967-3A8AF9B93D86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="1" xr2:uid="{026AB82B-103F-4DF3-A0CA-05AA2F209D25}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{026AB82B-103F-4DF3-A0CA-05AA2F209D25}"/>
   </bookViews>
   <sheets>
     <sheet name="runsheet-k" sheetId="5" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="74">
   <si>
     <t>Time &amp; Grade/Year</t>
   </si>
@@ -57,9 +57,6 @@
     <t>_9_c2_s_</t>
   </si>
   <si>
-    <t>1pm Years 7/8</t>
-  </si>
-  <si>
     <t>_1_c1_b_</t>
   </si>
   <si>
@@ -70,9 +67,6 @@
   </si>
   <si>
     <t>_10_c2_s_</t>
-  </si>
-  <si>
-    <t>2pm Years 7/8</t>
   </si>
   <si>
     <t>_2_c1_b_</t>
@@ -115,6 +109,9 @@
   </si>
   <si>
     <t>_2_c1_s_</t>
+  </si>
+  <si>
+    <t>2pm Years 7/8</t>
   </si>
   <si>
     <t>_2_c2_s_</t>
@@ -901,7 +898,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="91">
+  <cellXfs count="93">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1048,39 +1045,6 @@
     <xf numFmtId="0" fontId="6" fillId="7" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="15" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="7" borderId="31" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1091,27 +1055,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="7" borderId="29" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="27" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="34" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="33" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="28" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="27" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="32" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="6" fillId="7" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="7" borderId="35" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1127,6 +1070,15 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="7" borderId="35" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="27" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="28" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="27" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="14" fontId="11" fillId="0" borderId="27" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1146,6 +1098,57 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="7" borderId="27" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="33" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="32" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="34" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="6" fillId="7" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="15" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -6106,8 +6109,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06001A37-2C87-4F4D-8D59-4864FA219C19}">
   <dimension ref="A1:G20"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3:F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="33.7109375" defaultRowHeight="14.45"/>
@@ -6118,7 +6121,7 @@
     <col min="4" max="4" width="56.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="23.45">
+    <row r="1" spans="1:7" ht="23.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -6139,7 +6142,7 @@
       </c>
       <c r="G1" s="34"/>
     </row>
-    <row r="2" spans="1:7" ht="23.45">
+    <row r="2" spans="1:7" ht="23.25">
       <c r="A2" s="3" t="s">
         <v>3</v>
       </c>
@@ -6152,64 +6155,60 @@
       <c r="D2" s="35" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="E2" s="91" t="s">
         <v>6</v>
       </c>
-      <c r="F2" s="37" t="s">
-        <v>7</v>
-      </c>
+      <c r="F2" s="92"/>
       <c r="G2" s="34"/>
     </row>
-    <row r="3" spans="1:7" ht="23.45">
+    <row r="3" spans="1:7" ht="23.25">
       <c r="A3" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="35" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="35" t="s">
+      <c r="C3" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" s="35" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D3" s="35" t="s">
+      <c r="E3" s="91" t="s">
         <v>10</v>
       </c>
-      <c r="E3" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="F3" s="37" t="s">
-        <v>12</v>
-      </c>
+      <c r="F3" s="92"/>
       <c r="G3" s="34"/>
     </row>
-    <row r="4" spans="1:7" ht="23.45">
+    <row r="4" spans="1:7" ht="23.25">
       <c r="A4" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" s="35" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="B4" s="35" t="s">
+      <c r="D4" s="36" t="s">
         <v>14</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="D4" s="36" t="s">
-        <v>16</v>
       </c>
       <c r="E4" s="34"/>
       <c r="F4" s="34"/>
       <c r="G4" s="34"/>
     </row>
-    <row r="5" spans="1:7" ht="23.45">
+    <row r="5" spans="1:7" ht="23.25">
       <c r="A5" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" s="36" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5" s="36" t="s">
         <v>17</v>
-      </c>
-      <c r="B5" s="36" t="s">
-        <v>18</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="D5" s="36" t="s">
-        <v>19</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>0</v>
@@ -6219,105 +6218,101 @@
       </c>
       <c r="G5" s="34"/>
     </row>
-    <row r="6" spans="1:7" ht="23.45">
+    <row r="6" spans="1:7" ht="23.25">
       <c r="A6" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6" s="36" t="s">
+        <v>19</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D6" s="36" t="s">
         <v>20</v>
       </c>
-      <c r="B6" s="36" t="s">
+      <c r="E6" s="91" t="s">
         <v>21</v>
       </c>
-      <c r="C6" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="D6" s="36" t="s">
-        <v>22</v>
-      </c>
-      <c r="E6" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="F6" s="37" t="s">
-        <v>23</v>
-      </c>
+      <c r="F6" s="92"/>
       <c r="G6" s="34"/>
     </row>
     <row r="7" spans="1:7" ht="23.25">
       <c r="A7" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B7" s="36" t="s">
+        <v>23</v>
+      </c>
+      <c r="C7" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="B7" s="36" t="s">
+      <c r="D7" s="37" t="s">
         <v>25</v>
       </c>
-      <c r="C7" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="D7" s="37" t="s">
+      <c r="E7" s="91" t="s">
         <v>26</v>
       </c>
-      <c r="E7" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="F7" s="37" t="s">
-        <v>27</v>
-      </c>
+      <c r="F7" s="92"/>
       <c r="G7" s="34"/>
     </row>
     <row r="8" spans="1:7" ht="23.25">
       <c r="A8" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B8" s="37" t="s">
         <v>28</v>
       </c>
-      <c r="B8" s="37" t="s">
+      <c r="C8" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="C8" s="6" t="s">
+      <c r="D8" s="38" t="s">
         <v>30</v>
-      </c>
-      <c r="D8" s="38" t="s">
-        <v>31</v>
       </c>
       <c r="E8" s="34"/>
     </row>
     <row r="9" spans="1:7" ht="23.45">
       <c r="A9" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="B9" s="38" t="s">
         <v>32</v>
       </c>
-      <c r="B9" s="38" t="s">
+      <c r="C9" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="D9" s="38" t="s">
         <v>33</v>
-      </c>
-      <c r="C9" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="D9" s="38" t="s">
-        <v>34</v>
       </c>
       <c r="E9" s="34"/>
     </row>
     <row r="10" spans="1:7" ht="23.45">
       <c r="A10" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="B10" s="38" t="s">
         <v>35</v>
       </c>
-      <c r="B10" s="38" t="s">
+      <c r="C10" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="D10" s="38" t="s">
         <v>36</v>
-      </c>
-      <c r="C10" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="D10" s="38" t="s">
-        <v>37</v>
       </c>
       <c r="E10" s="34"/>
     </row>
     <row r="11" spans="1:7" ht="23.45">
       <c r="A11" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="B11" s="38" t="s">
         <v>38</v>
       </c>
-      <c r="B11" s="38" t="s">
+      <c r="C11" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="D11" s="38" t="s">
         <v>39</v>
-      </c>
-      <c r="C11" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="D11" s="38" t="s">
-        <v>40</v>
       </c>
       <c r="E11" s="34"/>
     </row>
@@ -6364,6 +6359,12 @@
       <c r="E20" s="34"/>
     </row>
   </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="E3:F3"/>
+  </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -6408,23 +6409,23 @@
       <c r="H1" s="30"/>
       <c r="I1" s="30"/>
       <c r="J1" s="30"/>
-      <c r="K1" s="85" t="s">
-        <v>41</v>
-      </c>
-      <c r="L1" s="86"/>
-      <c r="M1" s="86"/>
-      <c r="N1" s="86"/>
-      <c r="O1" s="86"/>
-      <c r="P1" s="86"/>
-      <c r="Q1" s="86"/>
-      <c r="R1" s="86"/>
-      <c r="S1" s="86"/>
-      <c r="T1" s="86"/>
-      <c r="U1" s="86"/>
-      <c r="V1" s="86"/>
-      <c r="W1" s="86"/>
-      <c r="X1" s="86"/>
-      <c r="Y1" s="86"/>
+      <c r="K1" s="70" t="s">
+        <v>40</v>
+      </c>
+      <c r="L1" s="71"/>
+      <c r="M1" s="71"/>
+      <c r="N1" s="71"/>
+      <c r="O1" s="71"/>
+      <c r="P1" s="71"/>
+      <c r="Q1" s="71"/>
+      <c r="R1" s="71"/>
+      <c r="S1" s="71"/>
+      <c r="T1" s="71"/>
+      <c r="U1" s="71"/>
+      <c r="V1" s="71"/>
+      <c r="W1" s="71"/>
+      <c r="X1" s="71"/>
+      <c r="Y1" s="71"/>
       <c r="Z1" s="29"/>
     </row>
     <row r="2" spans="1:26">
@@ -6433,24 +6434,24 @@
     </row>
     <row r="3" spans="1:26" ht="13.9" thickBot="1">
       <c r="A3" s="28"/>
-      <c r="K3" s="87" t="s">
+      <c r="K3" s="72" t="s">
+        <v>41</v>
+      </c>
+      <c r="L3" s="72"/>
+      <c r="M3" s="72"/>
+      <c r="N3" s="72"/>
+      <c r="O3" s="72"/>
+      <c r="P3" s="72"/>
+      <c r="Q3" s="72"/>
+      <c r="S3" s="72" t="s">
         <v>42</v>
       </c>
-      <c r="L3" s="87"/>
-      <c r="M3" s="87"/>
-      <c r="N3" s="87"/>
-      <c r="O3" s="87"/>
-      <c r="P3" s="87"/>
-      <c r="Q3" s="87"/>
-      <c r="S3" s="87" t="s">
-        <v>43</v>
-      </c>
-      <c r="T3" s="87"/>
-      <c r="U3" s="87"/>
-      <c r="V3" s="87"/>
-      <c r="W3" s="87"/>
-      <c r="X3" s="87"/>
-      <c r="Y3" s="87"/>
+      <c r="T3" s="72"/>
+      <c r="U3" s="72"/>
+      <c r="V3" s="72"/>
+      <c r="W3" s="72"/>
+      <c r="X3" s="72"/>
+      <c r="Y3" s="72"/>
       <c r="Z3" s="27"/>
     </row>
     <row r="4" spans="1:26" ht="13.9">
@@ -6464,25 +6465,25 @@
       <c r="H4" s="19"/>
       <c r="I4" s="19"/>
       <c r="J4" s="19"/>
-      <c r="K4" s="88" t="s">
+      <c r="K4" s="73" t="s">
+        <v>43</v>
+      </c>
+      <c r="L4" s="73"/>
+      <c r="M4" s="73"/>
+      <c r="N4" s="73"/>
+      <c r="O4" s="73"/>
+      <c r="P4" s="73"/>
+      <c r="Q4" s="73"/>
+      <c r="R4" s="20"/>
+      <c r="S4" s="73" t="s">
         <v>44</v>
       </c>
-      <c r="L4" s="88"/>
-      <c r="M4" s="88"/>
-      <c r="N4" s="88"/>
-      <c r="O4" s="88"/>
-      <c r="P4" s="88"/>
-      <c r="Q4" s="88"/>
-      <c r="R4" s="20"/>
-      <c r="S4" s="88" t="s">
-        <v>45</v>
-      </c>
-      <c r="T4" s="88"/>
-      <c r="U4" s="88"/>
-      <c r="V4" s="88"/>
-      <c r="W4" s="88"/>
-      <c r="X4" s="88"/>
-      <c r="Y4" s="88"/>
+      <c r="T4" s="73"/>
+      <c r="U4" s="73"/>
+      <c r="V4" s="73"/>
+      <c r="W4" s="73"/>
+      <c r="X4" s="73"/>
+      <c r="Y4" s="73"/>
       <c r="Z4" s="25"/>
     </row>
     <row r="5" spans="1:26" ht="15.6" thickBot="1">
@@ -6496,25 +6497,25 @@
       <c r="H5" s="19"/>
       <c r="I5" s="19"/>
       <c r="J5" s="19"/>
-      <c r="K5" s="89" t="s">
+      <c r="K5" s="74" t="s">
+        <v>45</v>
+      </c>
+      <c r="L5" s="74"/>
+      <c r="M5" s="74"/>
+      <c r="N5" s="74"/>
+      <c r="O5" s="74"/>
+      <c r="P5" s="74"/>
+      <c r="Q5" s="74"/>
+      <c r="R5" s="20"/>
+      <c r="S5" s="74" t="s">
         <v>46</v>
       </c>
-      <c r="L5" s="89"/>
-      <c r="M5" s="89"/>
-      <c r="N5" s="89"/>
-      <c r="O5" s="89"/>
-      <c r="P5" s="89"/>
-      <c r="Q5" s="89"/>
-      <c r="R5" s="20"/>
-      <c r="S5" s="89" t="s">
-        <v>47</v>
-      </c>
-      <c r="T5" s="89"/>
-      <c r="U5" s="89"/>
-      <c r="V5" s="89"/>
-      <c r="W5" s="89"/>
-      <c r="X5" s="89"/>
-      <c r="Y5" s="89"/>
+      <c r="T5" s="74"/>
+      <c r="U5" s="74"/>
+      <c r="V5" s="74"/>
+      <c r="W5" s="74"/>
+      <c r="X5" s="74"/>
+      <c r="Y5" s="74"/>
       <c r="Z5" s="25"/>
     </row>
     <row r="6" spans="1:26">
@@ -6528,25 +6529,25 @@
       <c r="H6" s="19"/>
       <c r="I6" s="19"/>
       <c r="J6" s="19"/>
-      <c r="K6" s="90" t="s">
+      <c r="K6" s="75" t="s">
+        <v>47</v>
+      </c>
+      <c r="L6" s="75"/>
+      <c r="M6" s="75"/>
+      <c r="N6" s="75"/>
+      <c r="O6" s="75"/>
+      <c r="P6" s="75"/>
+      <c r="Q6" s="75"/>
+      <c r="R6" s="20"/>
+      <c r="S6" s="75" t="s">
         <v>48</v>
       </c>
-      <c r="L6" s="90"/>
-      <c r="M6" s="90"/>
-      <c r="N6" s="90"/>
-      <c r="O6" s="90"/>
-      <c r="P6" s="90"/>
-      <c r="Q6" s="90"/>
-      <c r="R6" s="20"/>
-      <c r="S6" s="90" t="s">
-        <v>49</v>
-      </c>
-      <c r="T6" s="90"/>
-      <c r="U6" s="90"/>
-      <c r="V6" s="90"/>
-      <c r="W6" s="90"/>
-      <c r="X6" s="90"/>
-      <c r="Y6" s="90"/>
+      <c r="T6" s="75"/>
+      <c r="U6" s="75"/>
+      <c r="V6" s="75"/>
+      <c r="W6" s="75"/>
+      <c r="X6" s="75"/>
+      <c r="Y6" s="75"/>
       <c r="Z6" s="25"/>
     </row>
     <row r="7" spans="1:26" ht="13.9" thickBot="1">
@@ -6561,18 +6562,18 @@
       <c r="I7" s="19"/>
       <c r="J7" s="19"/>
       <c r="K7" s="20"/>
-      <c r="L7" s="79" t="s">
+      <c r="L7" s="81" t="s">
+        <v>49</v>
+      </c>
+      <c r="M7" s="80"/>
+      <c r="N7" s="80"/>
+      <c r="O7" s="82"/>
+      <c r="P7" s="20"/>
+      <c r="Q7" s="79" t="s">
         <v>50</v>
       </c>
-      <c r="M7" s="63"/>
-      <c r="N7" s="63"/>
-      <c r="O7" s="62"/>
-      <c r="P7" s="20"/>
-      <c r="Q7" s="61" t="s">
-        <v>51</v>
-      </c>
-      <c r="R7" s="63"/>
-      <c r="S7" s="62"/>
+      <c r="R7" s="80"/>
+      <c r="S7" s="82"/>
       <c r="T7" s="20"/>
       <c r="U7" s="20"/>
       <c r="V7" s="20"/>
@@ -6582,33 +6583,33 @@
       <c r="Z7" s="25"/>
     </row>
     <row r="8" spans="1:26" ht="16.149999999999999" thickBot="1">
-      <c r="A8" s="69" t="s">
-        <v>44</v>
-      </c>
-      <c r="B8" s="70"/>
-      <c r="C8" s="70"/>
-      <c r="D8" s="71" t="s">
+      <c r="A8" s="58" t="s">
+        <v>43</v>
+      </c>
+      <c r="B8" s="59"/>
+      <c r="C8" s="59"/>
+      <c r="D8" s="60" t="s">
+        <v>51</v>
+      </c>
+      <c r="E8" s="61"/>
+      <c r="F8" s="61"/>
+      <c r="G8" s="61"/>
+      <c r="H8" s="61"/>
+      <c r="I8" s="61"/>
+      <c r="J8" s="62"/>
+      <c r="K8" s="20"/>
+      <c r="L8" s="63" t="s">
         <v>52</v>
       </c>
-      <c r="E8" s="72"/>
-      <c r="F8" s="72"/>
-      <c r="G8" s="72"/>
-      <c r="H8" s="72"/>
-      <c r="I8" s="72"/>
-      <c r="J8" s="80"/>
-      <c r="K8" s="20"/>
-      <c r="L8" s="81" t="s">
+      <c r="M8" s="63"/>
+      <c r="N8" s="63"/>
+      <c r="O8" s="63"/>
+      <c r="P8" s="20"/>
+      <c r="Q8" s="63" t="s">
         <v>53</v>
       </c>
-      <c r="M8" s="81"/>
-      <c r="N8" s="81"/>
-      <c r="O8" s="81"/>
-      <c r="P8" s="20"/>
-      <c r="Q8" s="81" t="s">
-        <v>54</v>
-      </c>
-      <c r="R8" s="81"/>
-      <c r="S8" s="81"/>
+      <c r="R8" s="63"/>
+      <c r="S8" s="63"/>
       <c r="T8" s="20"/>
       <c r="U8" s="26"/>
       <c r="V8" s="20"/>
@@ -6618,46 +6619,46 @@
       <c r="Z8" s="25"/>
     </row>
     <row r="9" spans="1:26" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A9" s="76" t="s">
+      <c r="A9" s="68" t="s">
+        <v>54</v>
+      </c>
+      <c r="B9" s="69"/>
+      <c r="C9" s="69"/>
+      <c r="D9" s="69"/>
+      <c r="E9" s="67" t="s">
         <v>55</v>
       </c>
-      <c r="B9" s="77"/>
-      <c r="C9" s="77"/>
-      <c r="D9" s="77"/>
-      <c r="E9" s="73" t="s">
+      <c r="F9" s="67"/>
+      <c r="G9" s="67"/>
+      <c r="H9" s="67"/>
+      <c r="I9" s="67"/>
+      <c r="J9" s="40"/>
+      <c r="K9" s="64" t="s">
         <v>56</v>
       </c>
-      <c r="F9" s="73"/>
-      <c r="G9" s="73"/>
-      <c r="H9" s="73"/>
-      <c r="I9" s="73"/>
-      <c r="J9" s="40"/>
-      <c r="K9" s="82" t="s">
-        <v>57</v>
-      </c>
-      <c r="L9" s="83"/>
-      <c r="M9" s="83"/>
-      <c r="N9" s="83"/>
-      <c r="O9" s="83"/>
-      <c r="P9" s="83"/>
-      <c r="Q9" s="83"/>
-      <c r="R9" s="83"/>
-      <c r="S9" s="83"/>
-      <c r="T9" s="83"/>
-      <c r="U9" s="83"/>
-      <c r="V9" s="83"/>
-      <c r="W9" s="83"/>
-      <c r="X9" s="83"/>
-      <c r="Y9" s="83"/>
-      <c r="Z9" s="84"/>
+      <c r="L9" s="65"/>
+      <c r="M9" s="65"/>
+      <c r="N9" s="65"/>
+      <c r="O9" s="65"/>
+      <c r="P9" s="65"/>
+      <c r="Q9" s="65"/>
+      <c r="R9" s="65"/>
+      <c r="S9" s="65"/>
+      <c r="T9" s="65"/>
+      <c r="U9" s="65"/>
+      <c r="V9" s="65"/>
+      <c r="W9" s="65"/>
+      <c r="X9" s="65"/>
+      <c r="Y9" s="65"/>
+      <c r="Z9" s="66"/>
     </row>
     <row r="10" spans="1:26" ht="15.75" customHeight="1" thickBot="1">
       <c r="A10" s="21"/>
-      <c r="B10" s="61"/>
-      <c r="C10" s="62"/>
+      <c r="B10" s="79"/>
+      <c r="C10" s="82"/>
       <c r="D10" s="19"/>
       <c r="E10" s="39" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F10" s="41">
         <v>1</v>
@@ -6672,43 +6673,43 @@
         <v>4</v>
       </c>
       <c r="J10" s="19"/>
-      <c r="K10" s="74" t="s">
+      <c r="K10" s="78" t="s">
+        <v>58</v>
+      </c>
+      <c r="L10" s="76"/>
+      <c r="M10" s="76" t="s">
         <v>59</v>
       </c>
-      <c r="L10" s="75"/>
-      <c r="M10" s="75" t="s">
-        <v>60</v>
-      </c>
-      <c r="N10" s="78"/>
-      <c r="O10" s="74" t="s">
+      <c r="N10" s="77"/>
+      <c r="O10" s="78" t="s">
+        <v>58</v>
+      </c>
+      <c r="P10" s="76"/>
+      <c r="Q10" s="76" t="s">
         <v>59</v>
       </c>
-      <c r="P10" s="75"/>
-      <c r="Q10" s="75" t="s">
-        <v>60</v>
-      </c>
-      <c r="R10" s="78"/>
-      <c r="S10" s="74" t="s">
+      <c r="R10" s="77"/>
+      <c r="S10" s="78" t="s">
+        <v>58</v>
+      </c>
+      <c r="T10" s="76"/>
+      <c r="U10" s="76" t="s">
         <v>59</v>
       </c>
-      <c r="T10" s="75"/>
-      <c r="U10" s="75" t="s">
-        <v>60</v>
-      </c>
-      <c r="V10" s="78"/>
-      <c r="W10" s="74" t="s">
+      <c r="V10" s="77"/>
+      <c r="W10" s="78" t="s">
+        <v>58</v>
+      </c>
+      <c r="X10" s="76"/>
+      <c r="Y10" s="76" t="s">
         <v>59</v>
       </c>
-      <c r="X10" s="75"/>
-      <c r="Y10" s="75" t="s">
-        <v>60</v>
-      </c>
-      <c r="Z10" s="78"/>
+      <c r="Z10" s="77"/>
     </row>
     <row r="11" spans="1:26" ht="13.9" thickBot="1">
       <c r="A11" s="21"/>
-      <c r="B11" s="61"/>
-      <c r="C11" s="62"/>
+      <c r="B11" s="79"/>
+      <c r="C11" s="82"/>
       <c r="D11" s="20"/>
       <c r="E11" s="20"/>
       <c r="F11" s="44">
@@ -6759,11 +6760,11 @@
     </row>
     <row r="12" spans="1:26" ht="15.75" customHeight="1" thickBot="1">
       <c r="A12" s="21"/>
-      <c r="B12" s="61"/>
-      <c r="C12" s="62"/>
+      <c r="B12" s="79"/>
+      <c r="C12" s="82"/>
       <c r="D12" s="19"/>
       <c r="E12" s="39" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F12" s="47">
         <v>1</v>
@@ -6813,8 +6814,8 @@
     </row>
     <row r="13" spans="1:26" ht="13.9" thickBot="1">
       <c r="A13" s="21"/>
-      <c r="B13" s="61"/>
-      <c r="C13" s="62"/>
+      <c r="B13" s="79"/>
+      <c r="C13" s="82"/>
       <c r="D13" s="20"/>
       <c r="E13" s="20"/>
       <c r="F13" s="41">
@@ -6865,11 +6866,11 @@
     </row>
     <row r="14" spans="1:26" ht="15" customHeight="1">
       <c r="A14" s="21"/>
-      <c r="B14" s="61"/>
-      <c r="C14" s="62"/>
+      <c r="B14" s="79"/>
+      <c r="C14" s="82"/>
       <c r="D14" s="11"/>
       <c r="E14" s="19" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F14" s="20"/>
       <c r="G14" s="19"/>
@@ -6910,18 +6911,18 @@
       <c r="Z14" s="15"/>
     </row>
     <row r="15" spans="1:26">
-      <c r="A15" s="61"/>
-      <c r="B15" s="63"/>
-      <c r="C15" s="62"/>
+      <c r="A15" s="79"/>
+      <c r="B15" s="80"/>
+      <c r="C15" s="82"/>
       <c r="D15" s="19"/>
       <c r="E15" s="19"/>
-      <c r="F15" s="61" t="s">
-        <v>63</v>
-      </c>
-      <c r="G15" s="63"/>
-      <c r="H15" s="63"/>
-      <c r="I15" s="63"/>
-      <c r="J15" s="63"/>
+      <c r="F15" s="79" t="s">
+        <v>62</v>
+      </c>
+      <c r="G15" s="80"/>
+      <c r="H15" s="80"/>
+      <c r="I15" s="80"/>
+      <c r="J15" s="80"/>
       <c r="K15" s="16"/>
       <c r="L15" s="22">
         <v>5</v>
@@ -6956,15 +6957,15 @@
       <c r="Z15" s="15"/>
     </row>
     <row r="16" spans="1:26">
-      <c r="A16" s="61" t="s">
+      <c r="A16" s="79" t="s">
+        <v>63</v>
+      </c>
+      <c r="B16" s="80"/>
+      <c r="C16" s="82"/>
+      <c r="D16" s="84" t="s">
         <v>64</v>
       </c>
-      <c r="B16" s="63"/>
-      <c r="C16" s="62"/>
-      <c r="D16" s="67" t="s">
-        <v>65</v>
-      </c>
-      <c r="E16" s="68"/>
+      <c r="E16" s="85"/>
       <c r="F16" s="50">
         <v>1</v>
       </c>
@@ -7014,14 +7015,14 @@
       <c r="Z16" s="15"/>
     </row>
     <row r="17" spans="1:26">
-      <c r="A17" s="64" t="s">
+      <c r="A17" s="83" t="s">
+        <v>65</v>
+      </c>
+      <c r="B17" s="82"/>
+      <c r="C17" s="79"/>
+      <c r="D17" s="82"/>
+      <c r="E17" s="18" t="s">
         <v>66</v>
-      </c>
-      <c r="B17" s="62"/>
-      <c r="C17" s="61"/>
-      <c r="D17" s="62"/>
-      <c r="E17" s="18" t="s">
-        <v>67</v>
       </c>
       <c r="F17" s="11"/>
       <c r="G17" s="11"/>
@@ -7062,10 +7063,10 @@
       <c r="Z17" s="15"/>
     </row>
     <row r="18" spans="1:26">
-      <c r="A18" s="64"/>
-      <c r="B18" s="62"/>
-      <c r="C18" s="61"/>
-      <c r="D18" s="62"/>
+      <c r="A18" s="83"/>
+      <c r="B18" s="82"/>
+      <c r="C18" s="79"/>
+      <c r="D18" s="82"/>
       <c r="E18" s="18"/>
       <c r="F18" s="18"/>
       <c r="G18" s="11"/>
@@ -7106,10 +7107,10 @@
       <c r="Z18" s="15"/>
     </row>
     <row r="19" spans="1:26">
-      <c r="A19" s="64"/>
-      <c r="B19" s="62"/>
-      <c r="C19" s="61"/>
-      <c r="D19" s="62"/>
+      <c r="A19" s="83"/>
+      <c r="B19" s="82"/>
+      <c r="C19" s="79"/>
+      <c r="D19" s="82"/>
       <c r="E19" s="18"/>
       <c r="F19" s="18"/>
       <c r="G19" s="11"/>
@@ -7150,10 +7151,10 @@
       <c r="Z19" s="15"/>
     </row>
     <row r="20" spans="1:26">
-      <c r="A20" s="64"/>
-      <c r="B20" s="62"/>
-      <c r="C20" s="61"/>
-      <c r="D20" s="62"/>
+      <c r="A20" s="83"/>
+      <c r="B20" s="82"/>
+      <c r="C20" s="79"/>
+      <c r="D20" s="82"/>
       <c r="E20" s="18"/>
       <c r="F20" s="18"/>
       <c r="G20" s="11"/>
@@ -7194,10 +7195,10 @@
       <c r="Z20" s="15"/>
     </row>
     <row r="21" spans="1:26">
-      <c r="A21" s="64"/>
-      <c r="B21" s="62"/>
-      <c r="C21" s="61"/>
-      <c r="D21" s="62"/>
+      <c r="A21" s="83"/>
+      <c r="B21" s="82"/>
+      <c r="C21" s="79"/>
+      <c r="D21" s="82"/>
       <c r="E21" s="18"/>
       <c r="F21" s="18"/>
       <c r="G21" s="11"/>
@@ -7238,10 +7239,10 @@
       <c r="Z21" s="15"/>
     </row>
     <row r="22" spans="1:26">
-      <c r="A22" s="64"/>
-      <c r="B22" s="62"/>
-      <c r="C22" s="61"/>
-      <c r="D22" s="62"/>
+      <c r="A22" s="83"/>
+      <c r="B22" s="82"/>
+      <c r="C22" s="79"/>
+      <c r="D22" s="82"/>
       <c r="E22" s="18"/>
       <c r="F22" s="18"/>
       <c r="G22" s="11"/>
@@ -7282,10 +7283,10 @@
       <c r="Z22" s="15"/>
     </row>
     <row r="23" spans="1:26">
-      <c r="A23" s="64"/>
-      <c r="B23" s="62"/>
-      <c r="C23" s="61"/>
-      <c r="D23" s="62"/>
+      <c r="A23" s="83"/>
+      <c r="B23" s="82"/>
+      <c r="C23" s="79"/>
+      <c r="D23" s="82"/>
       <c r="E23" s="18"/>
       <c r="F23" s="18"/>
       <c r="G23" s="11"/>
@@ -7326,10 +7327,10 @@
       <c r="Z23" s="15"/>
     </row>
     <row r="24" spans="1:26">
-      <c r="A24" s="64"/>
-      <c r="B24" s="62"/>
-      <c r="C24" s="61"/>
-      <c r="D24" s="62"/>
+      <c r="A24" s="83"/>
+      <c r="B24" s="82"/>
+      <c r="C24" s="79"/>
+      <c r="D24" s="82"/>
       <c r="E24" s="18"/>
       <c r="F24" s="18"/>
       <c r="G24" s="11"/>
@@ -7370,10 +7371,10 @@
       <c r="Z24" s="15"/>
     </row>
     <row r="25" spans="1:26">
-      <c r="A25" s="64"/>
-      <c r="B25" s="62"/>
-      <c r="C25" s="61"/>
-      <c r="D25" s="62"/>
+      <c r="A25" s="83"/>
+      <c r="B25" s="82"/>
+      <c r="C25" s="79"/>
+      <c r="D25" s="82"/>
       <c r="E25" s="18"/>
       <c r="F25" s="18"/>
       <c r="G25" s="11"/>
@@ -7414,10 +7415,10 @@
       <c r="Z25" s="15"/>
     </row>
     <row r="26" spans="1:26">
-      <c r="A26" s="64"/>
-      <c r="B26" s="62"/>
-      <c r="C26" s="61"/>
-      <c r="D26" s="62"/>
+      <c r="A26" s="83"/>
+      <c r="B26" s="82"/>
+      <c r="C26" s="79"/>
+      <c r="D26" s="82"/>
       <c r="E26" s="18"/>
       <c r="F26" s="18"/>
       <c r="G26" s="11"/>
@@ -7458,10 +7459,10 @@
       <c r="Z26" s="15"/>
     </row>
     <row r="27" spans="1:26">
-      <c r="A27" s="64"/>
-      <c r="B27" s="62"/>
-      <c r="C27" s="61"/>
-      <c r="D27" s="62"/>
+      <c r="A27" s="83"/>
+      <c r="B27" s="82"/>
+      <c r="C27" s="79"/>
+      <c r="D27" s="82"/>
       <c r="E27" s="18"/>
       <c r="F27" s="18"/>
       <c r="G27" s="11"/>
@@ -7502,10 +7503,10 @@
       <c r="Z27" s="15"/>
     </row>
     <row r="28" spans="1:26" ht="13.9" thickBot="1">
-      <c r="A28" s="64"/>
-      <c r="B28" s="62"/>
-      <c r="C28" s="61"/>
-      <c r="D28" s="62"/>
+      <c r="A28" s="83"/>
+      <c r="B28" s="82"/>
+      <c r="C28" s="79"/>
+      <c r="D28" s="82"/>
       <c r="E28" s="18"/>
       <c r="F28" s="18"/>
       <c r="G28" s="11"/>
@@ -7546,20 +7547,20 @@
       <c r="Z28" s="15"/>
     </row>
     <row r="29" spans="1:26" ht="16.149999999999999" thickBot="1">
-      <c r="A29" s="69" t="s">
-        <v>45</v>
-      </c>
-      <c r="B29" s="70"/>
-      <c r="C29" s="70"/>
-      <c r="D29" s="71" t="s">
-        <v>68</v>
-      </c>
-      <c r="E29" s="72"/>
-      <c r="F29" s="72"/>
-      <c r="G29" s="72"/>
-      <c r="H29" s="72"/>
-      <c r="I29" s="72"/>
-      <c r="J29" s="72"/>
+      <c r="A29" s="58" t="s">
+        <v>44</v>
+      </c>
+      <c r="B29" s="59"/>
+      <c r="C29" s="59"/>
+      <c r="D29" s="60" t="s">
+        <v>67</v>
+      </c>
+      <c r="E29" s="61"/>
+      <c r="F29" s="61"/>
+      <c r="G29" s="61"/>
+      <c r="H29" s="61"/>
+      <c r="I29" s="61"/>
+      <c r="J29" s="61"/>
       <c r="K29" s="16"/>
       <c r="L29" s="22">
         <v>19</v>
@@ -7594,19 +7595,19 @@
       <c r="Z29" s="15"/>
     </row>
     <row r="30" spans="1:26" ht="13.9" thickBot="1">
-      <c r="A30" s="76" t="s">
+      <c r="A30" s="68" t="s">
+        <v>54</v>
+      </c>
+      <c r="B30" s="69"/>
+      <c r="C30" s="69"/>
+      <c r="D30" s="69"/>
+      <c r="E30" s="67" t="s">
         <v>55</v>
       </c>
-      <c r="B30" s="77"/>
-      <c r="C30" s="77"/>
-      <c r="D30" s="77"/>
-      <c r="E30" s="73" t="s">
-        <v>56</v>
-      </c>
-      <c r="F30" s="73"/>
-      <c r="G30" s="73"/>
-      <c r="H30" s="73"/>
-      <c r="I30" s="73"/>
+      <c r="F30" s="67"/>
+      <c r="G30" s="67"/>
+      <c r="H30" s="67"/>
+      <c r="I30" s="67"/>
       <c r="J30" s="40"/>
       <c r="K30" s="16"/>
       <c r="L30" s="22">
@@ -7643,11 +7644,11 @@
     </row>
     <row r="31" spans="1:26" ht="13.9" thickBot="1">
       <c r="A31" s="21"/>
-      <c r="B31" s="61"/>
-      <c r="C31" s="62"/>
+      <c r="B31" s="79"/>
+      <c r="C31" s="82"/>
       <c r="D31" s="19"/>
       <c r="E31" s="39" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F31" s="41">
         <v>1</v>
@@ -7697,8 +7698,8 @@
     </row>
     <row r="32" spans="1:26" ht="13.9" thickBot="1">
       <c r="A32" s="21"/>
-      <c r="B32" s="61"/>
-      <c r="C32" s="62"/>
+      <c r="B32" s="79"/>
+      <c r="C32" s="82"/>
       <c r="D32" s="20"/>
       <c r="E32" s="20"/>
       <c r="F32" s="44">
@@ -7749,11 +7750,11 @@
     </row>
     <row r="33" spans="1:26" ht="13.9" thickBot="1">
       <c r="A33" s="21"/>
-      <c r="B33" s="61"/>
-      <c r="C33" s="62"/>
+      <c r="B33" s="79"/>
+      <c r="C33" s="82"/>
       <c r="D33" s="19"/>
       <c r="E33" s="39" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F33" s="47">
         <v>1</v>
@@ -7803,8 +7804,8 @@
     </row>
     <row r="34" spans="1:26" ht="13.9" thickBot="1">
       <c r="A34" s="21"/>
-      <c r="B34" s="61"/>
-      <c r="C34" s="62"/>
+      <c r="B34" s="79"/>
+      <c r="C34" s="82"/>
       <c r="D34" s="20"/>
       <c r="E34" s="20"/>
       <c r="F34" s="41">
@@ -7855,11 +7856,11 @@
     </row>
     <row r="35" spans="1:26">
       <c r="A35" s="21"/>
-      <c r="B35" s="61"/>
-      <c r="C35" s="62"/>
+      <c r="B35" s="79"/>
+      <c r="C35" s="82"/>
       <c r="D35" s="11"/>
       <c r="E35" s="19" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F35" s="20"/>
       <c r="G35" s="19"/>
@@ -7900,18 +7901,18 @@
       <c r="Z35" s="15"/>
     </row>
     <row r="36" spans="1:26">
-      <c r="A36" s="61"/>
-      <c r="B36" s="63"/>
-      <c r="C36" s="62"/>
+      <c r="A36" s="79"/>
+      <c r="B36" s="80"/>
+      <c r="C36" s="82"/>
       <c r="D36" s="19"/>
       <c r="E36" s="19"/>
-      <c r="F36" s="61" t="s">
-        <v>63</v>
-      </c>
-      <c r="G36" s="63"/>
-      <c r="H36" s="63"/>
-      <c r="I36" s="63"/>
-      <c r="J36" s="63"/>
+      <c r="F36" s="79" t="s">
+        <v>62</v>
+      </c>
+      <c r="G36" s="80"/>
+      <c r="H36" s="80"/>
+      <c r="I36" s="80"/>
+      <c r="J36" s="80"/>
       <c r="K36" s="16"/>
       <c r="L36" s="22">
         <v>26</v>
@@ -7946,15 +7947,15 @@
       <c r="Z36" s="15"/>
     </row>
     <row r="37" spans="1:26">
-      <c r="A37" s="61" t="s">
+      <c r="A37" s="79" t="s">
+        <v>63</v>
+      </c>
+      <c r="B37" s="80"/>
+      <c r="C37" s="82"/>
+      <c r="D37" s="84" t="s">
         <v>64</v>
       </c>
-      <c r="B37" s="63"/>
-      <c r="C37" s="62"/>
-      <c r="D37" s="67" t="s">
-        <v>65</v>
-      </c>
-      <c r="E37" s="68"/>
+      <c r="E37" s="85"/>
       <c r="F37" s="50">
         <v>1</v>
       </c>
@@ -8004,14 +8005,14 @@
       <c r="Z37" s="15"/>
     </row>
     <row r="38" spans="1:26">
-      <c r="A38" s="64" t="s">
+      <c r="A38" s="83" t="s">
+        <v>68</v>
+      </c>
+      <c r="B38" s="82"/>
+      <c r="C38" s="79"/>
+      <c r="D38" s="82"/>
+      <c r="E38" s="18" t="s">
         <v>69</v>
-      </c>
-      <c r="B38" s="62"/>
-      <c r="C38" s="61"/>
-      <c r="D38" s="62"/>
-      <c r="E38" s="18" t="s">
-        <v>70</v>
       </c>
       <c r="F38" s="18"/>
       <c r="G38" s="11"/>
@@ -8052,10 +8053,10 @@
       <c r="Z38" s="15"/>
     </row>
     <row r="39" spans="1:26">
-      <c r="A39" s="64"/>
-      <c r="B39" s="62"/>
-      <c r="C39" s="61"/>
-      <c r="D39" s="62"/>
+      <c r="A39" s="83"/>
+      <c r="B39" s="82"/>
+      <c r="C39" s="79"/>
+      <c r="D39" s="82"/>
       <c r="E39" s="18"/>
       <c r="F39" s="18"/>
       <c r="G39" s="11"/>
@@ -8096,10 +8097,10 @@
       <c r="Z39" s="15"/>
     </row>
     <row r="40" spans="1:26">
-      <c r="A40" s="64"/>
-      <c r="B40" s="62"/>
-      <c r="C40" s="61"/>
-      <c r="D40" s="62"/>
+      <c r="A40" s="83"/>
+      <c r="B40" s="82"/>
+      <c r="C40" s="79"/>
+      <c r="D40" s="82"/>
       <c r="E40" s="18"/>
       <c r="F40" s="18"/>
       <c r="G40" s="11"/>
@@ -8140,10 +8141,10 @@
       <c r="Z40" s="15"/>
     </row>
     <row r="41" spans="1:26">
-      <c r="A41" s="64"/>
-      <c r="B41" s="62"/>
-      <c r="C41" s="61"/>
-      <c r="D41" s="62"/>
+      <c r="A41" s="83"/>
+      <c r="B41" s="82"/>
+      <c r="C41" s="79"/>
+      <c r="D41" s="82"/>
       <c r="E41" s="18"/>
       <c r="F41" s="18"/>
       <c r="G41" s="11"/>
@@ -8184,10 +8185,10 @@
       <c r="Z41" s="15"/>
     </row>
     <row r="42" spans="1:26">
-      <c r="A42" s="64"/>
-      <c r="B42" s="62"/>
-      <c r="C42" s="61"/>
-      <c r="D42" s="62"/>
+      <c r="A42" s="83"/>
+      <c r="B42" s="82"/>
+      <c r="C42" s="79"/>
+      <c r="D42" s="82"/>
       <c r="E42" s="18"/>
       <c r="F42" s="18"/>
       <c r="G42" s="11"/>
@@ -8228,10 +8229,10 @@
       <c r="Z42" s="15"/>
     </row>
     <row r="43" spans="1:26">
-      <c r="A43" s="64"/>
-      <c r="B43" s="62"/>
-      <c r="C43" s="61"/>
-      <c r="D43" s="62"/>
+      <c r="A43" s="83"/>
+      <c r="B43" s="82"/>
+      <c r="C43" s="79"/>
+      <c r="D43" s="82"/>
       <c r="E43" s="18"/>
       <c r="F43" s="18"/>
       <c r="G43" s="11"/>
@@ -8272,10 +8273,10 @@
       <c r="Z43" s="15"/>
     </row>
     <row r="44" spans="1:26">
-      <c r="A44" s="64"/>
-      <c r="B44" s="62"/>
-      <c r="C44" s="61"/>
-      <c r="D44" s="62"/>
+      <c r="A44" s="83"/>
+      <c r="B44" s="82"/>
+      <c r="C44" s="79"/>
+      <c r="D44" s="82"/>
       <c r="E44" s="18"/>
       <c r="F44" s="18"/>
       <c r="G44" s="11"/>
@@ -8316,10 +8317,10 @@
       <c r="Z44" s="15"/>
     </row>
     <row r="45" spans="1:26">
-      <c r="A45" s="64"/>
-      <c r="B45" s="62"/>
-      <c r="C45" s="61"/>
-      <c r="D45" s="62"/>
+      <c r="A45" s="83"/>
+      <c r="B45" s="82"/>
+      <c r="C45" s="79"/>
+      <c r="D45" s="82"/>
       <c r="E45" s="18"/>
       <c r="F45" s="18"/>
       <c r="G45" s="11"/>
@@ -8360,10 +8361,10 @@
       <c r="Z45" s="15"/>
     </row>
     <row r="46" spans="1:26">
-      <c r="A46" s="64"/>
-      <c r="B46" s="62"/>
-      <c r="C46" s="61"/>
-      <c r="D46" s="62"/>
+      <c r="A46" s="83"/>
+      <c r="B46" s="82"/>
+      <c r="C46" s="79"/>
+      <c r="D46" s="82"/>
       <c r="E46" s="18"/>
       <c r="F46" s="18"/>
       <c r="G46" s="11"/>
@@ -8404,10 +8405,10 @@
       <c r="Z46" s="15"/>
     </row>
     <row r="47" spans="1:26">
-      <c r="A47" s="64"/>
-      <c r="B47" s="62"/>
-      <c r="C47" s="61"/>
-      <c r="D47" s="62"/>
+      <c r="A47" s="83"/>
+      <c r="B47" s="82"/>
+      <c r="C47" s="79"/>
+      <c r="D47" s="82"/>
       <c r="E47" s="18"/>
       <c r="F47" s="18"/>
       <c r="G47" s="11"/>
@@ -8448,10 +8449,10 @@
       <c r="Z47" s="15"/>
     </row>
     <row r="48" spans="1:26">
-      <c r="A48" s="64"/>
-      <c r="B48" s="62"/>
-      <c r="C48" s="61"/>
-      <c r="D48" s="62"/>
+      <c r="A48" s="83"/>
+      <c r="B48" s="82"/>
+      <c r="C48" s="79"/>
+      <c r="D48" s="82"/>
       <c r="E48" s="18"/>
       <c r="F48" s="18"/>
       <c r="G48" s="11"/>
@@ -8492,10 +8493,10 @@
       <c r="Z48" s="15"/>
     </row>
     <row r="49" spans="1:26">
-      <c r="A49" s="64"/>
-      <c r="B49" s="62"/>
-      <c r="C49" s="61"/>
-      <c r="D49" s="62"/>
+      <c r="A49" s="83"/>
+      <c r="B49" s="82"/>
+      <c r="C49" s="79"/>
+      <c r="D49" s="82"/>
       <c r="E49" s="18"/>
       <c r="F49" s="18"/>
       <c r="G49" s="11"/>
@@ -8536,12 +8537,12 @@
       <c r="Z49" s="15"/>
     </row>
     <row r="50" spans="1:26" ht="15" customHeight="1">
-      <c r="A50" s="58" t="s">
-        <v>71</v>
-      </c>
-      <c r="B50" s="59"/>
-      <c r="C50" s="59"/>
-      <c r="D50" s="60"/>
+      <c r="A50" s="88" t="s">
+        <v>70</v>
+      </c>
+      <c r="B50" s="89"/>
+      <c r="C50" s="89"/>
+      <c r="D50" s="90"/>
       <c r="E50" s="14"/>
       <c r="F50" s="14"/>
       <c r="G50" s="14"/>
@@ -8582,22 +8583,22 @@
       <c r="Z50" s="12"/>
     </row>
     <row r="51" spans="1:26" ht="15" customHeight="1">
-      <c r="A51" s="61" t="s">
+      <c r="A51" s="79" t="s">
+        <v>57</v>
+      </c>
+      <c r="B51" s="80"/>
+      <c r="C51" s="80"/>
+      <c r="D51" s="82"/>
+      <c r="E51" s="57" t="s">
         <v>58</v>
       </c>
-      <c r="B51" s="63"/>
-      <c r="C51" s="63"/>
-      <c r="D51" s="62"/>
-      <c r="E51" s="57" t="s">
+      <c r="F51" s="86"/>
+      <c r="G51" s="86"/>
+      <c r="H51" s="56" t="s">
         <v>59</v>
       </c>
-      <c r="F51" s="65"/>
-      <c r="G51" s="65"/>
-      <c r="H51" s="56" t="s">
-        <v>60</v>
-      </c>
-      <c r="I51" s="65"/>
-      <c r="J51" s="65"/>
+      <c r="I51" s="86"/>
+      <c r="J51" s="86"/>
       <c r="K51" s="10"/>
       <c r="L51" s="10"/>
       <c r="M51" s="10"/>
@@ -8616,79 +8617,79 @@
       <c r="Z51" s="10"/>
     </row>
     <row r="52" spans="1:26" ht="15" customHeight="1">
-      <c r="A52" s="61" t="s">
-        <v>61</v>
-      </c>
-      <c r="B52" s="63"/>
-      <c r="C52" s="63"/>
-      <c r="D52" s="62"/>
+      <c r="A52" s="79" t="s">
+        <v>60</v>
+      </c>
+      <c r="B52" s="80"/>
+      <c r="C52" s="80"/>
+      <c r="D52" s="82"/>
       <c r="E52" s="57" t="s">
+        <v>58</v>
+      </c>
+      <c r="F52" s="86"/>
+      <c r="G52" s="86"/>
+      <c r="H52" s="56" t="s">
         <v>59</v>
       </c>
-      <c r="F52" s="65"/>
-      <c r="G52" s="65"/>
-      <c r="H52" s="56" t="s">
-        <v>60</v>
-      </c>
-      <c r="I52" s="65"/>
-      <c r="J52" s="65"/>
-      <c r="K52" s="58" t="s">
-        <v>72</v>
-      </c>
-      <c r="L52" s="59"/>
-      <c r="M52" s="59"/>
-      <c r="N52" s="59"/>
-      <c r="O52" s="60"/>
-      <c r="P52" s="65" t="s">
+      <c r="I52" s="86"/>
+      <c r="J52" s="86"/>
+      <c r="K52" s="88" t="s">
+        <v>71</v>
+      </c>
+      <c r="L52" s="89"/>
+      <c r="M52" s="89"/>
+      <c r="N52" s="89"/>
+      <c r="O52" s="90"/>
+      <c r="P52" s="86" t="s">
+        <v>43</v>
+      </c>
+      <c r="Q52" s="86"/>
+      <c r="R52" s="86"/>
+      <c r="S52" s="86"/>
+      <c r="T52" s="86"/>
+      <c r="U52" s="86" t="s">
         <v>44</v>
       </c>
-      <c r="Q52" s="65"/>
-      <c r="R52" s="65"/>
-      <c r="S52" s="65"/>
-      <c r="T52" s="65"/>
-      <c r="U52" s="65" t="s">
-        <v>45</v>
-      </c>
-      <c r="V52" s="65"/>
-      <c r="W52" s="65"/>
-      <c r="X52" s="65"/>
-      <c r="Y52" s="65"/>
+      <c r="V52" s="86"/>
+      <c r="W52" s="86"/>
+      <c r="X52" s="86"/>
+      <c r="Y52" s="86"/>
       <c r="Z52" s="10"/>
     </row>
     <row r="53" spans="1:26" ht="15" customHeight="1">
-      <c r="A53" s="58" t="s">
+      <c r="A53" s="88" t="s">
+        <v>72</v>
+      </c>
+      <c r="B53" s="89"/>
+      <c r="C53" s="89"/>
+      <c r="D53" s="90"/>
+      <c r="E53" s="57" t="s">
+        <v>58</v>
+      </c>
+      <c r="F53" s="86"/>
+      <c r="G53" s="86"/>
+      <c r="H53" s="56" t="s">
+        <v>59</v>
+      </c>
+      <c r="I53" s="86"/>
+      <c r="J53" s="86"/>
+      <c r="K53" s="87" t="s">
         <v>73</v>
       </c>
-      <c r="B53" s="59"/>
-      <c r="C53" s="59"/>
-      <c r="D53" s="60"/>
-      <c r="E53" s="57" t="s">
-        <v>59</v>
-      </c>
-      <c r="F53" s="65"/>
-      <c r="G53" s="65"/>
-      <c r="H53" s="56" t="s">
-        <v>60</v>
-      </c>
-      <c r="I53" s="65"/>
-      <c r="J53" s="65"/>
-      <c r="K53" s="66" t="s">
-        <v>74</v>
-      </c>
-      <c r="L53" s="66"/>
-      <c r="M53" s="66"/>
-      <c r="N53" s="66"/>
-      <c r="O53" s="66"/>
-      <c r="P53" s="66"/>
-      <c r="Q53" s="66"/>
-      <c r="R53" s="65"/>
-      <c r="S53" s="65"/>
-      <c r="T53" s="65"/>
-      <c r="U53" s="65"/>
-      <c r="V53" s="65"/>
-      <c r="W53" s="65"/>
-      <c r="X53" s="65"/>
-      <c r="Y53" s="65"/>
+      <c r="L53" s="87"/>
+      <c r="M53" s="87"/>
+      <c r="N53" s="87"/>
+      <c r="O53" s="87"/>
+      <c r="P53" s="87"/>
+      <c r="Q53" s="87"/>
+      <c r="R53" s="86"/>
+      <c r="S53" s="86"/>
+      <c r="T53" s="86"/>
+      <c r="U53" s="86"/>
+      <c r="V53" s="86"/>
+      <c r="W53" s="86"/>
+      <c r="X53" s="86"/>
+      <c r="Y53" s="86"/>
       <c r="Z53" s="10"/>
     </row>
     <row r="55" spans="1:26">
@@ -8820,95 +8821,6 @@
     </row>
   </sheetData>
   <mergeCells count="113">
-    <mergeCell ref="A8:C8"/>
-    <mergeCell ref="D8:J8"/>
-    <mergeCell ref="L8:O8"/>
-    <mergeCell ref="Q8:S8"/>
-    <mergeCell ref="K9:Z9"/>
-    <mergeCell ref="E9:I9"/>
-    <mergeCell ref="A9:D9"/>
-    <mergeCell ref="K1:Y1"/>
-    <mergeCell ref="K3:Q3"/>
-    <mergeCell ref="S3:Y3"/>
-    <mergeCell ref="K4:Q4"/>
-    <mergeCell ref="S4:Y4"/>
-    <mergeCell ref="K5:Q5"/>
-    <mergeCell ref="S5:Y5"/>
-    <mergeCell ref="K6:Q6"/>
-    <mergeCell ref="S6:Y6"/>
-    <mergeCell ref="M10:N10"/>
-    <mergeCell ref="O10:P10"/>
-    <mergeCell ref="Q10:R10"/>
-    <mergeCell ref="S10:T10"/>
-    <mergeCell ref="U10:V10"/>
-    <mergeCell ref="W10:X10"/>
-    <mergeCell ref="Y10:Z10"/>
-    <mergeCell ref="F15:J15"/>
-    <mergeCell ref="L7:O7"/>
-    <mergeCell ref="Q7:S7"/>
-    <mergeCell ref="K10:L10"/>
-    <mergeCell ref="A20:B20"/>
-    <mergeCell ref="C20:D20"/>
-    <mergeCell ref="A21:B21"/>
-    <mergeCell ref="C21:D21"/>
-    <mergeCell ref="A30:D30"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="B13:C13"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="A15:C15"/>
-    <mergeCell ref="C17:D17"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="C19:D19"/>
-    <mergeCell ref="C38:D38"/>
-    <mergeCell ref="A39:B39"/>
-    <mergeCell ref="C39:D39"/>
-    <mergeCell ref="A40:B40"/>
-    <mergeCell ref="C40:D40"/>
-    <mergeCell ref="A29:C29"/>
-    <mergeCell ref="D29:J29"/>
-    <mergeCell ref="E30:I30"/>
-    <mergeCell ref="A16:C16"/>
-    <mergeCell ref="D16:E16"/>
-    <mergeCell ref="A17:B17"/>
-    <mergeCell ref="A18:B18"/>
-    <mergeCell ref="C18:D18"/>
-    <mergeCell ref="F53:G53"/>
-    <mergeCell ref="I53:J53"/>
-    <mergeCell ref="K53:Q53"/>
-    <mergeCell ref="R53:Y53"/>
-    <mergeCell ref="F51:G51"/>
-    <mergeCell ref="I51:J51"/>
-    <mergeCell ref="F52:G52"/>
-    <mergeCell ref="I52:J52"/>
-    <mergeCell ref="P52:R52"/>
-    <mergeCell ref="S52:T52"/>
-    <mergeCell ref="K52:O52"/>
-    <mergeCell ref="B31:C31"/>
-    <mergeCell ref="B32:C32"/>
-    <mergeCell ref="U52:W52"/>
-    <mergeCell ref="X52:Y52"/>
-    <mergeCell ref="A46:B46"/>
-    <mergeCell ref="C46:D46"/>
-    <mergeCell ref="A47:B47"/>
-    <mergeCell ref="C47:D47"/>
-    <mergeCell ref="A48:B48"/>
-    <mergeCell ref="C48:D48"/>
-    <mergeCell ref="A49:B49"/>
-    <mergeCell ref="C49:D49"/>
-    <mergeCell ref="A41:B41"/>
-    <mergeCell ref="C41:D41"/>
-    <mergeCell ref="A42:B42"/>
-    <mergeCell ref="C42:D42"/>
-    <mergeCell ref="A43:B43"/>
-    <mergeCell ref="C43:D43"/>
-    <mergeCell ref="A44:B44"/>
-    <mergeCell ref="C45:D45"/>
-    <mergeCell ref="F36:J36"/>
-    <mergeCell ref="A37:C37"/>
-    <mergeCell ref="D37:E37"/>
-    <mergeCell ref="A38:B38"/>
     <mergeCell ref="A53:D53"/>
     <mergeCell ref="B33:C33"/>
     <mergeCell ref="B34:C34"/>
@@ -8933,6 +8845,95 @@
     <mergeCell ref="A52:D52"/>
     <mergeCell ref="C44:D44"/>
     <mergeCell ref="A45:B45"/>
+    <mergeCell ref="A46:B46"/>
+    <mergeCell ref="C46:D46"/>
+    <mergeCell ref="A47:B47"/>
+    <mergeCell ref="C47:D47"/>
+    <mergeCell ref="A48:B48"/>
+    <mergeCell ref="C48:D48"/>
+    <mergeCell ref="A49:B49"/>
+    <mergeCell ref="C49:D49"/>
+    <mergeCell ref="A41:B41"/>
+    <mergeCell ref="C41:D41"/>
+    <mergeCell ref="A42:B42"/>
+    <mergeCell ref="C42:D42"/>
+    <mergeCell ref="A43:B43"/>
+    <mergeCell ref="C43:D43"/>
+    <mergeCell ref="A44:B44"/>
+    <mergeCell ref="C45:D45"/>
+    <mergeCell ref="F53:G53"/>
+    <mergeCell ref="I53:J53"/>
+    <mergeCell ref="K53:Q53"/>
+    <mergeCell ref="R53:Y53"/>
+    <mergeCell ref="F51:G51"/>
+    <mergeCell ref="I51:J51"/>
+    <mergeCell ref="F52:G52"/>
+    <mergeCell ref="I52:J52"/>
+    <mergeCell ref="P52:R52"/>
+    <mergeCell ref="S52:T52"/>
+    <mergeCell ref="K52:O52"/>
+    <mergeCell ref="U52:W52"/>
+    <mergeCell ref="X52:Y52"/>
+    <mergeCell ref="C38:D38"/>
+    <mergeCell ref="A39:B39"/>
+    <mergeCell ref="C39:D39"/>
+    <mergeCell ref="A40:B40"/>
+    <mergeCell ref="C40:D40"/>
+    <mergeCell ref="A29:C29"/>
+    <mergeCell ref="D29:J29"/>
+    <mergeCell ref="E30:I30"/>
+    <mergeCell ref="A16:C16"/>
+    <mergeCell ref="D16:E16"/>
+    <mergeCell ref="A17:B17"/>
+    <mergeCell ref="A18:B18"/>
+    <mergeCell ref="C18:D18"/>
+    <mergeCell ref="B31:C31"/>
+    <mergeCell ref="B32:C32"/>
+    <mergeCell ref="F36:J36"/>
+    <mergeCell ref="A37:C37"/>
+    <mergeCell ref="D37:E37"/>
+    <mergeCell ref="A38:B38"/>
+    <mergeCell ref="A20:B20"/>
+    <mergeCell ref="C20:D20"/>
+    <mergeCell ref="A21:B21"/>
+    <mergeCell ref="C21:D21"/>
+    <mergeCell ref="A30:D30"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="A15:C15"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="M10:N10"/>
+    <mergeCell ref="O10:P10"/>
+    <mergeCell ref="Q10:R10"/>
+    <mergeCell ref="S10:T10"/>
+    <mergeCell ref="U10:V10"/>
+    <mergeCell ref="W10:X10"/>
+    <mergeCell ref="Y10:Z10"/>
+    <mergeCell ref="F15:J15"/>
+    <mergeCell ref="L7:O7"/>
+    <mergeCell ref="Q7:S7"/>
+    <mergeCell ref="K10:L10"/>
+    <mergeCell ref="A8:C8"/>
+    <mergeCell ref="D8:J8"/>
+    <mergeCell ref="L8:O8"/>
+    <mergeCell ref="Q8:S8"/>
+    <mergeCell ref="K9:Z9"/>
+    <mergeCell ref="E9:I9"/>
+    <mergeCell ref="A9:D9"/>
+    <mergeCell ref="K1:Y1"/>
+    <mergeCell ref="K3:Q3"/>
+    <mergeCell ref="S3:Y3"/>
+    <mergeCell ref="K4:Q4"/>
+    <mergeCell ref="S4:Y4"/>
+    <mergeCell ref="K5:Q5"/>
+    <mergeCell ref="S5:Y5"/>
+    <mergeCell ref="K6:Q6"/>
+    <mergeCell ref="S6:Y6"/>
   </mergeCells>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
   <pageMargins left="0.47244094488188981" right="0.35433070866141736" top="0.47244094488188981" bottom="0.19685039370078741" header="0.19685039370078741" footer="0.19685039370078741"/>

</xml_diff>

<commit_message>
- cleaning up chrome drivers now it all works - changing Pathlib.open to using a with block - updating template styling
</commit_message>
<xml_diff>
--- a/data/template.xlsx
+++ b/data/template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\me\Desktop\Development\NSBL\runsheet-script\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F0E7C7F-C646-40C1-9635-A0BA16B144BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D50657D5-698D-4F8C-934F-2239FA200E00}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="53925" yWindow="0" windowWidth="22875" windowHeight="21000" activeTab="1" xr2:uid="{026AB82B-103F-4DF3-A0CA-05AA2F209D25}"/>
+    <workbookView xWindow="22860" yWindow="0" windowWidth="31065" windowHeight="21000" activeTab="1" xr2:uid="{026AB82B-103F-4DF3-A0CA-05AA2F209D25}"/>
   </bookViews>
   <sheets>
     <sheet name="runsheet-k" sheetId="5" r:id="rId1"/>
@@ -1343,189 +1343,189 @@
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="34" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="25" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="26" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="25" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="10" fillId="7" borderId="25" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="25" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="7" borderId="35" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="25" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="7" borderId="35" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="25" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="31" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="30" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="32" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="16" fillId="7" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="7" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="7" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="7" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="44" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="38" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="48" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="29" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="27" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="33" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="7" borderId="28" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="7" borderId="27" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="7" borderId="33" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="29" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="27" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="47" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="7" borderId="26" xfId="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="7" borderId="25" xfId="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="7" borderId="25" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="7" borderId="14" xfId="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="50" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="50" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="51" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="57" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="55" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="58" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="45" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="34" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="46" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="44" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="38" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="54" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="55" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="56" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="50" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="53" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="43" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="50" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="7" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="52" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="48" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="7" borderId="49" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="45" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="29" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="27" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="47" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="7" borderId="28" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="7" borderId="27" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="7" borderId="33" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="25" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="46" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="26" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="50" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="50" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="25" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="50" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="50" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="31" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="51" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="30" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="52" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="32" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="53" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="16" fillId="7" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="43" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="7" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="54" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="7" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="55" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="7" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="56" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="29" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="27" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="33" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="10" fillId="7" borderId="25" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="25" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="35" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="57" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="25" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="55" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="7" borderId="35" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="58" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="25" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1648,8 +1648,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="300302" y="3249059"/>
-          <a:ext cx="406655" cy="108000"/>
+          <a:off x="306187" y="3227699"/>
+          <a:ext cx="406001" cy="108000"/>
           <a:chOff x="408650" y="3345734"/>
           <a:chExt cx="322695" cy="108000"/>
         </a:xfrm>
@@ -1887,8 +1887,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="300302" y="3409480"/>
-          <a:ext cx="406655" cy="108000"/>
+          <a:off x="306187" y="3393351"/>
+          <a:ext cx="406001" cy="108000"/>
           <a:chOff x="408650" y="3345734"/>
           <a:chExt cx="322695" cy="108000"/>
         </a:xfrm>
@@ -2075,8 +2075,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="300302" y="3569901"/>
-          <a:ext cx="406655" cy="108000"/>
+          <a:off x="306187" y="3559003"/>
+          <a:ext cx="406001" cy="108000"/>
           <a:chOff x="408650" y="3345734"/>
           <a:chExt cx="322695" cy="108000"/>
         </a:xfrm>
@@ -2263,8 +2263,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="300302" y="3730323"/>
-          <a:ext cx="406655" cy="108000"/>
+          <a:off x="306187" y="3724655"/>
+          <a:ext cx="406001" cy="108000"/>
           <a:chOff x="408650" y="3345734"/>
           <a:chExt cx="322695" cy="108000"/>
         </a:xfrm>
@@ -2451,8 +2451,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="300302" y="3890744"/>
-          <a:ext cx="406655" cy="108000"/>
+          <a:off x="306187" y="3890308"/>
+          <a:ext cx="406001" cy="108000"/>
           <a:chOff x="408650" y="3345734"/>
           <a:chExt cx="322695" cy="108000"/>
         </a:xfrm>
@@ -2639,8 +2639,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="300302" y="4051165"/>
-          <a:ext cx="406655" cy="108000"/>
+          <a:off x="306187" y="4055960"/>
+          <a:ext cx="406001" cy="108000"/>
           <a:chOff x="408650" y="3345734"/>
           <a:chExt cx="322695" cy="108000"/>
         </a:xfrm>
@@ -2827,8 +2827,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="300302" y="4211586"/>
-          <a:ext cx="406655" cy="108000"/>
+          <a:off x="306187" y="4221612"/>
+          <a:ext cx="406001" cy="108000"/>
           <a:chOff x="408650" y="3345734"/>
           <a:chExt cx="322695" cy="108000"/>
         </a:xfrm>
@@ -3015,8 +3015,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="300302" y="4372007"/>
-          <a:ext cx="406655" cy="108000"/>
+          <a:off x="306187" y="4387264"/>
+          <a:ext cx="406001" cy="108000"/>
           <a:chOff x="408650" y="3345734"/>
           <a:chExt cx="322695" cy="108000"/>
         </a:xfrm>
@@ -3203,8 +3203,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="300302" y="6888612"/>
-          <a:ext cx="406655" cy="108000"/>
+          <a:off x="306187" y="6930025"/>
+          <a:ext cx="406001" cy="108000"/>
           <a:chOff x="408650" y="3345734"/>
           <a:chExt cx="322695" cy="108000"/>
         </a:xfrm>
@@ -3391,8 +3391,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="300302" y="6728191"/>
-          <a:ext cx="406655" cy="108000"/>
+          <a:off x="306187" y="6764373"/>
+          <a:ext cx="406001" cy="108000"/>
           <a:chOff x="408650" y="3345734"/>
           <a:chExt cx="322695" cy="108000"/>
         </a:xfrm>
@@ -3579,8 +3579,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="300302" y="7049033"/>
-          <a:ext cx="406655" cy="108000"/>
+          <a:off x="306187" y="7095677"/>
+          <a:ext cx="406001" cy="108000"/>
           <a:chOff x="408650" y="3345734"/>
           <a:chExt cx="322695" cy="108000"/>
         </a:xfrm>
@@ -3767,8 +3767,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="300302" y="7209454"/>
-          <a:ext cx="406655" cy="108000"/>
+          <a:off x="306187" y="7261329"/>
+          <a:ext cx="406001" cy="108000"/>
           <a:chOff x="408650" y="3345734"/>
           <a:chExt cx="322695" cy="108000"/>
         </a:xfrm>
@@ -3955,8 +3955,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="300302" y="7369875"/>
-          <a:ext cx="406655" cy="108000"/>
+          <a:off x="306187" y="7426982"/>
+          <a:ext cx="406001" cy="108000"/>
           <a:chOff x="408650" y="3345734"/>
           <a:chExt cx="322695" cy="108000"/>
         </a:xfrm>
@@ -4143,8 +4143,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="300302" y="7530296"/>
-          <a:ext cx="406655" cy="108000"/>
+          <a:off x="306187" y="7592634"/>
+          <a:ext cx="406001" cy="108000"/>
           <a:chOff x="408650" y="3345734"/>
           <a:chExt cx="322695" cy="108000"/>
         </a:xfrm>
@@ -4331,8 +4331,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="300302" y="7690717"/>
-          <a:ext cx="406655" cy="108000"/>
+          <a:off x="306187" y="7758286"/>
+          <a:ext cx="406001" cy="108000"/>
           <a:chOff x="408650" y="3345734"/>
           <a:chExt cx="322695" cy="108000"/>
         </a:xfrm>
@@ -4519,8 +4519,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="300302" y="7851138"/>
-          <a:ext cx="406655" cy="108000"/>
+          <a:off x="306187" y="7923938"/>
+          <a:ext cx="406001" cy="108000"/>
           <a:chOff x="408650" y="3345734"/>
           <a:chExt cx="322695" cy="108000"/>
         </a:xfrm>
@@ -5256,8 +5256,8 @@
   </sheetPr>
   <dimension ref="A1:AB61"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="AB4" sqref="AA4:AB4"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="AJ29" sqref="AJ29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -5277,299 +5277,299 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:28" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="96"/>
-      <c r="B1" s="97"/>
-      <c r="C1" s="98"/>
-      <c r="D1" s="97"/>
-      <c r="E1" s="97"/>
+      <c r="A1" s="58"/>
+      <c r="B1" s="59"/>
+      <c r="C1" s="60"/>
+      <c r="D1" s="59"/>
+      <c r="E1" s="59"/>
       <c r="F1" s="49"/>
       <c r="G1" s="49"/>
       <c r="H1" s="49"/>
       <c r="I1" s="49"/>
       <c r="J1" s="49"/>
-      <c r="K1" s="62" t="s">
+      <c r="K1" s="117" t="s">
         <v>43</v>
       </c>
-      <c r="L1" s="63"/>
-      <c r="M1" s="63"/>
-      <c r="N1" s="63"/>
-      <c r="O1" s="63"/>
-      <c r="P1" s="63"/>
-      <c r="Q1" s="63"/>
-      <c r="R1" s="63"/>
-      <c r="S1" s="63"/>
-      <c r="T1" s="63"/>
-      <c r="U1" s="63"/>
-      <c r="V1" s="63"/>
-      <c r="W1" s="63"/>
-      <c r="X1" s="63"/>
-      <c r="Y1" s="63"/>
+      <c r="L1" s="118"/>
+      <c r="M1" s="118"/>
+      <c r="N1" s="118"/>
+      <c r="O1" s="118"/>
+      <c r="P1" s="118"/>
+      <c r="Q1" s="118"/>
+      <c r="R1" s="118"/>
+      <c r="S1" s="118"/>
+      <c r="T1" s="118"/>
+      <c r="U1" s="118"/>
+      <c r="V1" s="118"/>
+      <c r="W1" s="118"/>
+      <c r="X1" s="118"/>
+      <c r="Y1" s="118"/>
       <c r="Z1" s="50"/>
     </row>
     <row r="2" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A2" s="99"/>
-      <c r="B2" s="100"/>
-      <c r="C2" s="101"/>
-      <c r="D2" s="100"/>
-      <c r="E2" s="100"/>
-      <c r="F2" s="100"/>
-      <c r="G2" s="100"/>
-      <c r="H2" s="100"/>
-      <c r="I2" s="100"/>
-      <c r="J2" s="100"/>
-      <c r="K2" s="101"/>
-      <c r="L2" s="101"/>
-      <c r="M2" s="101"/>
-      <c r="N2" s="101"/>
-      <c r="O2" s="101"/>
-      <c r="P2" s="101"/>
-      <c r="Q2" s="101"/>
-      <c r="R2" s="101"/>
-      <c r="S2" s="101"/>
-      <c r="T2" s="101"/>
-      <c r="U2" s="101"/>
-      <c r="V2" s="101"/>
-      <c r="W2" s="101"/>
-      <c r="X2" s="101"/>
-      <c r="Y2" s="101"/>
+      <c r="A2" s="61"/>
+      <c r="B2" s="62"/>
+      <c r="C2" s="63"/>
+      <c r="D2" s="62"/>
+      <c r="E2" s="62"/>
+      <c r="F2" s="62"/>
+      <c r="G2" s="62"/>
+      <c r="H2" s="62"/>
+      <c r="I2" s="62"/>
+      <c r="J2" s="62"/>
+      <c r="K2" s="63"/>
+      <c r="L2" s="63"/>
+      <c r="M2" s="63"/>
+      <c r="N2" s="63"/>
+      <c r="O2" s="63"/>
+      <c r="P2" s="63"/>
+      <c r="Q2" s="63"/>
+      <c r="R2" s="63"/>
+      <c r="S2" s="63"/>
+      <c r="T2" s="63"/>
+      <c r="U2" s="63"/>
+      <c r="V2" s="63"/>
+      <c r="W2" s="63"/>
+      <c r="X2" s="63"/>
+      <c r="Y2" s="63"/>
       <c r="Z2" s="51"/>
     </row>
     <row r="3" spans="1:28" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="99"/>
-      <c r="B3" s="100"/>
-      <c r="C3" s="101"/>
-      <c r="D3" s="100"/>
-      <c r="E3" s="100"/>
-      <c r="F3" s="100"/>
-      <c r="G3" s="100"/>
-      <c r="H3" s="100"/>
-      <c r="I3" s="100"/>
-      <c r="J3" s="100"/>
-      <c r="K3" s="64" t="s">
+      <c r="A3" s="61"/>
+      <c r="B3" s="62"/>
+      <c r="C3" s="63"/>
+      <c r="D3" s="62"/>
+      <c r="E3" s="62"/>
+      <c r="F3" s="62"/>
+      <c r="G3" s="62"/>
+      <c r="H3" s="62"/>
+      <c r="I3" s="62"/>
+      <c r="J3" s="62"/>
+      <c r="K3" s="119" t="s">
         <v>44</v>
       </c>
-      <c r="L3" s="64"/>
-      <c r="M3" s="64"/>
-      <c r="N3" s="64"/>
-      <c r="O3" s="64"/>
-      <c r="P3" s="64"/>
-      <c r="Q3" s="64"/>
-      <c r="R3" s="101"/>
-      <c r="S3" s="64" t="s">
+      <c r="L3" s="119"/>
+      <c r="M3" s="119"/>
+      <c r="N3" s="119"/>
+      <c r="O3" s="119"/>
+      <c r="P3" s="119"/>
+      <c r="Q3" s="119"/>
+      <c r="R3" s="63"/>
+      <c r="S3" s="119" t="s">
         <v>45</v>
       </c>
-      <c r="T3" s="64"/>
-      <c r="U3" s="64"/>
-      <c r="V3" s="64"/>
-      <c r="W3" s="64"/>
-      <c r="X3" s="64"/>
-      <c r="Y3" s="64"/>
+      <c r="T3" s="119"/>
+      <c r="U3" s="119"/>
+      <c r="V3" s="119"/>
+      <c r="W3" s="119"/>
+      <c r="X3" s="119"/>
+      <c r="Y3" s="119"/>
       <c r="Z3" s="51"/>
     </row>
     <row r="4" spans="1:28" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A4" s="16"/>
-      <c r="B4" s="102"/>
-      <c r="C4" s="103"/>
-      <c r="D4" s="102"/>
-      <c r="E4" s="102"/>
-      <c r="F4" s="102"/>
-      <c r="G4" s="102"/>
-      <c r="H4" s="102"/>
-      <c r="I4" s="102"/>
-      <c r="J4" s="102"/>
-      <c r="K4" s="65" t="s">
+      <c r="B4" s="64"/>
+      <c r="C4" s="65"/>
+      <c r="D4" s="64"/>
+      <c r="E4" s="64"/>
+      <c r="F4" s="64"/>
+      <c r="G4" s="64"/>
+      <c r="H4" s="64"/>
+      <c r="I4" s="64"/>
+      <c r="J4" s="64"/>
+      <c r="K4" s="120" t="s">
         <v>46</v>
       </c>
-      <c r="L4" s="65"/>
-      <c r="M4" s="65"/>
-      <c r="N4" s="65"/>
-      <c r="O4" s="65"/>
-      <c r="P4" s="65"/>
-      <c r="Q4" s="65"/>
-      <c r="R4" s="103"/>
-      <c r="S4" s="65" t="s">
+      <c r="L4" s="120"/>
+      <c r="M4" s="120"/>
+      <c r="N4" s="120"/>
+      <c r="O4" s="120"/>
+      <c r="P4" s="120"/>
+      <c r="Q4" s="120"/>
+      <c r="R4" s="65"/>
+      <c r="S4" s="120" t="s">
         <v>47</v>
       </c>
-      <c r="T4" s="65"/>
-      <c r="U4" s="65"/>
-      <c r="V4" s="65"/>
-      <c r="W4" s="65"/>
-      <c r="X4" s="65"/>
-      <c r="Y4" s="65"/>
+      <c r="T4" s="120"/>
+      <c r="U4" s="120"/>
+      <c r="V4" s="120"/>
+      <c r="W4" s="120"/>
+      <c r="X4" s="120"/>
+      <c r="Y4" s="120"/>
       <c r="Z4" s="20"/>
     </row>
     <row r="5" spans="1:28" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="16"/>
-      <c r="B5" s="102"/>
-      <c r="C5" s="103"/>
-      <c r="D5" s="102"/>
-      <c r="E5" s="102"/>
-      <c r="F5" s="102"/>
-      <c r="G5" s="102"/>
-      <c r="H5" s="102"/>
-      <c r="I5" s="102"/>
-      <c r="J5" s="102"/>
-      <c r="K5" s="66" t="s">
+      <c r="B5" s="64"/>
+      <c r="C5" s="65"/>
+      <c r="D5" s="64"/>
+      <c r="E5" s="64"/>
+      <c r="F5" s="64"/>
+      <c r="G5" s="64"/>
+      <c r="H5" s="64"/>
+      <c r="I5" s="64"/>
+      <c r="J5" s="64"/>
+      <c r="K5" s="121" t="s">
         <v>48</v>
       </c>
-      <c r="L5" s="66"/>
-      <c r="M5" s="66"/>
-      <c r="N5" s="66"/>
-      <c r="O5" s="66"/>
-      <c r="P5" s="66"/>
-      <c r="Q5" s="66"/>
-      <c r="R5" s="103"/>
-      <c r="S5" s="66" t="s">
+      <c r="L5" s="121"/>
+      <c r="M5" s="121"/>
+      <c r="N5" s="121"/>
+      <c r="O5" s="121"/>
+      <c r="P5" s="121"/>
+      <c r="Q5" s="121"/>
+      <c r="R5" s="65"/>
+      <c r="S5" s="121" t="s">
         <v>49</v>
       </c>
-      <c r="T5" s="66"/>
-      <c r="U5" s="66"/>
-      <c r="V5" s="66"/>
-      <c r="W5" s="66"/>
-      <c r="X5" s="66"/>
-      <c r="Y5" s="66"/>
+      <c r="T5" s="121"/>
+      <c r="U5" s="121"/>
+      <c r="V5" s="121"/>
+      <c r="W5" s="121"/>
+      <c r="X5" s="121"/>
+      <c r="Y5" s="121"/>
       <c r="Z5" s="20"/>
     </row>
     <row r="6" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A6" s="16"/>
-      <c r="B6" s="102"/>
-      <c r="C6" s="103"/>
-      <c r="D6" s="102"/>
-      <c r="E6" s="102"/>
-      <c r="F6" s="102"/>
-      <c r="G6" s="102"/>
-      <c r="H6" s="102"/>
-      <c r="I6" s="102"/>
-      <c r="J6" s="102"/>
-      <c r="K6" s="67" t="s">
+      <c r="B6" s="64"/>
+      <c r="C6" s="65"/>
+      <c r="D6" s="64"/>
+      <c r="E6" s="64"/>
+      <c r="F6" s="64"/>
+      <c r="G6" s="64"/>
+      <c r="H6" s="64"/>
+      <c r="I6" s="64"/>
+      <c r="J6" s="64"/>
+      <c r="K6" s="122" t="s">
         <v>50</v>
       </c>
-      <c r="L6" s="67"/>
-      <c r="M6" s="67"/>
-      <c r="N6" s="67"/>
-      <c r="O6" s="67"/>
-      <c r="P6" s="67"/>
-      <c r="Q6" s="67"/>
-      <c r="R6" s="103"/>
-      <c r="S6" s="67" t="s">
+      <c r="L6" s="122"/>
+      <c r="M6" s="122"/>
+      <c r="N6" s="122"/>
+      <c r="O6" s="122"/>
+      <c r="P6" s="122"/>
+      <c r="Q6" s="122"/>
+      <c r="R6" s="65"/>
+      <c r="S6" s="122" t="s">
         <v>51</v>
       </c>
-      <c r="T6" s="67"/>
-      <c r="U6" s="67"/>
-      <c r="V6" s="67"/>
-      <c r="W6" s="67"/>
-      <c r="X6" s="67"/>
-      <c r="Y6" s="67"/>
+      <c r="T6" s="122"/>
+      <c r="U6" s="122"/>
+      <c r="V6" s="122"/>
+      <c r="W6" s="122"/>
+      <c r="X6" s="122"/>
+      <c r="Y6" s="122"/>
       <c r="Z6" s="20"/>
     </row>
     <row r="7" spans="1:28" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="16"/>
-      <c r="B7" s="102"/>
-      <c r="C7" s="103"/>
-      <c r="D7" s="102"/>
-      <c r="E7" s="102"/>
-      <c r="F7" s="102"/>
-      <c r="G7" s="102"/>
-      <c r="H7" s="102"/>
-      <c r="I7" s="102"/>
-      <c r="J7" s="102"/>
-      <c r="K7" s="103"/>
-      <c r="L7" s="73" t="s">
+      <c r="B7" s="64"/>
+      <c r="C7" s="65"/>
+      <c r="D7" s="64"/>
+      <c r="E7" s="64"/>
+      <c r="F7" s="64"/>
+      <c r="G7" s="64"/>
+      <c r="H7" s="64"/>
+      <c r="I7" s="64"/>
+      <c r="J7" s="64"/>
+      <c r="K7" s="65"/>
+      <c r="L7" s="110" t="s">
         <v>52</v>
       </c>
-      <c r="M7" s="74"/>
-      <c r="N7" s="74"/>
-      <c r="O7" s="75"/>
-      <c r="P7" s="103"/>
-      <c r="Q7" s="76" t="s">
+      <c r="M7" s="111"/>
+      <c r="N7" s="111"/>
+      <c r="O7" s="112"/>
+      <c r="P7" s="65"/>
+      <c r="Q7" s="113" t="s">
         <v>53</v>
       </c>
-      <c r="R7" s="74"/>
-      <c r="S7" s="75"/>
-      <c r="T7" s="103"/>
-      <c r="U7" s="103"/>
-      <c r="V7" s="103"/>
-      <c r="W7" s="103"/>
-      <c r="X7" s="103"/>
-      <c r="Y7" s="103"/>
+      <c r="R7" s="111"/>
+      <c r="S7" s="112"/>
+      <c r="T7" s="65"/>
+      <c r="U7" s="65"/>
+      <c r="V7" s="65"/>
+      <c r="W7" s="65"/>
+      <c r="X7" s="65"/>
+      <c r="Y7" s="65"/>
       <c r="Z7" s="20"/>
       <c r="AB7" s="52"/>
     </row>
-    <row r="8" spans="1:28" ht="16.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="93" t="s">
+    <row r="8" spans="1:28" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="97" t="s">
         <v>46</v>
       </c>
-      <c r="B8" s="94"/>
-      <c r="C8" s="94"/>
-      <c r="D8" s="90" t="s">
+      <c r="B8" s="98"/>
+      <c r="C8" s="98"/>
+      <c r="D8" s="100" t="s">
         <v>54</v>
       </c>
-      <c r="E8" s="91"/>
-      <c r="F8" s="91"/>
-      <c r="G8" s="91"/>
-      <c r="H8" s="91"/>
-      <c r="I8" s="91"/>
-      <c r="J8" s="92"/>
-      <c r="K8" s="103"/>
-      <c r="L8" s="58" t="s">
+      <c r="E8" s="101"/>
+      <c r="F8" s="101"/>
+      <c r="G8" s="101"/>
+      <c r="H8" s="101"/>
+      <c r="I8" s="101"/>
+      <c r="J8" s="102"/>
+      <c r="K8" s="65"/>
+      <c r="L8" s="74" t="s">
         <v>55</v>
       </c>
-      <c r="M8" s="58"/>
-      <c r="N8" s="58"/>
-      <c r="O8" s="58"/>
-      <c r="P8" s="103"/>
-      <c r="Q8" s="58" t="s">
+      <c r="M8" s="74"/>
+      <c r="N8" s="74"/>
+      <c r="O8" s="74"/>
+      <c r="P8" s="65"/>
+      <c r="Q8" s="74" t="s">
         <v>3</v>
       </c>
-      <c r="R8" s="58"/>
-      <c r="S8" s="58"/>
-      <c r="T8" s="103"/>
-      <c r="U8" s="104"/>
-      <c r="V8" s="103"/>
-      <c r="W8" s="103"/>
-      <c r="X8" s="103"/>
-      <c r="Y8" s="103"/>
+      <c r="R8" s="74"/>
+      <c r="S8" s="74"/>
+      <c r="T8" s="65"/>
+      <c r="U8" s="66"/>
+      <c r="V8" s="65"/>
+      <c r="W8" s="65"/>
+      <c r="X8" s="65"/>
+      <c r="Y8" s="65"/>
       <c r="Z8" s="20"/>
     </row>
     <row r="9" spans="1:28" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="60" t="s">
+      <c r="A9" s="105" t="s">
         <v>56</v>
       </c>
-      <c r="B9" s="61"/>
-      <c r="C9" s="61"/>
-      <c r="D9" s="61"/>
-      <c r="E9" s="59" t="s">
+      <c r="B9" s="106"/>
+      <c r="C9" s="106"/>
+      <c r="D9" s="106"/>
+      <c r="E9" s="103" t="s">
         <v>57</v>
       </c>
-      <c r="F9" s="59"/>
-      <c r="G9" s="59"/>
-      <c r="H9" s="59"/>
-      <c r="I9" s="59"/>
+      <c r="F9" s="103"/>
+      <c r="G9" s="103"/>
+      <c r="H9" s="103"/>
+      <c r="I9" s="103"/>
       <c r="J9" s="27"/>
-      <c r="K9" s="87" t="s">
+      <c r="K9" s="114" t="s">
         <v>58</v>
       </c>
-      <c r="L9" s="88"/>
-      <c r="M9" s="88"/>
-      <c r="N9" s="88"/>
-      <c r="O9" s="88"/>
-      <c r="P9" s="88"/>
-      <c r="Q9" s="88"/>
-      <c r="R9" s="88"/>
-      <c r="S9" s="88"/>
-      <c r="T9" s="88"/>
-      <c r="U9" s="88"/>
-      <c r="V9" s="88"/>
-      <c r="W9" s="88"/>
-      <c r="X9" s="88"/>
-      <c r="Y9" s="88"/>
-      <c r="Z9" s="89"/>
+      <c r="L9" s="115"/>
+      <c r="M9" s="115"/>
+      <c r="N9" s="115"/>
+      <c r="O9" s="115"/>
+      <c r="P9" s="115"/>
+      <c r="Q9" s="115"/>
+      <c r="R9" s="115"/>
+      <c r="S9" s="115"/>
+      <c r="T9" s="115"/>
+      <c r="U9" s="115"/>
+      <c r="V9" s="115"/>
+      <c r="W9" s="115"/>
+      <c r="X9" s="115"/>
+      <c r="Y9" s="115"/>
+      <c r="Z9" s="116"/>
     </row>
     <row r="10" spans="1:28" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" s="16"/>
-      <c r="B10" s="71"/>
+      <c r="B10" s="76"/>
       <c r="C10" s="77"/>
-      <c r="D10" s="102"/>
+      <c r="D10" s="64"/>
       <c r="E10" s="26" t="s">
         <v>59</v>
       </c>
@@ -5585,46 +5585,46 @@
       <c r="I10" s="30">
         <v>4</v>
       </c>
-      <c r="J10" s="102"/>
-      <c r="K10" s="70" t="s">
+      <c r="J10" s="64"/>
+      <c r="K10" s="109" t="s">
         <v>60</v>
       </c>
-      <c r="L10" s="68"/>
-      <c r="M10" s="68" t="s">
+      <c r="L10" s="107"/>
+      <c r="M10" s="107" t="s">
         <v>61</v>
       </c>
-      <c r="N10" s="69"/>
-      <c r="O10" s="70" t="s">
+      <c r="N10" s="108"/>
+      <c r="O10" s="109" t="s">
         <v>60</v>
       </c>
-      <c r="P10" s="68"/>
-      <c r="Q10" s="68" t="s">
+      <c r="P10" s="107"/>
+      <c r="Q10" s="107" t="s">
         <v>61</v>
       </c>
-      <c r="R10" s="69"/>
-      <c r="S10" s="70" t="s">
+      <c r="R10" s="108"/>
+      <c r="S10" s="109" t="s">
         <v>60</v>
       </c>
-      <c r="T10" s="68"/>
-      <c r="U10" s="68" t="s">
+      <c r="T10" s="107"/>
+      <c r="U10" s="107" t="s">
         <v>61</v>
       </c>
-      <c r="V10" s="69"/>
-      <c r="W10" s="70" t="s">
+      <c r="V10" s="108"/>
+      <c r="W10" s="109" t="s">
         <v>60</v>
       </c>
-      <c r="X10" s="68"/>
-      <c r="Y10" s="68" t="s">
+      <c r="X10" s="107"/>
+      <c r="Y10" s="107" t="s">
         <v>61</v>
       </c>
-      <c r="Z10" s="69"/>
+      <c r="Z10" s="108"/>
     </row>
     <row r="11" spans="1:28" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A11" s="16"/>
-      <c r="B11" s="71"/>
+      <c r="B11" s="76"/>
       <c r="C11" s="77"/>
-      <c r="D11" s="103"/>
-      <c r="E11" s="103"/>
+      <c r="D11" s="65"/>
+      <c r="E11" s="65"/>
       <c r="F11" s="31">
         <v>5</v>
       </c>
@@ -5637,7 +5637,7 @@
       <c r="I11" s="33">
         <v>8</v>
       </c>
-      <c r="J11" s="102"/>
+      <c r="J11" s="64"/>
       <c r="K11" s="13"/>
       <c r="L11" s="17">
         <v>1</v>
@@ -5673,9 +5673,9 @@
     </row>
     <row r="12" spans="1:28" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12" s="16"/>
-      <c r="B12" s="71"/>
+      <c r="B12" s="76"/>
       <c r="C12" s="77"/>
-      <c r="D12" s="102"/>
+      <c r="D12" s="64"/>
       <c r="E12" s="26" t="s">
         <v>62</v>
       </c>
@@ -5691,7 +5691,7 @@
       <c r="I12" s="36">
         <v>4</v>
       </c>
-      <c r="J12" s="102"/>
+      <c r="J12" s="64"/>
       <c r="K12" s="13"/>
       <c r="L12" s="17">
         <v>2</v>
@@ -5727,10 +5727,10 @@
     </row>
     <row r="13" spans="1:28" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A13" s="16"/>
-      <c r="B13" s="71"/>
+      <c r="B13" s="76"/>
       <c r="C13" s="77"/>
-      <c r="D13" s="103"/>
-      <c r="E13" s="103"/>
+      <c r="D13" s="65"/>
+      <c r="E13" s="65"/>
       <c r="F13" s="28">
         <v>5</v>
       </c>
@@ -5743,7 +5743,7 @@
       <c r="I13" s="30">
         <v>8</v>
       </c>
-      <c r="J13" s="102"/>
+      <c r="J13" s="64"/>
       <c r="K13" s="13"/>
       <c r="L13" s="17">
         <v>3</v>
@@ -5779,17 +5779,17 @@
     </row>
     <row r="14" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="16"/>
-      <c r="B14" s="71"/>
+      <c r="B14" s="76"/>
       <c r="C14" s="77"/>
       <c r="D14" s="10"/>
-      <c r="E14" s="102" t="s">
+      <c r="E14" s="64" t="s">
         <v>63</v>
       </c>
-      <c r="F14" s="103"/>
-      <c r="G14" s="102"/>
-      <c r="H14" s="102"/>
-      <c r="I14" s="102"/>
-      <c r="J14" s="102"/>
+      <c r="F14" s="65"/>
+      <c r="G14" s="64"/>
+      <c r="H14" s="64"/>
+      <c r="I14" s="64"/>
+      <c r="J14" s="64"/>
       <c r="K14" s="13"/>
       <c r="L14" s="17">
         <v>4</v>
@@ -5825,17 +5825,17 @@
     </row>
     <row r="15" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A15" s="78"/>
-      <c r="B15" s="72"/>
+      <c r="B15" s="79"/>
       <c r="C15" s="77"/>
-      <c r="D15" s="102"/>
-      <c r="E15" s="102"/>
-      <c r="F15" s="71" t="s">
+      <c r="D15" s="64"/>
+      <c r="E15" s="64"/>
+      <c r="F15" s="76" t="s">
         <v>64</v>
       </c>
-      <c r="G15" s="72"/>
-      <c r="H15" s="72"/>
-      <c r="I15" s="72"/>
-      <c r="J15" s="72"/>
+      <c r="G15" s="79"/>
+      <c r="H15" s="79"/>
+      <c r="I15" s="79"/>
+      <c r="J15" s="79"/>
       <c r="K15" s="13"/>
       <c r="L15" s="17">
         <v>5</v>
@@ -5873,12 +5873,12 @@
       <c r="A16" s="78" t="s">
         <v>65</v>
       </c>
-      <c r="B16" s="72"/>
+      <c r="B16" s="79"/>
       <c r="C16" s="77"/>
-      <c r="D16" s="79" t="s">
+      <c r="D16" s="104" t="s">
         <v>66</v>
       </c>
-      <c r="E16" s="80"/>
+      <c r="E16" s="81"/>
       <c r="F16" s="37">
         <v>1</v>
       </c>
@@ -5932,7 +5932,7 @@
         <v>67</v>
       </c>
       <c r="B17" s="77"/>
-      <c r="C17" s="71"/>
+      <c r="C17" s="76"/>
       <c r="D17" s="77"/>
       <c r="E17" s="15" t="s">
         <v>68</v>
@@ -5978,7 +5978,7 @@
     <row r="18" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A18" s="78"/>
       <c r="B18" s="77"/>
-      <c r="C18" s="71"/>
+      <c r="C18" s="76"/>
       <c r="D18" s="77"/>
       <c r="E18" s="15"/>
       <c r="F18" s="15"/>
@@ -6022,7 +6022,7 @@
     <row r="19" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A19" s="78"/>
       <c r="B19" s="77"/>
-      <c r="C19" s="71"/>
+      <c r="C19" s="76"/>
       <c r="D19" s="77"/>
       <c r="E19" s="15"/>
       <c r="F19" s="15"/>
@@ -6066,7 +6066,7 @@
     <row r="20" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A20" s="78"/>
       <c r="B20" s="77"/>
-      <c r="C20" s="71"/>
+      <c r="C20" s="76"/>
       <c r="D20" s="77"/>
       <c r="E20" s="15"/>
       <c r="F20" s="15"/>
@@ -6110,7 +6110,7 @@
     <row r="21" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A21" s="78"/>
       <c r="B21" s="77"/>
-      <c r="C21" s="71"/>
+      <c r="C21" s="76"/>
       <c r="D21" s="77"/>
       <c r="E21" s="15"/>
       <c r="F21" s="15"/>
@@ -6154,7 +6154,7 @@
     <row r="22" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A22" s="78"/>
       <c r="B22" s="77"/>
-      <c r="C22" s="71"/>
+      <c r="C22" s="76"/>
       <c r="D22" s="77"/>
       <c r="E22" s="15"/>
       <c r="F22" s="15"/>
@@ -6198,7 +6198,7 @@
     <row r="23" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A23" s="78"/>
       <c r="B23" s="77"/>
-      <c r="C23" s="71"/>
+      <c r="C23" s="76"/>
       <c r="D23" s="77"/>
       <c r="E23" s="15"/>
       <c r="F23" s="15"/>
@@ -6242,7 +6242,7 @@
     <row r="24" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A24" s="78"/>
       <c r="B24" s="77"/>
-      <c r="C24" s="71"/>
+      <c r="C24" s="76"/>
       <c r="D24" s="77"/>
       <c r="E24" s="15"/>
       <c r="F24" s="15"/>
@@ -6286,7 +6286,7 @@
     <row r="25" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A25" s="78"/>
       <c r="B25" s="77"/>
-      <c r="C25" s="71"/>
+      <c r="C25" s="76"/>
       <c r="D25" s="77"/>
       <c r="E25" s="15"/>
       <c r="F25" s="15"/>
@@ -6330,7 +6330,7 @@
     <row r="26" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A26" s="78"/>
       <c r="B26" s="77"/>
-      <c r="C26" s="71"/>
+      <c r="C26" s="76"/>
       <c r="D26" s="77"/>
       <c r="E26" s="15"/>
       <c r="F26" s="15"/>
@@ -6374,7 +6374,7 @@
     <row r="27" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A27" s="78"/>
       <c r="B27" s="77"/>
-      <c r="C27" s="71"/>
+      <c r="C27" s="76"/>
       <c r="D27" s="77"/>
       <c r="E27" s="15"/>
       <c r="F27" s="15"/>
@@ -6416,10 +6416,10 @@
       <c r="Z27" s="12"/>
     </row>
     <row r="28" spans="1:26" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="84"/>
-      <c r="B28" s="80"/>
-      <c r="C28" s="85"/>
-      <c r="D28" s="80"/>
+      <c r="A28" s="80"/>
+      <c r="B28" s="81"/>
+      <c r="C28" s="82"/>
+      <c r="D28" s="81"/>
       <c r="E28" s="53"/>
       <c r="F28" s="53"/>
       <c r="G28" s="11"/>
@@ -6459,21 +6459,21 @@
       </c>
       <c r="Z28" s="12"/>
     </row>
-    <row r="29" spans="1:26" ht="16.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="93" t="s">
+    <row r="29" spans="1:26" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="97" t="s">
         <v>47</v>
       </c>
-      <c r="B29" s="94"/>
-      <c r="C29" s="95"/>
-      <c r="D29" s="90" t="s">
+      <c r="B29" s="98"/>
+      <c r="C29" s="99"/>
+      <c r="D29" s="100" t="s">
         <v>69</v>
       </c>
-      <c r="E29" s="91"/>
-      <c r="F29" s="91"/>
-      <c r="G29" s="91"/>
-      <c r="H29" s="91"/>
-      <c r="I29" s="91"/>
-      <c r="J29" s="92"/>
+      <c r="E29" s="101"/>
+      <c r="F29" s="101"/>
+      <c r="G29" s="101"/>
+      <c r="H29" s="101"/>
+      <c r="I29" s="101"/>
+      <c r="J29" s="102"/>
       <c r="K29" s="13"/>
       <c r="L29" s="17">
         <v>19</v>
@@ -6508,19 +6508,19 @@
       <c r="Z29" s="12"/>
     </row>
     <row r="30" spans="1:26" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="60" t="s">
+      <c r="A30" s="105" t="s">
         <v>56</v>
       </c>
-      <c r="B30" s="61"/>
-      <c r="C30" s="61"/>
-      <c r="D30" s="61"/>
-      <c r="E30" s="59" t="s">
+      <c r="B30" s="106"/>
+      <c r="C30" s="106"/>
+      <c r="D30" s="106"/>
+      <c r="E30" s="103" t="s">
         <v>57</v>
       </c>
-      <c r="F30" s="59"/>
-      <c r="G30" s="59"/>
-      <c r="H30" s="59"/>
-      <c r="I30" s="59"/>
+      <c r="F30" s="103"/>
+      <c r="G30" s="103"/>
+      <c r="H30" s="103"/>
+      <c r="I30" s="103"/>
       <c r="J30" s="27"/>
       <c r="K30" s="13"/>
       <c r="L30" s="17">
@@ -6557,9 +6557,9 @@
     </row>
     <row r="31" spans="1:26" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A31" s="16"/>
-      <c r="B31" s="71"/>
+      <c r="B31" s="76"/>
       <c r="C31" s="77"/>
-      <c r="D31" s="102"/>
+      <c r="D31" s="64"/>
       <c r="E31" s="26" t="s">
         <v>59</v>
       </c>
@@ -6575,7 +6575,7 @@
       <c r="I31" s="30">
         <v>4</v>
       </c>
-      <c r="J31" s="102"/>
+      <c r="J31" s="64"/>
       <c r="K31" s="13"/>
       <c r="L31" s="17">
         <v>21</v>
@@ -6611,10 +6611,10 @@
     </row>
     <row r="32" spans="1:26" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A32" s="16"/>
-      <c r="B32" s="71"/>
+      <c r="B32" s="76"/>
       <c r="C32" s="77"/>
-      <c r="D32" s="103"/>
-      <c r="E32" s="103"/>
+      <c r="D32" s="65"/>
+      <c r="E32" s="65"/>
       <c r="F32" s="31">
         <v>5</v>
       </c>
@@ -6627,7 +6627,7 @@
       <c r="I32" s="33">
         <v>8</v>
       </c>
-      <c r="J32" s="102"/>
+      <c r="J32" s="64"/>
       <c r="K32" s="13"/>
       <c r="L32" s="17">
         <v>22</v>
@@ -6663,9 +6663,9 @@
     </row>
     <row r="33" spans="1:26" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A33" s="16"/>
-      <c r="B33" s="71"/>
+      <c r="B33" s="76"/>
       <c r="C33" s="77"/>
-      <c r="D33" s="102"/>
+      <c r="D33" s="64"/>
       <c r="E33" s="26" t="s">
         <v>62</v>
       </c>
@@ -6681,7 +6681,7 @@
       <c r="I33" s="36">
         <v>4</v>
       </c>
-      <c r="J33" s="102"/>
+      <c r="J33" s="64"/>
       <c r="K33" s="13"/>
       <c r="L33" s="17">
         <v>23</v>
@@ -6717,10 +6717,10 @@
     </row>
     <row r="34" spans="1:26" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A34" s="16"/>
-      <c r="B34" s="71"/>
+      <c r="B34" s="76"/>
       <c r="C34" s="77"/>
-      <c r="D34" s="103"/>
-      <c r="E34" s="103"/>
+      <c r="D34" s="65"/>
+      <c r="E34" s="65"/>
       <c r="F34" s="28">
         <v>5</v>
       </c>
@@ -6733,7 +6733,7 @@
       <c r="I34" s="30">
         <v>8</v>
       </c>
-      <c r="J34" s="102"/>
+      <c r="J34" s="64"/>
       <c r="K34" s="13"/>
       <c r="L34" s="17">
         <v>24</v>
@@ -6769,17 +6769,17 @@
     </row>
     <row r="35" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A35" s="16"/>
-      <c r="B35" s="71"/>
+      <c r="B35" s="76"/>
       <c r="C35" s="77"/>
       <c r="D35" s="10"/>
-      <c r="E35" s="102" t="s">
+      <c r="E35" s="64" t="s">
         <v>63</v>
       </c>
-      <c r="F35" s="103"/>
-      <c r="G35" s="102"/>
-      <c r="H35" s="102"/>
-      <c r="I35" s="102"/>
-      <c r="J35" s="102"/>
+      <c r="F35" s="65"/>
+      <c r="G35" s="64"/>
+      <c r="H35" s="64"/>
+      <c r="I35" s="64"/>
+      <c r="J35" s="64"/>
       <c r="K35" s="13"/>
       <c r="L35" s="17">
         <v>25</v>
@@ -6815,17 +6815,17 @@
     </row>
     <row r="36" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A36" s="78"/>
-      <c r="B36" s="72"/>
+      <c r="B36" s="79"/>
       <c r="C36" s="77"/>
-      <c r="D36" s="102"/>
-      <c r="E36" s="102"/>
-      <c r="F36" s="71" t="s">
+      <c r="D36" s="64"/>
+      <c r="E36" s="64"/>
+      <c r="F36" s="76" t="s">
         <v>64</v>
       </c>
-      <c r="G36" s="72"/>
-      <c r="H36" s="72"/>
-      <c r="I36" s="72"/>
-      <c r="J36" s="72"/>
+      <c r="G36" s="79"/>
+      <c r="H36" s="79"/>
+      <c r="I36" s="79"/>
+      <c r="J36" s="79"/>
       <c r="K36" s="13"/>
       <c r="L36" s="17">
         <v>26</v>
@@ -6863,12 +6863,12 @@
       <c r="A37" s="78" t="s">
         <v>65</v>
       </c>
-      <c r="B37" s="72"/>
+      <c r="B37" s="79"/>
       <c r="C37" s="77"/>
-      <c r="D37" s="79" t="s">
+      <c r="D37" s="104" t="s">
         <v>66</v>
       </c>
-      <c r="E37" s="80"/>
+      <c r="E37" s="81"/>
       <c r="F37" s="37">
         <v>1</v>
       </c>
@@ -6922,7 +6922,7 @@
         <v>70</v>
       </c>
       <c r="B38" s="77"/>
-      <c r="C38" s="71"/>
+      <c r="C38" s="76"/>
       <c r="D38" s="77"/>
       <c r="E38" s="15" t="s">
         <v>71</v>
@@ -6968,7 +6968,7 @@
     <row r="39" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A39" s="78"/>
       <c r="B39" s="77"/>
-      <c r="C39" s="71"/>
+      <c r="C39" s="76"/>
       <c r="D39" s="77"/>
       <c r="E39" s="15"/>
       <c r="F39" s="15"/>
@@ -7012,7 +7012,7 @@
     <row r="40" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A40" s="78"/>
       <c r="B40" s="77"/>
-      <c r="C40" s="71"/>
+      <c r="C40" s="76"/>
       <c r="D40" s="77"/>
       <c r="E40" s="15"/>
       <c r="F40" s="15"/>
@@ -7056,7 +7056,7 @@
     <row r="41" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A41" s="78"/>
       <c r="B41" s="77"/>
-      <c r="C41" s="71"/>
+      <c r="C41" s="76"/>
       <c r="D41" s="77"/>
       <c r="E41" s="15"/>
       <c r="F41" s="15"/>
@@ -7100,7 +7100,7 @@
     <row r="42" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A42" s="78"/>
       <c r="B42" s="77"/>
-      <c r="C42" s="71"/>
+      <c r="C42" s="76"/>
       <c r="D42" s="77"/>
       <c r="E42" s="15"/>
       <c r="F42" s="15"/>
@@ -7144,7 +7144,7 @@
     <row r="43" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A43" s="78"/>
       <c r="B43" s="77"/>
-      <c r="C43" s="71"/>
+      <c r="C43" s="76"/>
       <c r="D43" s="77"/>
       <c r="E43" s="15"/>
       <c r="F43" s="15"/>
@@ -7188,7 +7188,7 @@
     <row r="44" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A44" s="78"/>
       <c r="B44" s="77"/>
-      <c r="C44" s="71"/>
+      <c r="C44" s="76"/>
       <c r="D44" s="77"/>
       <c r="E44" s="15"/>
       <c r="F44" s="15"/>
@@ -7232,7 +7232,7 @@
     <row r="45" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A45" s="78"/>
       <c r="B45" s="77"/>
-      <c r="C45" s="71"/>
+      <c r="C45" s="76"/>
       <c r="D45" s="77"/>
       <c r="E45" s="15"/>
       <c r="F45" s="15"/>
@@ -7276,7 +7276,7 @@
     <row r="46" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A46" s="78"/>
       <c r="B46" s="77"/>
-      <c r="C46" s="71"/>
+      <c r="C46" s="76"/>
       <c r="D46" s="77"/>
       <c r="E46" s="15"/>
       <c r="F46" s="15"/>
@@ -7320,7 +7320,7 @@
     <row r="47" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A47" s="78"/>
       <c r="B47" s="77"/>
-      <c r="C47" s="71"/>
+      <c r="C47" s="76"/>
       <c r="D47" s="77"/>
       <c r="E47" s="15"/>
       <c r="F47" s="15"/>
@@ -7364,7 +7364,7 @@
     <row r="48" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A48" s="78"/>
       <c r="B48" s="77"/>
-      <c r="C48" s="71"/>
+      <c r="C48" s="76"/>
       <c r="D48" s="77"/>
       <c r="E48" s="15"/>
       <c r="F48" s="15"/>
@@ -7406,10 +7406,10 @@
       <c r="Z48" s="12"/>
     </row>
     <row r="49" spans="1:26" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="84"/>
-      <c r="B49" s="80"/>
-      <c r="C49" s="85"/>
-      <c r="D49" s="80"/>
+      <c r="A49" s="80"/>
+      <c r="B49" s="81"/>
+      <c r="C49" s="82"/>
+      <c r="D49" s="81"/>
       <c r="E49" s="11"/>
       <c r="F49" s="53"/>
       <c r="G49" s="11"/>
@@ -7450,18 +7450,18 @@
       <c r="Z49" s="12"/>
     </row>
     <row r="50" spans="1:26" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="117" t="s">
+      <c r="A50" s="83" t="s">
         <v>72</v>
       </c>
-      <c r="B50" s="118"/>
-      <c r="C50" s="118"/>
-      <c r="D50" s="119"/>
-      <c r="E50" s="120"/>
-      <c r="F50" s="121"/>
-      <c r="G50" s="121"/>
-      <c r="H50" s="121"/>
-      <c r="I50" s="121"/>
-      <c r="J50" s="122"/>
+      <c r="B50" s="84"/>
+      <c r="C50" s="84"/>
+      <c r="D50" s="85"/>
+      <c r="E50" s="70"/>
+      <c r="F50" s="71"/>
+      <c r="G50" s="71"/>
+      <c r="H50" s="71"/>
+      <c r="I50" s="71"/>
+      <c r="J50" s="72"/>
       <c r="K50" s="48"/>
       <c r="L50" s="44">
         <v>40</v>
@@ -7499,111 +7499,111 @@
       <c r="A51" s="78" t="s">
         <v>59</v>
       </c>
-      <c r="B51" s="72"/>
-      <c r="C51" s="72"/>
+      <c r="B51" s="79"/>
+      <c r="C51" s="79"/>
       <c r="D51" s="77"/>
       <c r="E51" s="41" t="s">
         <v>60</v>
       </c>
-      <c r="F51" s="81"/>
-      <c r="G51" s="81"/>
+      <c r="F51" s="90"/>
+      <c r="G51" s="90"/>
       <c r="H51" s="40" t="s">
         <v>61</v>
       </c>
-      <c r="I51" s="81"/>
-      <c r="J51" s="71"/>
-      <c r="K51" s="114"/>
-      <c r="L51" s="86"/>
-      <c r="M51" s="86"/>
-      <c r="N51" s="86"/>
-      <c r="O51" s="86"/>
-      <c r="P51" s="86"/>
-      <c r="Q51" s="86"/>
-      <c r="R51" s="86"/>
-      <c r="S51" s="86"/>
-      <c r="T51" s="86"/>
-      <c r="U51" s="86"/>
-      <c r="V51" s="86"/>
-      <c r="W51" s="86"/>
-      <c r="X51" s="86"/>
-      <c r="Y51" s="86"/>
-      <c r="Z51" s="106"/>
+      <c r="I51" s="90"/>
+      <c r="J51" s="76"/>
+      <c r="K51" s="94"/>
+      <c r="L51" s="95"/>
+      <c r="M51" s="95"/>
+      <c r="N51" s="95"/>
+      <c r="O51" s="95"/>
+      <c r="P51" s="95"/>
+      <c r="Q51" s="95"/>
+      <c r="R51" s="95"/>
+      <c r="S51" s="95"/>
+      <c r="T51" s="95"/>
+      <c r="U51" s="95"/>
+      <c r="V51" s="95"/>
+      <c r="W51" s="95"/>
+      <c r="X51" s="95"/>
+      <c r="Y51" s="95"/>
+      <c r="Z51" s="96"/>
     </row>
     <row r="52" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A52" s="78" t="s">
         <v>62</v>
       </c>
-      <c r="B52" s="72"/>
-      <c r="C52" s="72"/>
+      <c r="B52" s="79"/>
+      <c r="C52" s="79"/>
       <c r="D52" s="77"/>
       <c r="E52" s="41" t="s">
         <v>60</v>
       </c>
-      <c r="F52" s="81"/>
-      <c r="G52" s="81"/>
+      <c r="F52" s="90"/>
+      <c r="G52" s="90"/>
       <c r="H52" s="40" t="s">
         <v>61</v>
       </c>
-      <c r="I52" s="81"/>
-      <c r="J52" s="71"/>
-      <c r="K52" s="105" t="s">
+      <c r="I52" s="90"/>
+      <c r="J52" s="76"/>
+      <c r="K52" s="91" t="s">
         <v>73</v>
       </c>
-      <c r="L52" s="82"/>
-      <c r="M52" s="82"/>
-      <c r="N52" s="82"/>
-      <c r="O52" s="83"/>
-      <c r="P52" s="81" t="s">
+      <c r="L52" s="92"/>
+      <c r="M52" s="92"/>
+      <c r="N52" s="92"/>
+      <c r="O52" s="93"/>
+      <c r="P52" s="90" t="s">
         <v>46</v>
       </c>
-      <c r="Q52" s="81"/>
-      <c r="R52" s="81"/>
-      <c r="S52" s="81"/>
-      <c r="T52" s="81"/>
-      <c r="U52" s="81" t="s">
+      <c r="Q52" s="90"/>
+      <c r="R52" s="90"/>
+      <c r="S52" s="90"/>
+      <c r="T52" s="90"/>
+      <c r="U52" s="90" t="s">
         <v>47</v>
       </c>
-      <c r="V52" s="81"/>
-      <c r="W52" s="81"/>
-      <c r="X52" s="81"/>
-      <c r="Y52" s="81"/>
+      <c r="V52" s="90"/>
+      <c r="W52" s="90"/>
+      <c r="X52" s="90"/>
+      <c r="Y52" s="90"/>
       <c r="Z52" s="12"/>
     </row>
     <row r="53" spans="1:26" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="107" t="s">
+      <c r="A53" s="73" t="s">
         <v>74</v>
       </c>
-      <c r="B53" s="58"/>
-      <c r="C53" s="58"/>
-      <c r="D53" s="108"/>
-      <c r="E53" s="109" t="s">
+      <c r="B53" s="74"/>
+      <c r="C53" s="74"/>
+      <c r="D53" s="75"/>
+      <c r="E53" s="67" t="s">
         <v>60</v>
       </c>
-      <c r="F53" s="110"/>
-      <c r="G53" s="110"/>
-      <c r="H53" s="111" t="s">
+      <c r="F53" s="86"/>
+      <c r="G53" s="86"/>
+      <c r="H53" s="68" t="s">
         <v>61</v>
       </c>
-      <c r="I53" s="110"/>
-      <c r="J53" s="115"/>
-      <c r="K53" s="116" t="s">
+      <c r="I53" s="86"/>
+      <c r="J53" s="87"/>
+      <c r="K53" s="88" t="s">
         <v>75</v>
       </c>
-      <c r="L53" s="112"/>
-      <c r="M53" s="112"/>
-      <c r="N53" s="112"/>
-      <c r="O53" s="112"/>
-      <c r="P53" s="112"/>
-      <c r="Q53" s="112"/>
-      <c r="R53" s="110"/>
-      <c r="S53" s="110"/>
-      <c r="T53" s="110"/>
-      <c r="U53" s="110"/>
-      <c r="V53" s="110"/>
-      <c r="W53" s="110"/>
-      <c r="X53" s="110"/>
-      <c r="Y53" s="110"/>
-      <c r="Z53" s="113"/>
+      <c r="L53" s="89"/>
+      <c r="M53" s="89"/>
+      <c r="N53" s="89"/>
+      <c r="O53" s="89"/>
+      <c r="P53" s="89"/>
+      <c r="Q53" s="89"/>
+      <c r="R53" s="86"/>
+      <c r="S53" s="86"/>
+      <c r="T53" s="86"/>
+      <c r="U53" s="86"/>
+      <c r="V53" s="86"/>
+      <c r="W53" s="86"/>
+      <c r="X53" s="86"/>
+      <c r="Y53" s="86"/>
+      <c r="Z53" s="69"/>
     </row>
     <row r="55" spans="1:26" x14ac:dyDescent="0.2">
       <c r="D55" s="9"/>
@@ -7734,6 +7734,97 @@
     </row>
   </sheetData>
   <mergeCells count="115">
+    <mergeCell ref="A8:C8"/>
+    <mergeCell ref="D8:J8"/>
+    <mergeCell ref="L8:O8"/>
+    <mergeCell ref="Q8:S8"/>
+    <mergeCell ref="K9:Z9"/>
+    <mergeCell ref="E9:I9"/>
+    <mergeCell ref="A9:D9"/>
+    <mergeCell ref="K1:Y1"/>
+    <mergeCell ref="K3:Q3"/>
+    <mergeCell ref="S3:Y3"/>
+    <mergeCell ref="K4:Q4"/>
+    <mergeCell ref="S4:Y4"/>
+    <mergeCell ref="K5:Q5"/>
+    <mergeCell ref="S5:Y5"/>
+    <mergeCell ref="K6:Q6"/>
+    <mergeCell ref="S6:Y6"/>
+    <mergeCell ref="M10:N10"/>
+    <mergeCell ref="O10:P10"/>
+    <mergeCell ref="Q10:R10"/>
+    <mergeCell ref="S10:T10"/>
+    <mergeCell ref="U10:V10"/>
+    <mergeCell ref="W10:X10"/>
+    <mergeCell ref="Y10:Z10"/>
+    <mergeCell ref="F15:J15"/>
+    <mergeCell ref="L7:O7"/>
+    <mergeCell ref="Q7:S7"/>
+    <mergeCell ref="K10:L10"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="A15:C15"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="C38:D38"/>
+    <mergeCell ref="A39:B39"/>
+    <mergeCell ref="C39:D39"/>
+    <mergeCell ref="A40:B40"/>
+    <mergeCell ref="C40:D40"/>
+    <mergeCell ref="A29:C29"/>
+    <mergeCell ref="D29:J29"/>
+    <mergeCell ref="E30:I30"/>
+    <mergeCell ref="A16:C16"/>
+    <mergeCell ref="D16:E16"/>
+    <mergeCell ref="A17:B17"/>
+    <mergeCell ref="A18:B18"/>
+    <mergeCell ref="C18:D18"/>
+    <mergeCell ref="B31:C31"/>
+    <mergeCell ref="B32:C32"/>
+    <mergeCell ref="F36:J36"/>
+    <mergeCell ref="A37:C37"/>
+    <mergeCell ref="D37:E37"/>
+    <mergeCell ref="A38:B38"/>
+    <mergeCell ref="A20:B20"/>
+    <mergeCell ref="C20:D20"/>
+    <mergeCell ref="A21:B21"/>
+    <mergeCell ref="C21:D21"/>
+    <mergeCell ref="A30:D30"/>
+    <mergeCell ref="I53:J53"/>
+    <mergeCell ref="K53:Q53"/>
+    <mergeCell ref="R53:Y53"/>
+    <mergeCell ref="F51:G51"/>
+    <mergeCell ref="I51:J51"/>
+    <mergeCell ref="F52:G52"/>
+    <mergeCell ref="I52:J52"/>
+    <mergeCell ref="P52:R52"/>
+    <mergeCell ref="S52:T52"/>
+    <mergeCell ref="K52:O52"/>
+    <mergeCell ref="U52:W52"/>
+    <mergeCell ref="X52:Y52"/>
+    <mergeCell ref="K51:Z51"/>
+    <mergeCell ref="A41:B41"/>
+    <mergeCell ref="C41:D41"/>
+    <mergeCell ref="A42:B42"/>
+    <mergeCell ref="C42:D42"/>
+    <mergeCell ref="A43:B43"/>
+    <mergeCell ref="C43:D43"/>
+    <mergeCell ref="A44:B44"/>
+    <mergeCell ref="C45:D45"/>
+    <mergeCell ref="F53:G53"/>
+    <mergeCell ref="A45:B45"/>
+    <mergeCell ref="A46:B46"/>
+    <mergeCell ref="C46:D46"/>
+    <mergeCell ref="A47:B47"/>
+    <mergeCell ref="C47:D47"/>
+    <mergeCell ref="A48:B48"/>
+    <mergeCell ref="C48:D48"/>
+    <mergeCell ref="A49:B49"/>
+    <mergeCell ref="C49:D49"/>
     <mergeCell ref="E50:J50"/>
     <mergeCell ref="A53:D53"/>
     <mergeCell ref="B33:C33"/>
@@ -7758,97 +7849,6 @@
     <mergeCell ref="A51:D51"/>
     <mergeCell ref="A52:D52"/>
     <mergeCell ref="C44:D44"/>
-    <mergeCell ref="A45:B45"/>
-    <mergeCell ref="A46:B46"/>
-    <mergeCell ref="C46:D46"/>
-    <mergeCell ref="A47:B47"/>
-    <mergeCell ref="C47:D47"/>
-    <mergeCell ref="A48:B48"/>
-    <mergeCell ref="C48:D48"/>
-    <mergeCell ref="A49:B49"/>
-    <mergeCell ref="C49:D49"/>
-    <mergeCell ref="A41:B41"/>
-    <mergeCell ref="C41:D41"/>
-    <mergeCell ref="A42:B42"/>
-    <mergeCell ref="C42:D42"/>
-    <mergeCell ref="A43:B43"/>
-    <mergeCell ref="C43:D43"/>
-    <mergeCell ref="A44:B44"/>
-    <mergeCell ref="C45:D45"/>
-    <mergeCell ref="F53:G53"/>
-    <mergeCell ref="I53:J53"/>
-    <mergeCell ref="K53:Q53"/>
-    <mergeCell ref="R53:Y53"/>
-    <mergeCell ref="F51:G51"/>
-    <mergeCell ref="I51:J51"/>
-    <mergeCell ref="F52:G52"/>
-    <mergeCell ref="I52:J52"/>
-    <mergeCell ref="P52:R52"/>
-    <mergeCell ref="S52:T52"/>
-    <mergeCell ref="K52:O52"/>
-    <mergeCell ref="U52:W52"/>
-    <mergeCell ref="X52:Y52"/>
-    <mergeCell ref="K51:Z51"/>
-    <mergeCell ref="C38:D38"/>
-    <mergeCell ref="A39:B39"/>
-    <mergeCell ref="C39:D39"/>
-    <mergeCell ref="A40:B40"/>
-    <mergeCell ref="C40:D40"/>
-    <mergeCell ref="A29:C29"/>
-    <mergeCell ref="D29:J29"/>
-    <mergeCell ref="E30:I30"/>
-    <mergeCell ref="A16:C16"/>
-    <mergeCell ref="D16:E16"/>
-    <mergeCell ref="A17:B17"/>
-    <mergeCell ref="A18:B18"/>
-    <mergeCell ref="C18:D18"/>
-    <mergeCell ref="B31:C31"/>
-    <mergeCell ref="B32:C32"/>
-    <mergeCell ref="F36:J36"/>
-    <mergeCell ref="A37:C37"/>
-    <mergeCell ref="D37:E37"/>
-    <mergeCell ref="A38:B38"/>
-    <mergeCell ref="A20:B20"/>
-    <mergeCell ref="C20:D20"/>
-    <mergeCell ref="A21:B21"/>
-    <mergeCell ref="C21:D21"/>
-    <mergeCell ref="A30:D30"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="B13:C13"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="A15:C15"/>
-    <mergeCell ref="C17:D17"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="C19:D19"/>
-    <mergeCell ref="M10:N10"/>
-    <mergeCell ref="O10:P10"/>
-    <mergeCell ref="Q10:R10"/>
-    <mergeCell ref="S10:T10"/>
-    <mergeCell ref="U10:V10"/>
-    <mergeCell ref="W10:X10"/>
-    <mergeCell ref="Y10:Z10"/>
-    <mergeCell ref="F15:J15"/>
-    <mergeCell ref="L7:O7"/>
-    <mergeCell ref="Q7:S7"/>
-    <mergeCell ref="K10:L10"/>
-    <mergeCell ref="A8:C8"/>
-    <mergeCell ref="D8:J8"/>
-    <mergeCell ref="L8:O8"/>
-    <mergeCell ref="Q8:S8"/>
-    <mergeCell ref="K9:Z9"/>
-    <mergeCell ref="E9:I9"/>
-    <mergeCell ref="A9:D9"/>
-    <mergeCell ref="K1:Y1"/>
-    <mergeCell ref="K3:Q3"/>
-    <mergeCell ref="S3:Y3"/>
-    <mergeCell ref="K4:Q4"/>
-    <mergeCell ref="S4:Y4"/>
-    <mergeCell ref="K5:Q5"/>
-    <mergeCell ref="S5:Y5"/>
-    <mergeCell ref="K6:Q6"/>
-    <mergeCell ref="S6:Y6"/>
   </mergeCells>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
   <pageMargins left="0.47244094488188981" right="0.35433070866141736" top="0.47244094488188981" bottom="0.19685039370078741" header="0.19685039370078741" footer="0.19685039370078741"/>

</xml_diff>